<commit_message>
LvdB: update program formulas
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -1,28 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21803"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2e4d\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\school\WUR\Master\Programming in python\untitled\ACT\ACT2321\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0CB4CDC-ECE6-4778-B88D-A6F424EFBB31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="16215" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
     <sheet name="CO2eq (kg)" sheetId="1" r:id="rId2"/>
     <sheet name="Energy (MJ)" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={ED13EA6E-84B9-4566-9DD1-5F68795B2A3F}</author>
     <author>tc={AA2B32B5-7D1D-400A-A931-EBFBF82EF357}</author>
@@ -74,216 +70,431 @@
     <author>tc={3CBB2313-6869-4ADB-8678-F0A56C53B204}</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{ED13EA6E-84B9-4566-9DD1-5F68795B2A3F}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This is the time needed from seeds to maturity, but in the vertical farming, may be start to harvest before they are maturity (such as, microgreen mix), thus we decided to write 12 days for microgreen mix
 </t>
-      </text>
-    </comment>
-    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{AA2B32B5-7D1D-400A-A931-EBFBF82EF357}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://www.foodstandards.gov.au/science/monitoringnutrients/ausnut/foodmeasures/Pages/-Fruits-and-vegetable-measures-program---data-table.aspx
 </t>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{DAFEC4E5-6F24-4648-91ED-14AA6811292D}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://www.growgreatvegetables.com/plantinggrowing/germination/
 </t>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="3" shapeId="0" xr:uid="{8FE4F82F-6907-41E0-ACF1-311361FEC4C7}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://greenharvest.com.au/SeedOrganic/SeedsPerGram.html
 </t>
-      </text>
-    </comment>
-    <comment ref="E2" authorId="4" shapeId="0" xr:uid="{F0E4EA42-2698-47D0-A222-D1E83A6DAA7D}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="4" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://nevo-online.rivm.nl/ProductenDetailsGetabt.aspx?zoekstring=&amp;tabid=1
 </t>
-      </text>
-    </comment>
-    <comment ref="F2" authorId="5" shapeId="0" xr:uid="{D21AF469-E910-4274-AF0D-7D27B238D9E7}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="5" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://www.webgrower.com/regional/pdf/ND_Veg-Maturity-Dates_h912.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="6" shapeId="0" xr:uid="{DEC464CC-8A70-4C86-9116-9C8B145BBB1E}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="6" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.agriculturejournals.cz/publicFiles/00115.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="7" shapeId="0" xr:uid="{3C953827-5C2D-4742-A6F6-150B1C1BC74D}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="7" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://medcraveonline.com/APAR/APAR-05-00173.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="8" shapeId="0" xr:uid="{5667D7E8-CE45-48EB-8BEF-B2A681E2E308}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="8" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://sustainable-farming.rutgers.edu/wp-content/uploads/2017/12/urbanfringe-v07n01.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="9" shapeId="0" xr:uid="{3D18DAF9-FA04-48E1-A8CB-5C5ED8180794}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="9" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www-sciencedirect-com.ezproxy.library.wur.nl/science/article/pii/S030442381830894X
 </t>
-      </text>
-    </comment>
-    <comment ref="C5" authorId="10" shapeId="0" xr:uid="{81A05FB6-F8D5-4215-B674-8F1D2351605B}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="10" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.daff.gov.za/docs/Brochures/MbeanpGUDELINS.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="11" shapeId="0" xr:uid="{6CB3C0DC-854E-4A55-8539-9AD9B39ABB67}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="11" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.daff.gov.za/docs/Brochures/MbeanpGUDELINS.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="F5" authorId="12" shapeId="0" xr:uid="{EE065DF9-E183-4DC0-B823-54EEB2A83055}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="12" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://sproutpeople.org/growing-mung-bean-sprouts/
 </t>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="13" shapeId="0" xr:uid="{2CE7C953-E49E-4A79-B418-53F8AD2A6AFA}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="13" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.goodfood.com.au/recipes/brain-food-if-a-recipe-calls-for-a-bunch-of-herbs-exactly-how-much-is-a-bunch-20151102-gkjdjj
 </t>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="14" shapeId="0" xr:uid="{063C0FF8-3329-4679-9464-4142E1509E8B}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="14" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://onlinelibrary-wiley-com.ezproxy.library.wur.nl/doi/full/10.1111/jwas.12471
 </t>
-      </text>
-    </comment>
-    <comment ref="F7" authorId="15" shapeId="0" xr:uid="{382198E1-719A-47EB-9BBD-AEA3E9643F05}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="15" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://harvesttotable.com/how_to_grow_kale/
 </t>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="16" shapeId="0" xr:uid="{5DAD9E96-B1AC-40EC-A343-549D1C86441C}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="16" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.sciencedirect.com/science/article/pii/S0570178316300288
 </t>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="17" shapeId="0" xr:uid="{DE7DAB9C-E072-4C08-A524-CC36ABE006DC}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="17" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.nda.agric.za/docs/Brochures/ProGuiBasil.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="F8" authorId="18" shapeId="0" xr:uid="{7E9BDE2F-7436-4F06-AA05-76C0B6EF0151}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="18" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://harvesttotable.com/how_to_grow_basil/
 </t>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="19" shapeId="0" xr:uid="{746EE960-3E3F-4E97-B83D-3F630DD80F97}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="19" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://www.hortorumcultus.actapol.net/pub/8_4_23.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="20" shapeId="0" xr:uid="{F5C2A7A9-655F-44C8-BA17-5A544641CD31}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="20" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.westcoastseeds.com/blogs/how-to-grow/how-to-grow-arugula
 </t>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="21" shapeId="0" xr:uid="{38735AFA-08BE-46E7-8B5D-A6F6E71F9349}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="21" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.growitalian.com/arugula-rucola-selvatica-wild-arugula-115-5/
 </t>
-      </text>
-    </comment>
-    <comment ref="F9" authorId="22" shapeId="0" xr:uid="{0F9B3DFA-8ADC-4989-99B0-30B95C57E01E}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="22" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://veggieharvest.com/vegetables/arugula.html
 </t>
-      </text>
-    </comment>
-    <comment ref="A10" authorId="23" shapeId="0" xr:uid="{DA3C5C15-680E-484C-AC79-F93CD00D3328}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="23" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Microgreen mix including (Chives, Cabbage, Celery, Mustard, Kale, Watercress, Beets). 
@@ -292,11 +503,20 @@
 growth period : Chives(82.5), Cabbage(86), Celery(135), Mustard(50), Kale(75), Watercress(17.5), Beets(65).
 plant weight : Chives(0.01382), Cabbage(1.25), Celery(0.675), Mustard(0.07), Kale(0.040125), Watercress(0.12), Beets(0.31243).
 </t>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="24" shapeId="0" xr:uid="{E9E75DD3-E97D-42D3-83E8-E1069EC265E8}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="24" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://homegardeners.in/cabbage/
@@ -306,81 +526,154 @@
 https://www.sciencedirect.com/science/article/pii/S0889157515001003
 file:///C:/Users/H/Downloads/watercress170-177-1422017BR-1431.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="25" shapeId="0" xr:uid="{F31CB36E-DFFF-4430-8925-364B1248F789}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="25" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.westcoastseeds.com/blogs/how-to-grow/grow-chives
 </t>
-      </text>
-    </comment>
-    <comment ref="D10" authorId="26" shapeId="0" xr:uid="{032348BB-264C-4C04-A358-C90BDB0F2CBB}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="26" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Common microgreens: https://draxe.com/microgreens/
 Seed weights: https://greenharvest.com.au/SeedOrganic/SeedsPerGram.html
 </t>
-      </text>
-    </comment>
-    <comment ref="E10" authorId="27" shapeId="0" xr:uid="{34BA0857-7630-410F-ADEB-7CDE29F6F4E4}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="27" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://www.wsbentley.co.uk/explore-more/chefs-microgreens/
 </t>
-      </text>
-    </comment>
-    <comment ref="F10" authorId="28" shapeId="0" xr:uid="{2674CD71-C273-4501-8B80-5BDF411CCD11}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="28" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://harvesttotable.com/how_to_grow_chives/
 https://harvesttotable.com/how_to_grow_celery/
 https://harvesttotable.com/how_to_grow_cress/
 </t>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="29" shapeId="0" xr:uid="{23E3E1DE-1D30-401A-95D1-C8555D81F6BF}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="29" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     file:///C:/Users/H/Downloads/Spearmint.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="30" shapeId="0" xr:uid="{B619E217-C26E-484F-96C6-1045106C5109}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="30" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://www.academicjournals.org/app/webroot/article/article1380714927_Liopa-Tsakalidis%20et%20al.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="31" shapeId="0" xr:uid="{54D768C3-619F-4830-A4DF-B4A28BE5731C}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="31" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://herbgardening.com/growingmint.htm
 </t>
-      </text>
-    </comment>
-    <comment ref="F11" authorId="32" shapeId="0" xr:uid="{3CBB2313-6869-4ADB-8678-F0A56C53B204}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="32" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://homeguides.sfgate.com/long-mint-need-grow-70659.html
 </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -388,7 +681,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={53C940E0-2140-41F9-A6DF-6EA835ABEC64}</author>
     <author>tc={F8E5DC3C-6251-4EB4-8D84-9AAD62A6919A}</author>
@@ -412,187 +705,367 @@
     <author>tc={7A90E5E2-2E08-4861-A6C8-2E490EE47A92}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{53C940E0-2140-41F9-A6DF-6EA835ABEC64}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     We need to find the most interesting countries for this because here there is a wide variety
 </t>
-      </text>
-    </comment>
-    <comment ref="K2" authorId="1" shapeId="0" xr:uid="{F8E5DC3C-6251-4EB4-8D84-9AAD62A6919A}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://ira.lib.polyu.edu.hk/bitstream/10397/36019/1/Hong_Jingke_2015.pdf
 For green only hydro included atm!
 </t>
-      </text>
-    </comment>
-    <comment ref="L2" authorId="2" shapeId="0" xr:uid="{F049A3EB-816D-4F33-9493-D7CA7D0BC6D1}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://ira.lib.polyu.edu.hk/bitstream/10397/36019/1/Hong_Jingke_2015.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="3" shapeId="0" xr:uid="{14D3C766-2560-494A-97DB-D6CC08AA48F4}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent
 </t>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="4" shapeId="0" xr:uid="{9A67475F-7AFB-4218-BE16-67F64059BF09}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="4" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://ira.lib.polyu.edu.hk/bitstream/10397/36019/1/Hong_Jingke_2015.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{11C788DB-B1E6-4564-A49D-EF89ED2E9A6F}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="5" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent
 </t>
-      </text>
-    </comment>
-    <comment ref="J13" authorId="6" shapeId="0" xr:uid="{67393C48-310C-4E8B-87A7-6A02EA78F1F7}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="6" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent 3
 </t>
-      </text>
-    </comment>
-    <comment ref="J15" authorId="7" shapeId="0" xr:uid="{663D8CF0-4CFD-4F94-B3AD-E16830C73AAE}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J15" authorId="7" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     AGRIBALYSE (Adapted from Ecoinvent 2.2)
 </t>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="8" shapeId="0" xr:uid="{0BD08DC0-6AE2-48F8-BBCF-BAB58B87B9B4}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="8" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent v3
 </t>
-      </text>
-    </comment>
-    <comment ref="L20" authorId="9" shapeId="0" xr:uid="{A7925944-D01F-4C9C-B69E-643D7D71DBB7}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="L20" authorId="9" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Agri-footprint - economic allocation
 Reply:
     What concentration is used for these?
 </t>
-      </text>
-    </comment>
-    <comment ref="L30" authorId="10" shapeId="0" xr:uid="{E0F305EA-C278-435F-9FD8-E37E53F129BA}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="L30" authorId="10" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent system processes
 </t>
-      </text>
-    </comment>
-    <comment ref="K36" authorId="11" shapeId="0" xr:uid="{E98DA1EC-7D2D-417B-8BDC-16BE9804AC5D}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="K36" authorId="11" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://dspace.library.uu.nl/handle/1874/335731
 </t>
-      </text>
-    </comment>
-    <comment ref="L36" authorId="12" shapeId="0" xr:uid="{AD26B5D4-D252-4749-8261-86FA21A3D1E2}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="L36" authorId="12" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.iscc-system.org/wp-content/uploads/2017/02/ISCC_205_GHG_Emissions_3.0.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="J40" authorId="13" shapeId="0" xr:uid="{E5B41D43-DFB0-4609-8666-707809BF1FA0}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J40" authorId="13" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://www.fao.org/3/a-i8276e.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="L40" authorId="14" shapeId="0" xr:uid="{BF29E2A2-F230-4081-BB0A-3EEB1266FFB6}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="L40" authorId="14" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.iscc-system.org/wp-content/uploads/2017/02/ISCC_205_GHG_Emissions_3.0.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="M40" authorId="15" shapeId="0" xr:uid="{AF7E6B3F-84B4-4E74-8499-B9DD1A8DCCB5}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="M40" authorId="15" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.biogeosciences.net/10/7897/2013/bg-10-7897-2013.pdf
 </t>
-      </text>
-    </comment>
-    <comment ref="J42" authorId="16" shapeId="0" xr:uid="{A431C984-8612-4A74-82AA-B5C05F1E8636}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J42" authorId="16" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvest
 </t>
-      </text>
-    </comment>
-    <comment ref="J44" authorId="17" shapeId="0" xr:uid="{99E981B9-97EB-4BF1-93ED-293BFE8A4BF4}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J44" authorId="17" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     AGRIBALYSE
 </t>
-      </text>
-    </comment>
-    <comment ref="J46" authorId="18" shapeId="0" xr:uid="{79E25465-3D46-40B7-B8A8-18DD9D6306B0}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J46" authorId="18" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent 3
 </t>
-      </text>
-    </comment>
-    <comment ref="E50" authorId="19" shapeId="0" xr:uid="{7A90E5E2-2E08-4861-A6C8-2E490EE47A92}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="E50" authorId="19" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RIVM
 </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -600,7 +1073,7 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={28C0A1D0-E24D-4A94-B8D7-08380DAD163B}</author>
     <author>tc={F1D6A124-94E9-4537-87FD-64C5756431CC}</author>
@@ -617,121 +1090,238 @@
     <author>tc={EB5AF55A-D36E-4291-B324-6215D9703071}</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{28C0A1D0-E24D-4A94-B8D7-08380DAD163B}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent
 </t>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="1" shapeId="0" xr:uid="{F1D6A124-94E9-4537-87FD-64C5756431CC}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent
 </t>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="2" shapeId="0" xr:uid="{2A2FDC7F-6B63-4EB2-9514-8F273884490D}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent
 </t>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="3" shapeId="0" xr:uid="{75A964C6-E221-4021-9BCF-E318D4CBA659}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent
 </t>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="4" shapeId="0" xr:uid="{DB213962-8976-483B-B4B5-B4CD76A55796}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="4" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent
 </t>
-      </text>
-    </comment>
-    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{88B16166-346E-4A39-90D1-67B1D7130E04}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="5" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent
 </t>
-      </text>
-    </comment>
-    <comment ref="J13" authorId="6" shapeId="0" xr:uid="{4894AC73-6F3C-482C-BF3B-EF91AD8418D6}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="6" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     http://www.world-nuclear.org/information-library/facts-and-figures/heat-values-of-various-fuels.aspx
 </t>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="7" shapeId="0" xr:uid="{BFF5F8B5-9FA9-47FB-B65E-682B51E753EF}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="7" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent V3
 </t>
-      </text>
-    </comment>
-    <comment ref="J39" authorId="8" shapeId="0" xr:uid="{91C7F82C-9A9F-4C87-A739-6A581FAAD543}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J39" authorId="8" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://dspace.lib.cranfield.ac.uk/bitstream/handle/1826/3913/Estimation_of_the_greenhouse_gas_emissions_from_agricultural_pesticide_manufacture_and_use-2009.pdf;jsessionid=F7CBF742766A89A35DC6BC258D016501?sequence=1
 </t>
-      </text>
-    </comment>
-    <comment ref="K39" authorId="9" shapeId="0" xr:uid="{27297E8D-321A-49D8-9262-B18D44E94748}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="K39" authorId="9" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://books.google.nl/books?id=9kv5ZvX2qfUC&amp;pg=PA355&amp;lpg=PA355&amp;dq=pesticides+in+MJ+kg+in+america&amp;source=bl&amp;ots=KKoY-TYK_V&amp;sig=ACfU3U0lBflL2mkbLtwvxIkOYkX6fdLrug&amp;hl=en&amp;sa=X&amp;ved=2ahUKEwi30cflxtLiAhUDLlAKHaorAisQ6AEwAnoECAYQAQ#v=onepage&amp;q=pesticides%20in%20MJ%20kg%20in%20america&amp;f=false
 </t>
-      </text>
-    </comment>
-    <comment ref="J41" authorId="10" shapeId="0" xr:uid="{48EF0565-F5AA-4859-B328-8E1C327C14E9}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J41" authorId="10" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent system processes
 </t>
-      </text>
-    </comment>
-    <comment ref="J43" authorId="11" shapeId="0" xr:uid="{1B93F73B-A64C-41F2-9E79-1347DA5958C3}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J43" authorId="11" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     AGRIBALYSE
 </t>
-      </text>
-    </comment>
-    <comment ref="J45" authorId="12" shapeId="0" xr:uid="{EB5AF55A-D36E-4291-B324-6215D9703071}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
+        </r>
+      </text>
+    </comment>
+    <comment ref="J45" authorId="12" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ecoinvent 3
 </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -739,7 +1329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="183">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -1285,21 +1875,24 @@
   </si>
   <si>
     <t>T4</t>
+  </si>
+  <si>
+    <t>Pac1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.00000000"/>
-    <numFmt numFmtId="170" formatCode="0.000000000"/>
+    <numFmt numFmtId="169" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1535,7 +2128,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2163,14 +2756,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF74F14D-B9C3-485A-B148-17C5978D96E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="8" customWidth="1"/>
@@ -2181,7 +2774,7 @@
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -2199,7 +2792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
@@ -2219,7 +2812,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
@@ -2239,7 +2832,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
@@ -2259,7 +2852,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -2279,7 +2872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
@@ -2299,7 +2892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>21</v>
       </c>
@@ -2319,7 +2912,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>24</v>
       </c>
@@ -2339,7 +2932,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
@@ -2359,7 +2952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>31</v>
       </c>
@@ -2379,7 +2972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>34</v>
       </c>
@@ -2406,14 +2999,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.42578125" customWidth="1"/>
@@ -2425,7 +3018,7 @@
     <col min="12" max="17" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>37</v>
       </c>
@@ -2460,7 +3053,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -2503,7 +3096,7 @@
       </c>
       <c r="M2" s="29"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>51</v>
       </c>
@@ -2540,7 +3133,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -2559,7 +3152,7 @@
       <c r="L4" s="29"/>
       <c r="M4" s="29"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>55</v>
       </c>
@@ -2578,7 +3171,7 @@
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>57</v>
       </c>
@@ -2598,7 +3191,7 @@
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>59</v>
       </c>
@@ -2615,7 +3208,7 @@
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>60</v>
       </c>
@@ -2627,7 +3220,7 @@
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>61</v>
       </c>
@@ -2639,7 +3232,7 @@
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>62</v>
       </c>
@@ -2651,7 +3244,7 @@
       <c r="L10" s="29"/>
       <c r="M10" s="29"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>63</v>
       </c>
@@ -2663,7 +3256,7 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D12" s="33"/>
       <c r="E12" s="1"/>
       <c r="J12" s="1"/>
@@ -2671,7 +3264,7 @@
       <c r="L12" s="29"/>
       <c r="M12" s="29"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -2693,7 +3286,7 @@
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>67</v>
       </c>
@@ -2712,7 +3305,7 @@
       <c r="L14" s="29"/>
       <c r="M14" s="29"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>69</v>
       </c>
@@ -2731,7 +3324,7 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>71</v>
       </c>
@@ -2750,7 +3343,7 @@
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D17" s="33"/>
       <c r="E17" s="1"/>
       <c r="J17" s="1"/>
@@ -2758,7 +3351,7 @@
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -2777,7 +3370,7 @@
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D19" s="33"/>
       <c r="E19" s="1"/>
       <c r="J19" s="1"/>
@@ -2785,7 +3378,7 @@
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -2807,7 +3400,7 @@
       </c>
       <c r="M20" s="29"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>78</v>
       </c>
@@ -2826,7 +3419,7 @@
       </c>
       <c r="M21" s="29"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>80</v>
       </c>
@@ -2845,7 +3438,7 @@
       </c>
       <c r="M22" s="29"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>82</v>
       </c>
@@ -2864,7 +3457,7 @@
       </c>
       <c r="M23" s="29"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>84</v>
       </c>
@@ -2883,7 +3476,7 @@
       </c>
       <c r="M24" s="29"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>86</v>
       </c>
@@ -2902,7 +3495,7 @@
       </c>
       <c r="M25" s="29"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>88</v>
       </c>
@@ -2921,7 +3514,7 @@
       </c>
       <c r="M26" s="29"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>90</v>
       </c>
@@ -2940,7 +3533,7 @@
       </c>
       <c r="M27" s="29"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>92</v>
       </c>
@@ -2959,7 +3552,7 @@
       </c>
       <c r="M28" s="29"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>94</v>
       </c>
@@ -2978,7 +3571,7 @@
       </c>
       <c r="M29" s="29"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>96</v>
       </c>
@@ -2997,7 +3590,7 @@
       </c>
       <c r="M30" s="29"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>98</v>
       </c>
@@ -3011,7 +3604,7 @@
       <c r="L31" s="29"/>
       <c r="M31" s="29"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>100</v>
       </c>
@@ -3027,7 +3620,7 @@
       </c>
       <c r="M32" s="29"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>101</v>
       </c>
@@ -3037,7 +3630,7 @@
       <c r="L33" s="29"/>
       <c r="M33" s="29"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D34" s="33"/>
       <c r="E34" s="1"/>
       <c r="J34" s="1"/>
@@ -3045,7 +3638,7 @@
       <c r="L34" s="29"/>
       <c r="M34" s="29"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -3067,7 +3660,7 @@
       <c r="L35" s="29"/>
       <c r="M35" s="29"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>105</v>
       </c>
@@ -3090,7 +3683,7 @@
       </c>
       <c r="M36" s="29"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>107</v>
       </c>
@@ -3109,7 +3702,7 @@
       <c r="L37" s="29"/>
       <c r="M37" s="29"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>109</v>
       </c>
@@ -3128,7 +3721,7 @@
       <c r="L38" s="29"/>
       <c r="M38" s="29"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>111</v>
       </c>
@@ -3147,7 +3740,7 @@
       <c r="L39" s="28"/>
       <c r="M39" s="29"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>100</v>
       </c>
@@ -3167,14 +3760,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D41" s="33"/>
       <c r="E41" s="1"/>
       <c r="K41" s="29"/>
       <c r="L41" s="29"/>
       <c r="M41" s="29"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>113</v>
       </c>
@@ -3196,7 +3789,7 @@
       <c r="L42" s="29"/>
       <c r="M42" s="29"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>116</v>
       </c>
@@ -3215,7 +3808,7 @@
       <c r="L43" s="29"/>
       <c r="M43" s="29"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>118</v>
       </c>
@@ -3234,7 +3827,7 @@
       <c r="L44" s="29"/>
       <c r="M44" s="29"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>120</v>
       </c>
@@ -3253,7 +3846,7 @@
       <c r="L45" s="29"/>
       <c r="M45" s="29"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>122</v>
       </c>
@@ -3272,7 +3865,7 @@
       <c r="L46" s="29"/>
       <c r="M46" s="29"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>124</v>
       </c>
@@ -3291,7 +3884,7 @@
       <c r="L47" s="29"/>
       <c r="M47" s="29"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>100</v>
       </c>
@@ -3302,7 +3895,7 @@
       <c r="L48" s="29"/>
       <c r="M48" s="29"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D49" s="33"/>
       <c r="E49" s="1"/>
       <c r="J49" s="1"/>
@@ -3310,7 +3903,7 @@
       <c r="L49" s="29"/>
       <c r="M49" s="29"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>126</v>
       </c>
@@ -3335,7 +3928,7 @@
       </c>
       <c r="M50" s="31"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D51" s="33"/>
       <c r="E51" s="4"/>
       <c r="J51" s="1"/>
@@ -3343,12 +3936,15 @@
       <c r="L51" s="31"/>
       <c r="M51" s="31"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>129</v>
       </c>
       <c r="B52" t="s">
         <v>130</v>
+      </c>
+      <c r="C52" t="s">
+        <v>182</v>
       </c>
       <c r="D52" s="33">
         <f t="shared" si="0"/>
@@ -3362,7 +3958,7 @@
       <c r="L52" s="29"/>
       <c r="M52" s="29"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D53" s="33"/>
       <c r="E53" s="1"/>
       <c r="J53" s="1"/>
@@ -3370,7 +3966,7 @@
       <c r="L53" s="29"/>
       <c r="M53" s="29"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>131</v>
       </c>
@@ -3393,7 +3989,7 @@
       <c r="L54" s="29"/>
       <c r="M54" s="29"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>134</v>
       </c>
@@ -3413,105 +4009,105 @@
       <c r="L55" s="29"/>
       <c r="M55" s="29"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="29"/>
       <c r="L56" s="29"/>
       <c r="M56" s="29"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="29"/>
       <c r="L57" s="29"/>
       <c r="M57" s="29"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="29"/>
       <c r="L58" s="29"/>
       <c r="M58" s="29"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="29"/>
       <c r="L59" s="29"/>
       <c r="M59" s="29"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E62" s="21"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="2:13">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E65" s="2"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="2:13">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="2:13">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="2:13">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="2:13">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="2:13">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
       <c r="D70" s="22"/>
@@ -3521,28 +4117,28 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="2:13">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E71" s="21"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="2:13">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="2:13">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="2:13">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
@@ -3556,14 +4152,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A46C4D-B66C-44B4-A2C1-BFC1CE0490BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D12"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
@@ -3575,7 +4171,7 @@
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>37</v>
       </c>
@@ -3611,7 +4207,7 @@
       </c>
       <c r="N1" s="28"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -3651,7 +4247,7 @@
       <c r="M2" s="29"/>
       <c r="N2" s="28"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>51</v>
       </c>
@@ -3683,7 +4279,7 @@
       <c r="M3" s="29"/>
       <c r="N3" s="28"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
         <v>53</v>
       </c>
@@ -3703,7 +4299,7 @@
       <c r="M4" s="32"/>
       <c r="N4" s="28"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
         <v>55</v>
       </c>
@@ -3723,7 +4319,7 @@
       <c r="M5" s="32"/>
       <c r="N5" s="28"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
         <v>57</v>
       </c>
@@ -3744,7 +4340,7 @@
       <c r="M6" s="32"/>
       <c r="N6" s="28"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
         <v>59</v>
       </c>
@@ -3762,7 +4358,7 @@
       <c r="M7" s="32"/>
       <c r="N7" s="28"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
         <v>60</v>
       </c>
@@ -3775,7 +4371,7 @@
       <c r="M8" s="32"/>
       <c r="N8" s="28"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
         <v>61</v>
       </c>
@@ -3788,7 +4384,7 @@
       <c r="M9" s="32"/>
       <c r="N9" s="28"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
         <v>62</v>
       </c>
@@ -3801,7 +4397,7 @@
       <c r="M10" s="32"/>
       <c r="N10" s="28"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
         <v>63</v>
       </c>
@@ -3814,7 +4410,7 @@
       <c r="M11" s="32"/>
       <c r="N11" s="28"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="1"/>
       <c r="J12" s="1"/>
@@ -3823,7 +4419,7 @@
       <c r="M12" s="29"/>
       <c r="N12" s="28"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>142</v>
       </c>
@@ -3846,7 +4442,7 @@
       <c r="M13" s="29"/>
       <c r="N13" s="28"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>67</v>
       </c>
@@ -3866,7 +4462,7 @@
       <c r="M14" s="29"/>
       <c r="N14" s="28"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>69</v>
       </c>
@@ -3886,7 +4482,7 @@
       <c r="M15" s="29"/>
       <c r="N15" s="28"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>71</v>
       </c>
@@ -3906,7 +4502,7 @@
       <c r="M16" s="29"/>
       <c r="N16" s="28"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="1"/>
       <c r="J17" s="1"/>
@@ -3915,7 +4511,7 @@
       <c r="M17" s="29"/>
       <c r="N17" s="28"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>147</v>
       </c>
@@ -3935,7 +4531,7 @@
       <c r="M18" s="29"/>
       <c r="N18" s="28"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="1"/>
       <c r="J19" s="1"/>
@@ -3944,7 +4540,7 @@
       <c r="M19" s="29"/>
       <c r="N19" s="28"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3967,7 +4563,7 @@
       <c r="M20" s="29"/>
       <c r="N20" s="28"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>78</v>
       </c>
@@ -3987,7 +4583,7 @@
       <c r="M21" s="29"/>
       <c r="N21" s="28"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>80</v>
       </c>
@@ -4007,7 +4603,7 @@
       <c r="M22" s="29"/>
       <c r="N22" s="28"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>82</v>
       </c>
@@ -4027,7 +4623,7 @@
       <c r="M23" s="29"/>
       <c r="N23" s="28"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>84</v>
       </c>
@@ -4047,7 +4643,7 @@
       <c r="M24" s="29"/>
       <c r="N24" s="28"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>86</v>
       </c>
@@ -4067,7 +4663,7 @@
       <c r="M25" s="29"/>
       <c r="N25" s="28"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>88</v>
       </c>
@@ -4087,7 +4683,7 @@
       <c r="M26" s="29"/>
       <c r="N26" s="28"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>90</v>
       </c>
@@ -4107,7 +4703,7 @@
       <c r="M27" s="29"/>
       <c r="N27" s="28"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>92</v>
       </c>
@@ -4127,7 +4723,7 @@
       <c r="M28" s="29"/>
       <c r="N28" s="28"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>94</v>
       </c>
@@ -4147,7 +4743,7 @@
       <c r="M29" s="29"/>
       <c r="N29" s="28"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>96</v>
       </c>
@@ -4167,7 +4763,7 @@
       <c r="M30" s="29"/>
       <c r="N30" s="28"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>160</v>
       </c>
@@ -4182,7 +4778,7 @@
       <c r="M31" s="29"/>
       <c r="N31" s="28"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>100</v>
       </c>
@@ -4194,7 +4790,7 @@
       <c r="M32" s="29"/>
       <c r="N32" s="28"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D33" s="34"/>
       <c r="E33" s="1"/>
       <c r="J33" s="1"/>
@@ -4203,7 +4799,7 @@
       <c r="M33" s="29"/>
       <c r="N33" s="28"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>162</v>
       </c>
@@ -4226,7 +4822,7 @@
       <c r="M34" s="32"/>
       <c r="N34" s="28"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>105</v>
       </c>
@@ -4246,7 +4842,7 @@
       <c r="M35" s="32"/>
       <c r="N35" s="28"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>107</v>
       </c>
@@ -4266,7 +4862,7 @@
       <c r="M36" s="32"/>
       <c r="N36" s="28"/>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>109</v>
       </c>
@@ -4286,7 +4882,7 @@
       <c r="M37" s="32"/>
       <c r="N37" s="28"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>111</v>
       </c>
@@ -4306,7 +4902,7 @@
       <c r="M38" s="32"/>
       <c r="N38" s="28"/>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>100</v>
       </c>
@@ -4325,7 +4921,7 @@
       <c r="M39" s="29"/>
       <c r="N39" s="28"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D40" s="34"/>
       <c r="E40" s="1"/>
       <c r="J40" s="1"/>
@@ -4334,7 +4930,7 @@
       <c r="M40" s="29"/>
       <c r="N40" s="28"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>168</v>
       </c>
@@ -4357,7 +4953,7 @@
       <c r="M41" s="32"/>
       <c r="N41" s="28"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>116</v>
       </c>
@@ -4377,7 +4973,7 @@
       <c r="M42" s="32"/>
       <c r="N42" s="28"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>118</v>
       </c>
@@ -4397,7 +4993,7 @@
       <c r="M43" s="32"/>
       <c r="N43" s="28"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>120</v>
       </c>
@@ -4417,7 +5013,7 @@
       <c r="M44" s="32"/>
       <c r="N44" s="28"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>122</v>
       </c>
@@ -4437,7 +5033,7 @@
       <c r="M45" s="32"/>
       <c r="N45" s="28"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>124</v>
       </c>
@@ -4457,7 +5053,7 @@
       <c r="M46" s="32"/>
       <c r="N46" s="28"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>100</v>
       </c>
@@ -4469,7 +5065,7 @@
       <c r="M47" s="29"/>
       <c r="N47" s="28"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D48" s="34"/>
       <c r="E48" s="1"/>
       <c r="J48" s="1"/>
@@ -4478,7 +5074,7 @@
       <c r="M48" s="29"/>
       <c r="N48" s="28"/>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>175</v>
       </c>
@@ -4504,7 +5100,7 @@
       <c r="M49" s="30"/>
       <c r="N49" s="28"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D50" s="34"/>
       <c r="E50" s="1"/>
       <c r="J50" s="1"/>
@@ -4513,7 +5109,7 @@
       <c r="M50" s="29"/>
       <c r="N50" s="28"/>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>177</v>
       </c>
@@ -4536,7 +5132,7 @@
       <c r="M51" s="29"/>
       <c r="N51" s="28"/>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D52" s="34"/>
       <c r="E52" s="1"/>
       <c r="J52" s="1"/>
@@ -4545,7 +5141,7 @@
       <c r="M52" s="29"/>
       <c r="N52" s="28"/>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>179</v>
       </c>
@@ -4569,7 +5165,7 @@
       <c r="M53" s="29"/>
       <c r="N53" s="28"/>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>134</v>
       </c>
@@ -4589,7 +5185,7 @@
       <c r="M54" s="28"/>
       <c r="N54" s="28"/>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E55" s="1"/>
       <c r="J55" s="3"/>
       <c r="K55" s="29"/>
@@ -4597,7 +5193,7 @@
       <c r="M55" s="29"/>
       <c r="N55" s="28"/>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="29"/>
@@ -4605,7 +5201,7 @@
       <c r="M56" s="29"/>
       <c r="N56" s="28"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="29"/>
@@ -4613,7 +5209,7 @@
       <c r="M57" s="29"/>
       <c r="N57" s="28"/>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="29"/>
@@ -4621,7 +5217,7 @@
       <c r="M58" s="29"/>
       <c r="N58" s="28"/>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="29"/>
@@ -4629,7 +5225,7 @@
       <c r="M59" s="29"/>
       <c r="N59" s="28"/>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="29"/>
@@ -4637,7 +5233,7 @@
       <c r="M60" s="29"/>
       <c r="N60" s="28"/>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="29"/>
@@ -4645,7 +5241,7 @@
       <c r="M61" s="29"/>
       <c r="N61" s="28"/>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E62" s="2"/>
       <c r="J62" s="1"/>
       <c r="K62" s="29"/>
@@ -4653,49 +5249,49 @@
       <c r="M62" s="29"/>
       <c r="N62" s="28"/>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="5:13">
+    <row r="65" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="5:13">
+    <row r="66" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="5:13">
+    <row r="67" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="5:13">
+    <row r="68" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="5:13">
+    <row r="69" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>

</xml_diff>

<commit_message>
LvdB: reading the database, and added a new crop: mint
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
@@ -1329,7 +1329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="173">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -1349,33 +1349,21 @@
     <t>Lettuce</t>
   </si>
   <si>
-    <t>0.5863</t>
-  </si>
-  <si>
     <t>0.00000111</t>
   </si>
   <si>
     <t>Endive</t>
   </si>
   <si>
-    <t>0.5505</t>
-  </si>
-  <si>
     <t>Spinach</t>
   </si>
   <si>
-    <t>0.2268</t>
-  </si>
-  <si>
     <t>0.00001333</t>
   </si>
   <si>
     <t>Bean sprouts</t>
   </si>
   <si>
-    <t>0.0002328</t>
-  </si>
-  <si>
     <t>0.00005000</t>
   </si>
   <si>
@@ -1385,9 +1373,6 @@
     <t>Parsley</t>
   </si>
   <si>
-    <t>0.00458</t>
-  </si>
-  <si>
     <t>0.00000182</t>
   </si>
   <si>
@@ -1397,27 +1382,18 @@
     <t>Kale</t>
   </si>
   <si>
-    <t>0.040125</t>
-  </si>
-  <si>
     <t>0.00000364</t>
   </si>
   <si>
     <t>Basil</t>
   </si>
   <si>
-    <t>0.0966</t>
-  </si>
-  <si>
     <t>0.00000160</t>
   </si>
   <si>
     <t>Rucola</t>
   </si>
   <si>
-    <t>0.00626</t>
-  </si>
-  <si>
     <t>0.00000033</t>
   </si>
   <si>
@@ -1427,16 +1403,10 @@
     <t>Microgreen mix</t>
   </si>
   <si>
-    <t>0.3545</t>
-  </si>
-  <si>
     <t>0.00000085</t>
   </si>
   <si>
     <t>Mint</t>
-  </si>
-  <si>
-    <t>0.0791</t>
   </si>
   <si>
     <t>0.00000005</t>
@@ -1936,7 +1906,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2079,11 +2049,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2130,7 +2109,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2139,6 +2117,11 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2757,15 +2740,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="8" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" style="8" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="8" customWidth="1"/>
@@ -2774,7 +2757,7 @@
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -2792,18 +2775,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>6</v>
+      <c r="B2" s="9">
+        <v>0.58630000000000004</v>
       </c>
       <c r="C2" s="19">
         <v>0.8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="9">
         <v>620</v>
@@ -2811,19 +2794,22 @@
       <c r="F2" s="10">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.55049999999999999</v>
       </c>
       <c r="C3" s="19">
         <v>0.7</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="9">
         <v>710</v>
@@ -2832,18 +2818,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.2268</v>
       </c>
       <c r="C4" s="19">
         <v>0.6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" s="9">
         <v>1080</v>
@@ -2852,58 +2838,58 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2.3279999999999999E-4</v>
       </c>
       <c r="C5" s="19">
         <v>0.55000000000000004</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E5" s="9">
         <v>970</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4.5799999999999999E-3</v>
       </c>
       <c r="C6" s="19">
         <v>0.6</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E6" s="9">
         <v>1250</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="9">
+        <v>4.0125000000000001E-2</v>
       </c>
       <c r="C7" s="19">
         <v>0.75</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E7" s="9">
         <v>1930</v>
@@ -2912,18 +2898,18 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="9">
+        <v>9.6600000000000005E-2</v>
       </c>
       <c r="C8" s="19">
         <v>0.85</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E8" s="9">
         <v>2000</v>
@@ -2932,38 +2918,38 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="B9" s="9">
+        <v>6.2599999999999999E-3</v>
       </c>
       <c r="C9" s="19">
         <v>0.75</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E9" s="9">
         <v>980</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0.35449999999999998</v>
       </c>
       <c r="C10" s="19">
         <v>0.67</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E10" s="9">
         <v>790</v>
@@ -2972,18 +2958,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="B11" s="11">
+        <v>7.9100000000000004E-2</v>
       </c>
       <c r="C11" s="20">
         <v>0.5</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E11" s="11">
         <v>16760</v>
@@ -3002,8 +2988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,48 +3006,48 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="27" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1">
         <f>AVERAGE(E2:I2)</f>
@@ -3088,20 +3074,20 @@
         <v>5.9265000000000005E-2</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="30">
+      <c r="K2" s="29">
         <v>2E-3</v>
       </c>
-      <c r="L2" s="29">
+      <c r="L2" s="28">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="M2" s="29"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1">
         <f>AVERAGE(E3:I3)</f>
@@ -3123,24 +3109,24 @@
         <v>0.71640000000000004</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="29">
+      <c r="K3" s="28">
         <v>0.57150000000000001</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="28">
         <v>0.58150000000000002</v>
       </c>
-      <c r="M3" s="29">
+      <c r="M3" s="28">
         <v>0.47</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="33">
+        <v>43</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="32">
         <f>AVERAGE(E4:M4)</f>
         <v>7.3440000000000005E-2</v>
       </c>
@@ -3148,18 +3134,18 @@
       <c r="J4" s="1">
         <v>7.3440000000000005E-2</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="33">
+        <v>45</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="32">
         <f t="shared" ref="D5:D55" si="0">AVERAGE(E5:M5)</f>
         <v>1.6199999999999999E-2</v>
       </c>
@@ -3167,18 +3153,18 @@
       <c r="J5" s="1">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="33">
+        <v>47</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="32">
         <f t="shared" si="0"/>
         <v>0.13986000000000001</v>
       </c>
@@ -3187,16 +3173,16 @@
         <f>(0.1332+0.14652)/2</f>
         <v>0.13986000000000001</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="33">
+        <v>49</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="32">
         <f t="shared" si="0"/>
         <v>7.5599999999999999E-3</v>
       </c>
@@ -3204,77 +3190,77 @@
       <c r="J7" s="1">
         <v>7.5599999999999999E-3</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="33"/>
+        <v>50</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="33"/>
+        <v>51</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="33"/>
+        <v>52</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="33"/>
+        <v>53</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D12" s="33"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="33">
+        <v>56</v>
+      </c>
+      <c r="D13" s="32">
         <f t="shared" si="0"/>
         <v>3.2530000000000001</v>
       </c>
@@ -3282,18 +3268,18 @@
       <c r="J13" s="1">
         <v>3.2530000000000001</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="33">
+        <v>58</v>
+      </c>
+      <c r="D14" s="32">
         <f t="shared" si="0"/>
         <v>8.1639999999999997</v>
       </c>
@@ -3301,18 +3287,18 @@
       <c r="J14" s="1">
         <v>8.1639999999999997</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="33">
+        <v>60</v>
+      </c>
+      <c r="D15" s="32">
         <f t="shared" si="0"/>
         <v>3.0000000000000001E-3</v>
       </c>
@@ -3320,18 +3306,18 @@
       <c r="J15" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="33">
+        <v>62</v>
+      </c>
+      <c r="D16" s="32">
         <f t="shared" si="0"/>
         <v>3.8340000000000001</v>
       </c>
@@ -3339,26 +3325,26 @@
       <c r="J16" s="1">
         <v>3.8340000000000001</v>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D17" s="33"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="33">
+        <v>64</v>
+      </c>
+      <c r="D18" s="32">
         <f t="shared" si="0"/>
         <v>2.37</v>
       </c>
@@ -3366,289 +3352,289 @@
       <c r="J18" s="1">
         <v>2.37</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D19" s="33"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="33">
+        <v>67</v>
+      </c>
+      <c r="D20" s="32">
         <f t="shared" si="0"/>
         <v>2.29</v>
       </c>
       <c r="E20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29">
+      <c r="K20" s="28"/>
+      <c r="L20" s="28">
         <v>2.29</v>
       </c>
-      <c r="M20" s="29"/>
+      <c r="M20" s="28"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="33">
+        <v>69</v>
+      </c>
+      <c r="D21" s="32">
         <f t="shared" si="0"/>
         <v>1.74</v>
       </c>
       <c r="E21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29">
+      <c r="K21" s="28"/>
+      <c r="L21" s="28">
         <v>1.74</v>
       </c>
-      <c r="M21" s="29"/>
+      <c r="M21" s="28"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="33">
+        <v>71</v>
+      </c>
+      <c r="D22" s="32">
         <f t="shared" si="0"/>
         <v>0.61199999999999999</v>
       </c>
       <c r="E22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29">
+      <c r="K22" s="28"/>
+      <c r="L22" s="28">
         <v>0.61199999999999999</v>
       </c>
-      <c r="M22" s="29"/>
+      <c r="M22" s="28"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="33">
+        <v>73</v>
+      </c>
+      <c r="D23" s="32">
         <f t="shared" si="0"/>
         <v>0.55300000000000005</v>
       </c>
       <c r="E23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29">
+      <c r="K23" s="28"/>
+      <c r="L23" s="28">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M23" s="29"/>
+      <c r="M23" s="28"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="33">
+        <v>75</v>
+      </c>
+      <c r="D24" s="32">
         <f t="shared" si="0"/>
         <v>0.223</v>
       </c>
       <c r="E24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29">
+      <c r="K24" s="28"/>
+      <c r="L24" s="28">
         <v>0.223</v>
       </c>
-      <c r="M24" s="29"/>
+      <c r="M24" s="28"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="33">
+        <v>77</v>
+      </c>
+      <c r="D25" s="32">
         <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
       <c r="E25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29">
+      <c r="K25" s="28"/>
+      <c r="L25" s="28">
         <v>1.75</v>
       </c>
-      <c r="M25" s="29"/>
+      <c r="M25" s="28"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="33">
+        <v>79</v>
+      </c>
+      <c r="D26" s="32">
         <f t="shared" si="0"/>
         <v>8.3099999999999997E-3</v>
       </c>
       <c r="E26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29">
+      <c r="K26" s="28"/>
+      <c r="L26" s="28">
         <v>8.3099999999999997E-3</v>
       </c>
-      <c r="M26" s="29"/>
+      <c r="M26" s="28"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="33">
+        <v>81</v>
+      </c>
+      <c r="D27" s="32">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
       <c r="E27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29">
+      <c r="K27" s="28"/>
+      <c r="L27" s="28">
         <v>0.95</v>
       </c>
-      <c r="M27" s="29"/>
+      <c r="M27" s="28"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="33">
+        <v>83</v>
+      </c>
+      <c r="D28" s="32">
         <f t="shared" si="0"/>
         <v>0.56200000000000006</v>
       </c>
       <c r="E28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29">
+      <c r="K28" s="28"/>
+      <c r="L28" s="28">
         <v>0.56200000000000006</v>
       </c>
-      <c r="M28" s="29"/>
+      <c r="M28" s="28"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="33">
+        <v>85</v>
+      </c>
+      <c r="D29" s="32">
         <f t="shared" si="0"/>
         <v>1.9E-2</v>
       </c>
       <c r="E29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29">
+      <c r="K29" s="28"/>
+      <c r="L29" s="28">
         <v>1.9E-2</v>
       </c>
-      <c r="M29" s="29"/>
+      <c r="M29" s="28"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="33">
+        <v>87</v>
+      </c>
+      <c r="D30" s="32">
         <f t="shared" si="0"/>
         <v>0.91700000000000004</v>
       </c>
       <c r="E30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29">
+      <c r="K30" s="28"/>
+      <c r="L30" s="28">
         <v>0.91700000000000004</v>
       </c>
-      <c r="M30" s="29"/>
+      <c r="M30" s="28"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="33"/>
+        <v>89</v>
+      </c>
+      <c r="D31" s="32"/>
       <c r="E31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="33">
+        <v>90</v>
+      </c>
+      <c r="D32" s="32">
         <f t="shared" si="0"/>
         <v>0.87493727272727273</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29">
+      <c r="K32" s="28"/>
+      <c r="L32" s="28">
         <f>AVERAGE(L20:L30)</f>
         <v>0.87493727272727273</v>
       </c>
-      <c r="M32" s="29"/>
+      <c r="M32" s="28"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="33"/>
+        <v>91</v>
+      </c>
+      <c r="D33" s="32"/>
       <c r="E33" s="1"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D34" s="33"/>
+      <c r="D34" s="32"/>
       <c r="E34" s="1"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="33">
+        <v>94</v>
+      </c>
+      <c r="D35" s="32">
         <f t="shared" si="0"/>
         <v>12.4</v>
       </c>
@@ -3656,18 +3642,18 @@
       <c r="J35" s="1">
         <v>12.4</v>
       </c>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="33">
+        <v>96</v>
+      </c>
+      <c r="D36" s="32">
         <f t="shared" si="0"/>
         <v>15.236666666666666</v>
       </c>
@@ -3675,22 +3661,22 @@
       <c r="J36" s="1">
         <v>26.7</v>
       </c>
-      <c r="K36" s="29">
+      <c r="K36" s="28">
         <v>9.2200000000000006</v>
       </c>
-      <c r="L36" s="29">
+      <c r="L36" s="28">
         <v>9.7899999999999991</v>
       </c>
-      <c r="M36" s="29"/>
+      <c r="M36" s="28"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="33">
+        <v>98</v>
+      </c>
+      <c r="D37" s="32">
         <f t="shared" si="0"/>
         <v>22.6</v>
       </c>
@@ -3698,18 +3684,18 @@
       <c r="J37" s="1">
         <v>22.6</v>
       </c>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="33">
+        <v>100</v>
+      </c>
+      <c r="D38" s="32">
         <f t="shared" si="0"/>
         <v>16.7</v>
       </c>
@@ -3717,18 +3703,18 @@
       <c r="J38" s="1">
         <v>16.7</v>
       </c>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" s="33">
+        <v>102</v>
+      </c>
+      <c r="D39" s="32">
         <f t="shared" si="0"/>
         <v>12.7</v>
       </c>
@@ -3736,15 +3722,15 @@
       <c r="J39" s="1">
         <v>12.7</v>
       </c>
-      <c r="K39" s="29"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="29"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="28"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40" s="33">
+        <v>90</v>
+      </c>
+      <c r="D40" s="32">
         <f t="shared" si="0"/>
         <v>18.156666666666666</v>
       </c>
@@ -3752,32 +3738,32 @@
       <c r="J40">
         <v>25.5</v>
       </c>
-      <c r="K40" s="29"/>
-      <c r="L40" s="28">
+      <c r="K40" s="28"/>
+      <c r="L40" s="27">
         <v>10.97</v>
       </c>
-      <c r="M40" s="28">
+      <c r="M40" s="27">
         <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D41" s="33"/>
+      <c r="D41" s="32"/>
       <c r="E41" s="1"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="33">
+        <v>105</v>
+      </c>
+      <c r="D42" s="32">
         <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
@@ -3785,18 +3771,18 @@
       <c r="J42" s="1">
         <v>1.08</v>
       </c>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" s="33">
+        <v>107</v>
+      </c>
+      <c r="D43" s="32">
         <f t="shared" si="0"/>
         <v>1.32</v>
       </c>
@@ -3804,18 +3790,18 @@
       <c r="J43" s="1">
         <v>1.32</v>
       </c>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" s="33">
+        <v>109</v>
+      </c>
+      <c r="D44" s="32">
         <f t="shared" si="0"/>
         <v>0.33400000000000002</v>
       </c>
@@ -3823,18 +3809,18 @@
       <c r="J44" s="1">
         <v>0.33400000000000002</v>
       </c>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
-      </c>
-      <c r="D45" s="33">
+        <v>111</v>
+      </c>
+      <c r="D45" s="32">
         <f t="shared" si="0"/>
         <v>-0.62</v>
       </c>
@@ -3842,18 +3828,18 @@
       <c r="J45" s="1">
         <v>-0.62</v>
       </c>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="29"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="33">
+        <v>113</v>
+      </c>
+      <c r="D46" s="32">
         <f t="shared" si="0"/>
         <v>2.2700000000000001E-2</v>
       </c>
@@ -3861,18 +3847,18 @@
       <c r="J46" s="1">
         <v>2.2700000000000001E-2</v>
       </c>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
-      </c>
-      <c r="D47" s="33">
+        <v>115</v>
+      </c>
+      <c r="D47" s="32">
         <f t="shared" si="0"/>
         <v>0.1719</v>
       </c>
@@ -3880,40 +3866,40 @@
       <c r="J47" s="1">
         <v>0.1719</v>
       </c>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>100</v>
-      </c>
-      <c r="D48" s="33"/>
+        <v>90</v>
+      </c>
+      <c r="D48" s="32"/>
       <c r="E48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D49" s="33"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="29"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
-      </c>
-      <c r="D50" s="33">
+        <v>118</v>
+      </c>
+      <c r="D50" s="32">
         <f t="shared" si="0"/>
         <v>5.1250000000000004E-4</v>
       </c>
@@ -3921,32 +3907,32 @@
         <v>6.2500000000000001E-4</v>
       </c>
       <c r="J50" s="5"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="31">
+      <c r="K50" s="28"/>
+      <c r="L50" s="30">
         <f>0.0004</f>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="M50" s="31"/>
+      <c r="M50" s="30"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D51" s="33"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="4"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="29"/>
-      <c r="L51" s="31"/>
-      <c r="M51" s="31"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="30"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C52" t="s">
-        <v>182</v>
-      </c>
-      <c r="D52" s="33">
+        <v>172</v>
+      </c>
+      <c r="D52" s="32">
         <f t="shared" si="0"/>
         <v>0.28999999999999998</v>
       </c>
@@ -3954,88 +3940,86 @@
       <c r="J52" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="29"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D53" s="33"/>
+      <c r="D53" s="32"/>
       <c r="E53" s="1"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="33">
-        <f t="shared" si="0"/>
-        <v>1.6386666999999999E-4</v>
+        <v>123</v>
+      </c>
+      <c r="D54" s="35">
+        <v>5</v>
       </c>
       <c r="E54" s="3"/>
       <c r="J54" s="24">
         <f>0.16386667/1000</f>
         <v>1.6386666999999999E-4</v>
       </c>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="28"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>135</v>
-      </c>
-      <c r="D55" s="33">
-        <f t="shared" si="0"/>
-        <v>1.89E-3</v>
+        <v>125</v>
+      </c>
+      <c r="D55" s="35">
+        <v>5</v>
       </c>
       <c r="E55" s="1"/>
       <c r="J55">
         <f>1.89/1000</f>
         <v>1.89E-3</v>
       </c>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="28"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="29"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="29"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="28"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="29"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="29"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="28"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="29"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="28"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="29"/>
+      <c r="K59" s="28"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="28"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
@@ -4147,7 +4131,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4155,8 +4140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4173,49 +4158,49 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="28"/>
+      <c r="N1" s="27"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D2" s="1">
         <f>AVERAGE(E2:I2)</f>
@@ -4242,17 +4227,17 @@
         <v>0.35118000000000005</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D3" s="1">
         <f>AVERAGE(E3:I3)</f>
@@ -4274,19 +4259,19 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="34">
+        <v>43</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="33">
         <f>AVERAGE(E4:N4)</f>
         <v>1.008</v>
       </c>
@@ -4294,19 +4279,19 @@
       <c r="J4" s="7">
         <v>1.008</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="28"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" s="34">
+        <v>45</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="33">
         <f t="shared" ref="D5:D54" si="0">AVERAGE(E5:N5)</f>
         <v>0.18720000000000001</v>
       </c>
@@ -4314,19 +4299,19 @@
       <c r="J5" s="7">
         <v>0.18720000000000001</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="28"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="34">
+        <v>47</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="33">
         <f t="shared" si="0"/>
         <v>0.15192</v>
       </c>
@@ -4335,17 +4320,17 @@
         <f>(0.1332+0.17064)/2</f>
         <v>0.15192</v>
       </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="28"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="27"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="34">
+        <v>49</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="33">
         <f t="shared" si="0"/>
         <v>5.7599999999999998E-2</v>
       </c>
@@ -4353,83 +4338,83 @@
       <c r="J7" s="7">
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="28"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="34"/>
+        <v>50</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="7"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="28"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="27"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="34"/>
+        <v>51</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="28"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="27"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="34"/>
+        <v>52</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="28"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="27"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="34"/>
+        <v>53</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="28"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="27"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="34"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="27"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D13" s="34">
+        <v>133</v>
+      </c>
+      <c r="D13" s="33">
         <f t="shared" si="0"/>
         <v>82.275999999999996</v>
       </c>
@@ -4437,19 +4422,19 @@
       <c r="J13" s="1">
         <v>82.275999999999996</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="27"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D14" s="34">
+        <v>134</v>
+      </c>
+      <c r="D14" s="33">
         <f t="shared" si="0"/>
         <v>144.43</v>
       </c>
@@ -4457,19 +4442,19 @@
       <c r="J14" s="1">
         <v>144.43</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="27"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D15" s="34">
+        <v>135</v>
+      </c>
+      <c r="D15" s="33">
         <f t="shared" si="0"/>
         <v>7.3999999999999996E-2</v>
       </c>
@@ -4477,19 +4462,19 @@
       <c r="J15" s="1">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="27"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" s="34">
+        <v>136</v>
+      </c>
+      <c r="D16" s="33">
         <f t="shared" si="0"/>
         <v>97.024000000000001</v>
       </c>
@@ -4497,28 +4482,28 @@
       <c r="J16" s="1">
         <v>97.024000000000001</v>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="34"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="34">
+        <v>64</v>
+      </c>
+      <c r="D18" s="33">
         <f t="shared" si="0"/>
         <v>37.700000000000003</v>
       </c>
@@ -4526,290 +4511,294 @@
       <c r="J18" s="1">
         <v>37.700000000000003</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="27"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="34"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="27"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D20" s="34">
+        <v>139</v>
+      </c>
+      <c r="D20" s="33">
         <f t="shared" si="0"/>
         <v>14.5</v>
       </c>
       <c r="E20" s="7"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32">
+      <c r="K20" s="31"/>
+      <c r="L20" s="31">
         <v>14.5</v>
       </c>
-      <c r="M20" s="29"/>
-      <c r="N20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="27"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D21" s="34">
+        <v>140</v>
+      </c>
+      <c r="D21" s="33">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E21" s="7"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32">
+      <c r="K21" s="31"/>
+      <c r="L21" s="31">
         <v>11</v>
       </c>
-      <c r="M21" s="29"/>
-      <c r="N21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="27"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D22" s="34">
+        <v>141</v>
+      </c>
+      <c r="D22" s="33">
         <f t="shared" si="0"/>
         <v>15.6</v>
       </c>
       <c r="E22" s="7"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32">
+      <c r="K22" s="31"/>
+      <c r="L22" s="31">
         <v>15.6</v>
       </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="27"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D23" s="34">
+        <v>142</v>
+      </c>
+      <c r="D23" s="33">
         <f t="shared" si="0"/>
         <v>13.7</v>
       </c>
       <c r="E23" s="7"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32">
+      <c r="K23" s="31"/>
+      <c r="L23" s="31">
         <v>13.7</v>
       </c>
-      <c r="M23" s="29"/>
-      <c r="N23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="27"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="34">
+        <v>143</v>
+      </c>
+      <c r="D24" s="33">
         <f t="shared" si="0"/>
         <v>5.54</v>
       </c>
       <c r="E24" s="7"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32">
+      <c r="K24" s="31"/>
+      <c r="L24" s="31">
         <v>5.54</v>
       </c>
-      <c r="M24" s="29"/>
-      <c r="N24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="27"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D25" s="34">
+        <v>144</v>
+      </c>
+      <c r="D25" s="33">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="E25" s="7"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32">
+      <c r="K25" s="31"/>
+      <c r="L25" s="31">
         <v>34</v>
       </c>
-      <c r="M25" s="29"/>
-      <c r="N25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="27"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" s="34">
+        <v>145</v>
+      </c>
+      <c r="D26" s="33">
         <f t="shared" si="0"/>
         <v>8.7599999999999997E-2</v>
       </c>
       <c r="E26" s="7"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32">
+      <c r="K26" s="31"/>
+      <c r="L26" s="31">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="M26" s="29"/>
-      <c r="N26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="27"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D27" s="34">
+        <v>146</v>
+      </c>
+      <c r="D27" s="33">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E27" s="7"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32">
+      <c r="K27" s="31"/>
+      <c r="L27" s="31">
         <v>12</v>
       </c>
-      <c r="M27" s="29"/>
-      <c r="N27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="27"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D28" s="34">
+        <v>147</v>
+      </c>
+      <c r="D28" s="33">
         <f t="shared" si="0"/>
         <v>24.3</v>
       </c>
       <c r="E28" s="7"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32">
+      <c r="K28" s="31"/>
+      <c r="L28" s="31">
         <v>24.3</v>
       </c>
-      <c r="M28" s="29"/>
-      <c r="N28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="27"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="34">
+        <v>148</v>
+      </c>
+      <c r="D29" s="33">
         <f t="shared" si="0"/>
         <v>1.6739999999999999</v>
       </c>
       <c r="E29" s="7"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32">
+      <c r="K29" s="31"/>
+      <c r="L29" s="31">
         <v>1.6739999999999999</v>
       </c>
-      <c r="M29" s="29"/>
-      <c r="N29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="27"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D30" s="34">
+        <v>149</v>
+      </c>
+      <c r="D30" s="33">
         <f t="shared" si="0"/>
         <v>11.9</v>
       </c>
       <c r="E30" s="7"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32">
+      <c r="K30" s="31"/>
+      <c r="L30" s="31">
         <v>11.9</v>
       </c>
-      <c r="M30" s="29"/>
-      <c r="N30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="27"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D31" s="34"/>
+        <v>151</v>
+      </c>
+      <c r="D31" s="35">
+        <v>8.7599999999999997E-2</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="28"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="M31" s="28"/>
+      <c r="N31" s="27"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="34"/>
+        <v>90</v>
+      </c>
+      <c r="D32" s="33"/>
       <c r="E32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="27"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D33" s="34"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="27"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="34">
+        <v>153</v>
+      </c>
+      <c r="D34" s="33">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
@@ -4817,19 +4806,19 @@
       <c r="J34" s="7">
         <v>160</v>
       </c>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="28"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="27"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D35" s="34">
+        <v>154</v>
+      </c>
+      <c r="D35" s="33">
         <f t="shared" si="0"/>
         <v>324</v>
       </c>
@@ -4837,19 +4826,19 @@
       <c r="J35" s="7">
         <v>324</v>
       </c>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="28"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="27"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D36" s="34">
+        <v>155</v>
+      </c>
+      <c r="D36" s="33">
         <f t="shared" si="0"/>
         <v>284</v>
       </c>
@@ -4857,19 +4846,19 @@
       <c r="J36" s="7">
         <v>284</v>
       </c>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="28"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="27"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D37" s="34">
+        <v>156</v>
+      </c>
+      <c r="D37" s="33">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
@@ -4877,19 +4866,19 @@
       <c r="J37" s="7">
         <v>210</v>
       </c>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="28"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="27"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D38" s="34">
+        <v>157</v>
+      </c>
+      <c r="D38" s="33">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
@@ -4897,16 +4886,16 @@
       <c r="J38" s="7">
         <v>156</v>
       </c>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="28"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="27"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>100</v>
-      </c>
-      <c r="D39" s="34">
+        <v>90</v>
+      </c>
+      <c r="D39" s="33">
         <f t="shared" si="0"/>
         <v>257.25</v>
       </c>
@@ -4914,33 +4903,33 @@
       <c r="J39" s="1">
         <v>264.5</v>
       </c>
-      <c r="K39" s="29">
+      <c r="K39" s="28">
         <v>250</v>
       </c>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="27"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D40" s="34"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="27"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D41" s="34">
+        <v>159</v>
+      </c>
+      <c r="D41" s="33">
         <f t="shared" si="0"/>
         <v>16.2</v>
       </c>
@@ -4948,19 +4937,19 @@
       <c r="J41" s="7">
         <v>16.2</v>
       </c>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="28"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="27"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D42" s="34">
+        <v>160</v>
+      </c>
+      <c r="D42" s="33">
         <f t="shared" si="0"/>
         <v>13.4</v>
       </c>
@@ -4968,19 +4957,19 @@
       <c r="J42" s="7">
         <v>13.4</v>
       </c>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="28"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="27"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D43" s="34">
+        <v>161</v>
+      </c>
+      <c r="D43" s="33">
         <f t="shared" si="0"/>
         <v>6.7</v>
       </c>
@@ -4988,19 +4977,19 @@
       <c r="J43" s="7">
         <v>6.7</v>
       </c>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="28"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="27"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="D44" s="34">
+        <v>162</v>
+      </c>
+      <c r="D44" s="33">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -5008,19 +4997,19 @@
       <c r="J44" s="7">
         <v>5</v>
       </c>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="28"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="27"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" s="34">
+        <v>163</v>
+      </c>
+      <c r="D45" s="33">
         <f t="shared" si="0"/>
         <v>9.1999999999999993</v>
       </c>
@@ -5028,19 +5017,19 @@
       <c r="J45" s="7">
         <v>9.1999999999999993</v>
       </c>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="28"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+      <c r="N45" s="27"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" s="34">
+        <v>164</v>
+      </c>
+      <c r="D46" s="33">
         <f t="shared" si="0"/>
         <v>1.849</v>
       </c>
@@ -5048,43 +5037,43 @@
       <c r="J46" s="7">
         <v>1.849</v>
       </c>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="28"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="27"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="34"/>
+        <v>90</v>
+      </c>
+      <c r="D47" s="33"/>
       <c r="E47" s="1"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
-      <c r="N47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
+      <c r="N47" s="27"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D48" s="34"/>
+      <c r="D48" s="33"/>
       <c r="E48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
-      <c r="N48" s="28"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="27"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
-      </c>
-      <c r="D49" s="34">
+        <v>166</v>
+      </c>
+      <c r="D49" s="33">
         <f t="shared" si="0"/>
         <v>8.7050000000000009E-3</v>
       </c>
@@ -5092,66 +5081,66 @@
         <v>1.0410000000000001E-2</v>
       </c>
       <c r="J49" s="1"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="30">
+      <c r="K49" s="28"/>
+      <c r="L49" s="29">
         <f>0.007</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="M49" s="30"/>
-      <c r="N49" s="28"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="27"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D50" s="34"/>
+      <c r="D50" s="33"/>
       <c r="E50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="28"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="28"/>
+      <c r="N50" s="27"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C51" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" s="34">
+        <v>168</v>
+      </c>
+      <c r="D51" s="33">
         <f t="shared" si="0"/>
         <v>5.54</v>
       </c>
       <c r="E51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="29">
+      <c r="K51" s="28">
         <v>5.54</v>
       </c>
-      <c r="L51" s="29"/>
-      <c r="M51" s="29"/>
-      <c r="N51" s="28"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="27"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D52" s="34"/>
+      <c r="D52" s="33"/>
       <c r="E52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="29"/>
-      <c r="N52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="27"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>180</v>
-      </c>
-      <c r="D53" s="34">
+        <v>170</v>
+      </c>
+      <c r="D53" s="33">
         <f t="shared" si="0"/>
         <v>2.3279999999999998E-3</v>
       </c>
@@ -5160,19 +5149,19 @@
         <f>2.328/1000</f>
         <v>2.3279999999999998E-3</v>
       </c>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
-      <c r="N53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="27"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>181</v>
-      </c>
-      <c r="D54" s="34">
+        <v>171</v>
+      </c>
+      <c r="D54" s="33">
         <f t="shared" si="0"/>
         <v>2.81E-2</v>
       </c>
@@ -5180,74 +5169,74 @@
         <f>28.1/1000</f>
         <v>2.81E-2</v>
       </c>
-      <c r="K54" s="28"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="28"/>
-      <c r="N54" s="28"/>
+      <c r="K54" s="27"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="27"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E55" s="1"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
-      <c r="N55" s="28"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="28"/>
+      <c r="N55" s="27"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="29"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="29"/>
-      <c r="N56" s="28"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="27"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="29"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="29"/>
-      <c r="N57" s="28"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="28"/>
+      <c r="N57" s="27"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="29"/>
-      <c r="N58" s="28"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="28"/>
+      <c r="N58" s="27"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="29"/>
-      <c r="N59" s="28"/>
+      <c r="K59" s="28"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="28"/>
+      <c r="N59" s="27"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="29"/>
-      <c r="N60" s="28"/>
+      <c r="K60" s="28"/>
+      <c r="L60" s="28"/>
+      <c r="M60" s="28"/>
+      <c r="N60" s="27"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="29"/>
-      <c r="L61" s="29"/>
-      <c r="M61" s="29"/>
-      <c r="N61" s="28"/>
+      <c r="K61" s="28"/>
+      <c r="L61" s="28"/>
+      <c r="M61" s="28"/>
+      <c r="N61" s="27"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E62" s="2"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="29"/>
-      <c r="L62" s="29"/>
-      <c r="M62" s="29"/>
-      <c r="N62" s="28"/>
+      <c r="K62" s="28"/>
+      <c r="L62" s="28"/>
+      <c r="M62" s="28"/>
+      <c r="N62" s="27"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E63" s="1"/>

</xml_diff>

<commit_message>
JW: minor changes to database and to program
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\school\WUR\Master\Programming in python\untitled\ACT\ACT2321\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="56" documentId="11_6B6BDCC092AD0B9DB47A7F677C23A1D7B8037EC4" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{03CD75EB-7C66-4958-965A-5ACF33C7F3A9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
     <sheet name="CO2eq (kg)" sheetId="1" r:id="rId2"/>
     <sheet name="Energy (MJ)" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={ED13EA6E-84B9-4566-9DD1-5F68795B2A3F}</author>
     <author>tc={AA2B32B5-7D1D-400A-A931-EBFBF82EF357}</author>
@@ -70,7 +70,7 @@
     <author>tc={3CBB2313-6869-4ADB-8678-F0A56C53B204}</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="1" shapeId="0">
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="2" shapeId="0">
+    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="3" shapeId="0">
+    <comment ref="D2" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="4" shapeId="0">
+    <comment ref="E2" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="5" shapeId="0">
+    <comment ref="F2" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -178,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="6" shapeId="0">
+    <comment ref="B3" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -196,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="7" shapeId="0">
+    <comment ref="F3" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="8" shapeId="0">
+    <comment ref="B4" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -232,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="9" shapeId="0">
+    <comment ref="B5" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -250,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="10" shapeId="0">
+    <comment ref="C5" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="11" shapeId="0">
+    <comment ref="D5" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="12" shapeId="0">
+    <comment ref="F5" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -304,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="13" shapeId="0">
+    <comment ref="B6" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -322,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="14" shapeId="0">
+    <comment ref="B7" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -340,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="15" shapeId="0">
+    <comment ref="F7" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="16" shapeId="0">
+    <comment ref="B8" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -376,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="17" shapeId="0">
+    <comment ref="C8" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -394,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="18" shapeId="0">
+    <comment ref="F8" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -412,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="19" shapeId="0">
+    <comment ref="B9" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -430,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="20" shapeId="0">
+    <comment ref="C9" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -448,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="21" shapeId="0">
+    <comment ref="D9" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -466,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="22" shapeId="0">
+    <comment ref="F9" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -484,7 +484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="23" shapeId="0">
+    <comment ref="A10" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -506,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="24" shapeId="0">
+    <comment ref="B10" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -529,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="25" shapeId="0">
+    <comment ref="C10" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -547,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="26" shapeId="0">
+    <comment ref="D10" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -566,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="27" shapeId="0">
+    <comment ref="E10" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -584,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="28" shapeId="0">
+    <comment ref="F10" authorId="28" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -604,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="29" shapeId="0">
+    <comment ref="B11" authorId="29" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -622,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="30" shapeId="0">
+    <comment ref="C11" authorId="30" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -640,7 +640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="31" shapeId="0">
+    <comment ref="D11" authorId="31" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -658,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="32" shapeId="0">
+    <comment ref="F11" authorId="32" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -681,7 +681,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={53C940E0-2140-41F9-A6DF-6EA835ABEC64}</author>
     <author>tc={F8E5DC3C-6251-4EB4-8D84-9AAD62A6919A}</author>
@@ -705,7 +705,7 @@
     <author>tc={7A90E5E2-2E08-4861-A6C8-2E490EE47A92}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -723,7 +723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="1" shapeId="0">
+    <comment ref="K2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -742,7 +742,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="2" shapeId="0">
+    <comment ref="L2" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -760,7 +760,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="3" shapeId="0">
+    <comment ref="E3" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -778,7 +778,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="4" shapeId="0">
+    <comment ref="M3" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -796,7 +796,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0">
+    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -814,7 +814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="6" shapeId="0">
+    <comment ref="J13" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -832,7 +832,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="7" shapeId="0">
+    <comment ref="J15" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -850,7 +850,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="8" shapeId="0">
+    <comment ref="J18" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -868,7 +868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L20" authorId="9" shapeId="0">
+    <comment ref="L20" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -888,7 +888,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L30" authorId="10" shapeId="0">
+    <comment ref="L30" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -906,7 +906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K36" authorId="11" shapeId="0">
+    <comment ref="K36" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -924,7 +924,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L36" authorId="12" shapeId="0">
+    <comment ref="L36" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -942,7 +942,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J40" authorId="13" shapeId="0">
+    <comment ref="J40" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -960,7 +960,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L40" authorId="14" shapeId="0">
+    <comment ref="L40" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -978,7 +978,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M40" authorId="15" shapeId="0">
+    <comment ref="M40" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
       <text>
         <r>
           <rPr>
@@ -996,7 +996,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J42" authorId="16" shapeId="0">
+    <comment ref="J42" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1014,7 +1014,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J44" authorId="17" shapeId="0">
+    <comment ref="J44" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0100-000012000000}">
       <text>
         <r>
           <rPr>
@@ -1032,7 +1032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J46" authorId="18" shapeId="0">
+    <comment ref="J46" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0100-000013000000}">
       <text>
         <r>
           <rPr>
@@ -1050,7 +1050,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E50" authorId="19" shapeId="0">
+    <comment ref="E50" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0100-000014000000}">
       <text>
         <r>
           <rPr>
@@ -1073,7 +1073,7 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={28C0A1D0-E24D-4A94-B8D7-08380DAD163B}</author>
     <author>tc={F1D6A124-94E9-4537-87FD-64C5756431CC}</author>
@@ -1090,7 +1090,7 @@
     <author>tc={EB5AF55A-D36E-4291-B324-6215D9703071}</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1108,7 +1108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="1" shapeId="0">
+    <comment ref="F3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1126,7 +1126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="2" shapeId="0">
+    <comment ref="G3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1144,7 +1144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="3" shapeId="0">
+    <comment ref="H3" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1162,7 +1162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="4" shapeId="0">
+    <comment ref="I3" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1180,7 +1180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0">
+    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1198,7 +1198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="6" shapeId="0">
+    <comment ref="J13" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1216,7 +1216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="7" shapeId="0">
+    <comment ref="J18" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1234,7 +1234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J39" authorId="8" shapeId="0">
+    <comment ref="J39" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1252,7 +1252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="9" shapeId="0">
+    <comment ref="K39" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -1270,7 +1270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J41" authorId="10" shapeId="0">
+    <comment ref="J41" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1288,7 +1288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="11" shapeId="0">
+    <comment ref="J43" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -1306,7 +1306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J45" authorId="12" shapeId="0">
+    <comment ref="J45" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1329,7 +1329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="176">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -1848,19 +1848,29 @@
   </si>
   <si>
     <t>Pac1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural gas </t>
+  </si>
+  <si>
+    <t>kg/m3!</t>
+  </si>
+  <si>
+    <t>MJ/m3!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.00000000"/>
     <numFmt numFmtId="169" formatCode="0.000000000"/>
+    <numFmt numFmtId="170" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -2062,7 +2072,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2122,6 +2132,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2739,10 +2752,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -2985,11 +2998,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,7 +3159,7 @@
         <v>46</v>
       </c>
       <c r="D5" s="32">
-        <f t="shared" ref="D5:D55" si="0">AVERAGE(E5:M5)</f>
+        <f t="shared" ref="D5:D52" si="0">AVERAGE(E5:M5)</f>
         <v>1.6199999999999999E-2</v>
       </c>
       <c r="E5" s="1"/>
@@ -3292,15 +3305,18 @@
       <c r="M14" s="28"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>174</v>
+      </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="C15" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="32">
-        <f t="shared" si="0"/>
-        <v>3.0000000000000001E-3</v>
+        <f>AVERAGE(E15:M15)*1000</f>
+        <v>3</v>
       </c>
       <c r="E15" s="1"/>
       <c r="J15" s="1">
@@ -3899,7 +3915,7 @@
       <c r="C50" t="s">
         <v>118</v>
       </c>
-      <c r="D50" s="32">
+      <c r="D50" s="38">
         <f t="shared" si="0"/>
         <v>5.1250000000000004E-4</v>
       </c>
@@ -3962,8 +3978,9 @@
       <c r="C54" t="s">
         <v>123</v>
       </c>
-      <c r="D54" s="35">
-        <v>5</v>
+      <c r="D54" s="37">
+        <f>J54</f>
+        <v>1.6386666999999999E-4</v>
       </c>
       <c r="E54" s="3"/>
       <c r="J54" s="24">
@@ -3981,8 +3998,9 @@
       <c r="C55" t="s">
         <v>125</v>
       </c>
-      <c r="D55" s="35">
-        <v>5</v>
+      <c r="D55" s="37">
+        <f>J55</f>
+        <v>1.89E-3</v>
       </c>
       <c r="E55" s="1"/>
       <c r="J55">
@@ -4137,11 +4155,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4448,6 +4466,9 @@
       <c r="N14" s="27"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>175</v>
+      </c>
       <c r="B15" t="s">
         <v>59</v>
       </c>
@@ -4455,8 +4476,8 @@
         <v>135</v>
       </c>
       <c r="D15" s="33">
-        <f t="shared" si="0"/>
-        <v>7.3999999999999996E-2</v>
+        <f>AVERAGE(E15:N15)*1000</f>
+        <v>74</v>
       </c>
       <c r="E15" s="1"/>
       <c r="J15" s="1">
@@ -5140,7 +5161,7 @@
       <c r="C53" t="s">
         <v>170</v>
       </c>
-      <c r="D53" s="33">
+      <c r="D53" s="39">
         <f t="shared" si="0"/>
         <v>2.3279999999999998E-3</v>
       </c>
@@ -5161,7 +5182,7 @@
       <c r="C54" t="s">
         <v>171</v>
       </c>
-      <c r="D54" s="33">
+      <c r="D54" s="39">
         <f t="shared" si="0"/>
         <v>2.81E-2</v>
       </c>

</xml_diff>

<commit_message>
JW: added the processing of several countries. Tool is ready to be sent to farmers.
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\school\WUR\Master\Programming in python\untitled\ACT\ACT2321\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_8B3EBB66534E5EAFCCD0CBF7BE2EBD154F0680BD" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{66F2AFF4-4861-4F87-9438-8CE6555FCC2A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
     <sheet name="Energy (MJ)" sheetId="2" r:id="rId2"/>
     <sheet name="CO2eq (kg)" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={ED13EA6E-84B9-4566-9DD1-5F68795B2A3F}</author>
     <author>tc={AA2B32B5-7D1D-400A-A931-EBFBF82EF357}</author>
@@ -70,7 +70,7 @@
     <author>tc={3CBB2313-6869-4ADB-8678-F0A56C53B204}</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="1" shapeId="0">
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="2" shapeId="0">
+    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="3" shapeId="0">
+    <comment ref="D2" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="4" shapeId="0">
+    <comment ref="E2" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="5" shapeId="0">
+    <comment ref="F2" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -178,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="6" shapeId="0">
+    <comment ref="B3" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -196,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="7" shapeId="0">
+    <comment ref="F3" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="8" shapeId="0">
+    <comment ref="B4" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -232,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="9" shapeId="0">
+    <comment ref="B5" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -250,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="10" shapeId="0">
+    <comment ref="C5" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="11" shapeId="0">
+    <comment ref="D5" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="12" shapeId="0">
+    <comment ref="F5" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -304,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="13" shapeId="0">
+    <comment ref="B6" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -322,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="14" shapeId="0">
+    <comment ref="B7" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -340,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="15" shapeId="0">
+    <comment ref="F7" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="16" shapeId="0">
+    <comment ref="B8" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -376,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="17" shapeId="0">
+    <comment ref="C8" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -394,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="18" shapeId="0">
+    <comment ref="F8" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -412,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="19" shapeId="0">
+    <comment ref="B9" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -430,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="20" shapeId="0">
+    <comment ref="C9" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -448,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="21" shapeId="0">
+    <comment ref="D9" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -466,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="22" shapeId="0">
+    <comment ref="F9" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -484,7 +484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="23" shapeId="0">
+    <comment ref="A10" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -506,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="24" shapeId="0">
+    <comment ref="B10" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -529,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="25" shapeId="0">
+    <comment ref="C10" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -547,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="26" shapeId="0">
+    <comment ref="D10" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -566,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="27" shapeId="0">
+    <comment ref="E10" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -584,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="28" shapeId="0">
+    <comment ref="F10" authorId="28" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -604,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="29" shapeId="0">
+    <comment ref="B11" authorId="29" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -622,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="30" shapeId="0">
+    <comment ref="C11" authorId="30" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -640,7 +640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="31" shapeId="0">
+    <comment ref="D11" authorId="31" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -658,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="32" shapeId="0">
+    <comment ref="F11" authorId="32" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -681,7 +681,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={28C0A1D0-E24D-4A94-B8D7-08380DAD163B}</author>
     <author>tc={F1D6A124-94E9-4537-87FD-64C5756431CC}</author>
@@ -702,7 +702,7 @@
     <author>tc={EB5AF55A-D36E-4291-B324-6215D9703071}</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -720,7 +720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="1" shapeId="0">
+    <comment ref="E3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -738,7 +738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="2" shapeId="0">
+    <comment ref="F3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -756,7 +756,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="3" shapeId="0">
+    <comment ref="G3" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -774,7 +774,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="4" shapeId="0">
+    <comment ref="H3" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -792,7 +792,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0">
+    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -810,7 +810,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="6" shapeId="0">
+    <comment ref="E8" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -828,7 +828,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="7" shapeId="0">
+    <comment ref="F8" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -846,7 +846,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="8" shapeId="0">
+    <comment ref="G8" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -864,7 +864,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="9" shapeId="0">
+    <comment ref="H8" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -882,7 +882,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="10" shapeId="0">
+    <comment ref="J13" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -900,7 +900,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="11" shapeId="0">
+    <comment ref="J18" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -918,7 +918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J39" authorId="12" shapeId="0">
+    <comment ref="J39" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -936,7 +936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="13" shapeId="0">
+    <comment ref="K39" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -954,7 +954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J41" authorId="14" shapeId="0">
+    <comment ref="J41" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -972,7 +972,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="15" shapeId="0">
+    <comment ref="J43" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
       <text>
         <r>
           <rPr>
@@ -990,7 +990,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J45" authorId="16" shapeId="0">
+    <comment ref="J45" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1013,7 +1013,7 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={53C940E0-2140-41F9-A6DF-6EA835ABEC64}</author>
     <author>tc={F8E5DC3C-6251-4EB4-8D84-9AAD62A6919A}</author>
@@ -1045,7 +1045,7 @@
     <author>tc={25BEEA18-2FB0-45C9-B9D8-E5E62F8643F3}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1063,7 +1063,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="1" shapeId="0">
+    <comment ref="K2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1082,7 +1082,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="2" shapeId="0">
+    <comment ref="L2" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1100,7 +1100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="3" shapeId="0">
+    <comment ref="D3" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1118,7 +1118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="4" shapeId="0">
+    <comment ref="M3" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1136,7 +1136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0">
+    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1154,7 +1154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="6" shapeId="0">
+    <comment ref="D8" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1172,7 +1172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="7" shapeId="0">
+    <comment ref="E8" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1190,7 +1190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="8" shapeId="0">
+    <comment ref="F8" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1208,7 +1208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="9" shapeId="0">
+    <comment ref="G8" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -1226,7 +1226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="10" shapeId="0">
+    <comment ref="H8" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1244,7 +1244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="11" shapeId="0">
+    <comment ref="J13" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -1262,7 +1262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="12" shapeId="0">
+    <comment ref="J15" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1280,7 +1280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="13" shapeId="0">
+    <comment ref="J18" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -1298,7 +1298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="14" shapeId="0">
+    <comment ref="J20" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -1318,7 +1318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L20" authorId="15" shapeId="0">
+    <comment ref="L20" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
       <text>
         <r>
           <rPr>
@@ -1338,7 +1338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J30" authorId="16" shapeId="0">
+    <comment ref="J30" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1356,7 +1356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L30" authorId="17" shapeId="0">
+    <comment ref="L30" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
       <text>
         <r>
           <rPr>
@@ -1374,7 +1374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K36" authorId="18" shapeId="0">
+    <comment ref="K36" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
       <text>
         <r>
           <rPr>
@@ -1392,7 +1392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L36" authorId="19" shapeId="0">
+    <comment ref="L36" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
       <text>
         <r>
           <rPr>
@@ -1410,7 +1410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J40" authorId="20" shapeId="0">
+    <comment ref="J40" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
       <text>
         <r>
           <rPr>
@@ -1428,7 +1428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L40" authorId="21" shapeId="0">
+    <comment ref="L40" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
       <text>
         <r>
           <rPr>
@@ -1446,7 +1446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M40" authorId="22" shapeId="0">
+    <comment ref="M40" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
       <text>
         <r>
           <rPr>
@@ -1464,7 +1464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J42" authorId="23" shapeId="0">
+    <comment ref="J42" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
       <text>
         <r>
           <rPr>
@@ -1482,7 +1482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J44" authorId="24" shapeId="0">
+    <comment ref="J44" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
       <text>
         <r>
           <rPr>
@@ -1500,7 +1500,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J46" authorId="25" shapeId="0">
+    <comment ref="J46" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -1518,7 +1518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="26" shapeId="0">
+    <comment ref="D50" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J50" authorId="27" shapeId="0">
+    <comment ref="J50" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -1559,7 +1559,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="176">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -2084,12 +2084,15 @@
   </si>
   <si>
     <t>T3</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -3020,10 +3023,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3263,11 +3266,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,7 +3298,7 @@
         <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
       <c r="H1" t="s">
         <v>32</v>
@@ -4355,7 +4358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
LvdB: update in database
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\school\WUR\Master\Programming in python\untitled\ACT\ACT2321\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_8B3EBB66534E5EAFCCD0CBF7BE2EBD154F0680BD" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{66F2AFF4-4861-4F87-9438-8CE6555FCC2A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
     <sheet name="Energy (MJ)" sheetId="2" r:id="rId2"/>
     <sheet name="CO2eq (kg)" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={ED13EA6E-84B9-4566-9DD1-5F68795B2A3F}</author>
     <author>tc={AA2B32B5-7D1D-400A-A931-EBFBF82EF357}</author>
@@ -70,7 +69,7 @@
     <author>tc={3CBB2313-6869-4ADB-8678-F0A56C53B204}</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C2" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="D2" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="E2" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="F2" authorId="5" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B3" authorId="6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="F3" authorId="7" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B4" authorId="8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B5" authorId="9" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -250,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="C5" authorId="10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -268,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="D5" authorId="11" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="F5" authorId="12" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -304,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="B6" authorId="13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -322,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="B7" authorId="14" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -340,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="F7" authorId="15" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -358,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="B8" authorId="16" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -376,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="C8" authorId="17" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -394,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="F8" authorId="18" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -412,7 +411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="B9" authorId="19" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -430,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="C9" authorId="20" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -448,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="D9" authorId="21" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="F9" authorId="22" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -484,7 +483,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="A10" authorId="23" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -506,7 +505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+    <comment ref="B10" authorId="24" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -529,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
+    <comment ref="C10" authorId="25" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
+    <comment ref="D10" authorId="26" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -566,7 +565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
+    <comment ref="E10" authorId="27" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -584,7 +583,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="28" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
+    <comment ref="F10" authorId="28" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -604,7 +603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="29" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
+    <comment ref="B11" authorId="29" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -622,7 +621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="30" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
+    <comment ref="C11" authorId="30" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -640,7 +639,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="31" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
+    <comment ref="D11" authorId="31" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -658,7 +657,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="32" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
+    <comment ref="F11" authorId="32" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -681,7 +680,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={28C0A1D0-E24D-4A94-B8D7-08380DAD163B}</author>
     <author>tc={F1D6A124-94E9-4537-87FD-64C5756431CC}</author>
@@ -702,7 +701,7 @@
     <author>tc={EB5AF55A-D36E-4291-B324-6215D9703071}</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -720,7 +719,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="E3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -738,7 +737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="F3" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -756,7 +755,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="G3" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -774,7 +773,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="H3" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -792,7 +791,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="J4" authorId="5" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -810,7 +809,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="E8" authorId="6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -828,7 +827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="F8" authorId="7" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -846,7 +845,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="G8" authorId="8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -864,7 +863,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="H8" authorId="9" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -882,7 +881,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="J13" authorId="10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -900,7 +899,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
+    <comment ref="J18" authorId="11" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -918,7 +917,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J39" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="J39" authorId="12" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -936,7 +935,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
+    <comment ref="K39" authorId="13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -954,7 +953,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J41" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
+    <comment ref="J41" authorId="14" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -972,7 +971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
+    <comment ref="J43" authorId="15" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -990,7 +989,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J45" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
+    <comment ref="J45" authorId="16" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1013,7 +1012,7 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={53C940E0-2140-41F9-A6DF-6EA835ABEC64}</author>
     <author>tc={F8E5DC3C-6251-4EB4-8D84-9AAD62A6919A}</author>
@@ -1045,7 +1044,7 @@
     <author>tc={25BEEA18-2FB0-45C9-B9D8-E5E62F8643F3}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1063,7 +1062,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="K2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1082,7 +1081,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="L2" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1100,7 +1099,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="D3" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1118,7 +1117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="M3" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1136,7 +1135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+    <comment ref="J4" authorId="5" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1154,7 +1153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
+    <comment ref="D8" authorId="6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1172,7 +1171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
+    <comment ref="E8" authorId="7" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1190,7 +1189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
+    <comment ref="F8" authorId="8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1208,7 +1207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
+    <comment ref="G8" authorId="9" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1226,7 +1225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
+    <comment ref="H8" authorId="10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1244,7 +1243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
+    <comment ref="J13" authorId="11" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1262,7 +1261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
+    <comment ref="J15" authorId="12" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1280,7 +1279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
+    <comment ref="J18" authorId="13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1298,7 +1297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
+    <comment ref="J20" authorId="14" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1318,7 +1317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L20" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
+    <comment ref="L20" authorId="15" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1338,7 +1337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J30" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
+    <comment ref="J30" authorId="16" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1356,7 +1355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L30" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
+    <comment ref="L30" authorId="17" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1374,7 +1373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K36" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
+    <comment ref="K36" authorId="18" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1392,7 +1391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L36" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
+    <comment ref="L36" authorId="19" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1410,7 +1409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J40" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
+    <comment ref="J40" authorId="20" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1428,7 +1427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L40" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
+    <comment ref="L40" authorId="21" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1446,7 +1445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M40" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
+    <comment ref="M40" authorId="22" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1464,7 +1463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J42" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
+    <comment ref="J42" authorId="23" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1482,7 +1481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J44" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
+    <comment ref="J44" authorId="24" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1500,7 +1499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J46" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
+    <comment ref="J46" authorId="25" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1518,7 +1517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
+    <comment ref="D50" authorId="26" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1535,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J50" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
+    <comment ref="J50" authorId="27" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1559,7 +1558,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="162">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -1579,69 +1578,33 @@
     <t>Lettuce</t>
   </si>
   <si>
-    <t>0.00000111</t>
-  </si>
-  <si>
     <t>Endive</t>
   </si>
   <si>
     <t>Spinach</t>
   </si>
   <si>
-    <t>0.00001333</t>
-  </si>
-  <si>
     <t>Bean sprouts</t>
   </si>
   <si>
-    <t>0.00005000</t>
-  </si>
-  <si>
-    <t>3.5</t>
-  </si>
-  <si>
     <t>Parsley</t>
   </si>
   <si>
-    <t>0.00000182</t>
-  </si>
-  <si>
-    <t>77.5</t>
-  </si>
-  <si>
     <t>Kale</t>
   </si>
   <si>
-    <t>0.00000364</t>
-  </si>
-  <si>
     <t>Basil</t>
   </si>
   <si>
-    <t>0.00000160</t>
-  </si>
-  <si>
     <t>Rucola</t>
   </si>
   <si>
-    <t>0.00000033</t>
-  </si>
-  <si>
-    <t>17.5</t>
-  </si>
-  <si>
     <t>Microgreen mix</t>
   </si>
   <si>
-    <t>0.00000085</t>
-  </si>
-  <si>
     <t>Mint</t>
   </si>
   <si>
-    <t>0.00000005</t>
-  </si>
-  <si>
     <t>Parameter Name</t>
   </si>
   <si>
@@ -1654,9 +1617,6 @@
     <t>China</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>Japan</t>
   </si>
   <si>
@@ -1712,9 +1672,6 @@
   </si>
   <si>
     <t>Solar energy (%)</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Wind energy (%)</t>
@@ -2092,14 +2049,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.00000000"/>
-    <numFmt numFmtId="169" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -2292,31 +2245,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2328,31 +2264,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -3023,241 +2964,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C13" activeCellId="1" sqref="B2:F11 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="25">
         <v>0.58630000000000004</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="25">
         <v>0.8</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="25">
+        <v>1.11E-6</v>
+      </c>
+      <c r="E2" s="25">
+        <v>620</v>
+      </c>
+      <c r="F2" s="26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9">
-        <v>620</v>
-      </c>
-      <c r="F2" s="10">
+      <c r="B3" s="25">
+        <v>0.55049999999999999</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="25">
+        <v>1.11E-6</v>
+      </c>
+      <c r="E3" s="25">
+        <v>710</v>
+      </c>
+      <c r="F3" s="26">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="25">
+        <v>0.2268</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="D4" s="25">
+        <v>1.3329999999999999E-5</v>
+      </c>
+      <c r="E4" s="25">
+        <v>1080</v>
+      </c>
+      <c r="F4" s="26">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="9">
-        <v>0.55049999999999999</v>
-      </c>
-      <c r="C3" s="19">
-        <v>0.7</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="9">
-        <v>710</v>
-      </c>
-      <c r="F3" s="10">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9">
-        <v>0.2268</v>
-      </c>
-      <c r="C4" s="19">
+      <c r="B5" s="25">
+        <v>2.3279999999999999E-4</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D5" s="25">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="E5" s="25">
+        <v>970</v>
+      </c>
+      <c r="F5" s="26">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="25">
+        <v>4.5799999999999999E-3</v>
+      </c>
+      <c r="C6" s="25">
         <v>0.6</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1080</v>
-      </c>
-      <c r="F4" s="10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="D6" s="25">
+        <v>1.8199999999999999E-6</v>
+      </c>
+      <c r="E6" s="25">
+        <v>1250</v>
+      </c>
+      <c r="F6" s="26">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9">
-        <v>2.3279999999999999E-4</v>
-      </c>
-      <c r="C5" s="19">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="B7" s="25">
+        <v>4.0125000000000001E-2</v>
+      </c>
+      <c r="C7" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="25">
+        <v>3.6399999999999999E-6</v>
+      </c>
+      <c r="E7" s="25">
+        <v>1930</v>
+      </c>
+      <c r="F7" s="26">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="9">
-        <v>970</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="B8" s="25">
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="C8" s="25">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="25">
+        <v>1.5999999999999999E-6</v>
+      </c>
+      <c r="E8" s="25">
+        <v>2000</v>
+      </c>
+      <c r="F8" s="26">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="B9" s="25">
+        <v>6.2599999999999999E-3</v>
+      </c>
+      <c r="C9" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="25">
+        <v>3.3000000000000002E-7</v>
+      </c>
+      <c r="E9" s="25">
+        <v>980</v>
+      </c>
+      <c r="F9" s="26">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="9">
-        <v>4.5799999999999999E-3</v>
-      </c>
-      <c r="C6" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="B10" s="25">
+        <v>0.35449999999999998</v>
+      </c>
+      <c r="C10" s="25">
+        <v>0.67</v>
+      </c>
+      <c r="D10" s="25">
+        <v>8.5000000000000001E-7</v>
+      </c>
+      <c r="E10" s="25">
+        <v>790</v>
+      </c>
+      <c r="F10" s="26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="9">
-        <v>1250</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="9">
-        <v>4.0125000000000001E-2</v>
-      </c>
-      <c r="C7" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="9">
-        <v>1930</v>
-      </c>
-      <c r="F7" s="10">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="9">
-        <v>9.6600000000000005E-2</v>
-      </c>
-      <c r="C8" s="19">
-        <v>0.85</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="9">
-        <v>2000</v>
-      </c>
-      <c r="F8" s="10">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="9">
-        <v>6.2599999999999999E-3</v>
-      </c>
-      <c r="C9" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="9">
-        <v>980</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0.35449999999999998</v>
-      </c>
-      <c r="C10" s="19">
-        <v>0.67</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="9">
-        <v>790</v>
-      </c>
-      <c r="F10" s="10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="11">
+      <c r="B11" s="27">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="27">
         <v>0.5</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="11">
+      <c r="D11" s="27">
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="E11" s="27">
         <v>16760</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="28">
         <v>90</v>
       </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3266,11 +3210,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,49 +3230,49 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="28"/>
+        <v>21</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1">
         <f>(D8*J4+D9*J5+D10*J6+D11*J7)/108.4</f>
@@ -3350,957 +3294,1188 @@
         <f>(J4*H8+J5*H9+H10*J6+H11*J7)/SUM(H8:H11)</f>
         <v>0.45990486486486493</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>0.38519999999999999</v>
       </c>
       <c r="J2" s="1">
         <f>AVERAGE(D2:I2)</f>
         <v>0.26047889689199161</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="28"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="18"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1">
         <v>7.8840000000000003</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>7.3079999999999998</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>10.44</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>6.1920000000000002</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>9.5399999999999991</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>0.38519999999999999</v>
       </c>
       <c r="J3" s="1">
         <f>AVERAGE(D3:I3)</f>
         <v>6.9581999999999988</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="28"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="18"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="J4" s="7">
+      <c r="B4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="5">
         <v>1.008</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="28"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="18"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="J5" s="7">
+      <c r="B5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="5">
         <v>0.18720000000000001</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="28"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="18"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="J6" s="7">
+      <c r="B6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="5">
         <f>(0.1332+0.17064)/2</f>
         <v>0.15192</v>
       </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="28"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="18"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="7"/>
-      <c r="J7" s="7">
+      <c r="B7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="5">
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="28"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="18"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="27"/>
+      <c r="B8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="17"/>
       <c r="D8" s="1">
         <v>6.4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>11.7</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="24">
         <v>0.35</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>7.14</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>7</v>
       </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="28"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="27"/>
+      <c r="B9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="17"/>
       <c r="D9" s="1">
         <v>16.3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>27.7</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>9.98</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>21.73</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="28"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="18"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="27"/>
+      <c r="B10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="17"/>
       <c r="D10" s="1">
         <v>60.6</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>56.38</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>3.75</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>45.51</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>7</v>
       </c>
-      <c r="I10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="28"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="27"/>
+      <c r="B11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="17"/>
       <c r="D11" s="1">
         <v>25.1</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>4.26</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>85.93</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>25.61</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>3.5</v>
       </c>
-      <c r="I11" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="28"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="18"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="28"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="18"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1">
         <v>82.275999999999996</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="28"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="18"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1">
         <v>144.43</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="28"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="18"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1">
         <v>74</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="28"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="18"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
       <c r="J16" s="1">
         <v>97.024000000000001</v>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="28"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="18"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="28"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="18"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
       <c r="J18" s="1">
         <v>37.700000000000003</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="28"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="18"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="28"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="18"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="22">
+        <v>14.5</v>
+      </c>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20">
+        <v>14.5</v>
+      </c>
+      <c r="M20" s="19"/>
+      <c r="N20" s="18"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="22">
+        <v>11</v>
+      </c>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20">
+        <v>11</v>
+      </c>
+      <c r="M21" s="19"/>
+      <c r="N21" s="18"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="22">
+        <v>15.6</v>
+      </c>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20">
+        <v>15.6</v>
+      </c>
+      <c r="M22" s="19"/>
+      <c r="N22" s="18"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="22">
+        <v>13.7</v>
+      </c>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20">
+        <v>13.7</v>
+      </c>
+      <c r="M23" s="19"/>
+      <c r="N23" s="18"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="22">
+        <v>5.54</v>
+      </c>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20">
+        <v>5.54</v>
+      </c>
+      <c r="M24" s="19"/>
+      <c r="N24" s="18"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="22">
+        <v>34</v>
+      </c>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20">
+        <v>34</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="18"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="22">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="M26" s="19"/>
+      <c r="N26" s="18"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="J20" s="34">
-        <v>14.5</v>
-      </c>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32">
-        <v>14.5</v>
-      </c>
-      <c r="M20" s="29"/>
-      <c r="N20" s="28"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="D27" s="5"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="22">
+        <v>12</v>
+      </c>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20">
+        <v>12</v>
+      </c>
+      <c r="M27" s="19"/>
+      <c r="N27" s="18"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="J21" s="34">
-        <v>11</v>
-      </c>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32">
-        <v>11</v>
-      </c>
-      <c r="M21" s="29"/>
-      <c r="N21" s="28"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="D28" s="5"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="22">
+        <v>24.3</v>
+      </c>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20">
+        <v>24.3</v>
+      </c>
+      <c r="M28" s="19"/>
+      <c r="N28" s="18"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="J22" s="34">
-        <v>15.6</v>
-      </c>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32">
-        <v>15.6</v>
-      </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="28"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="D29" s="5"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="22">
+        <v>1.6739999999999999</v>
+      </c>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20">
+        <v>1.6739999999999999</v>
+      </c>
+      <c r="M29" s="19"/>
+      <c r="N29" s="18"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="J23" s="34">
-        <v>13.7</v>
-      </c>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32">
-        <v>13.7</v>
-      </c>
-      <c r="M23" s="29"/>
-      <c r="N23" s="28"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+      <c r="D30" s="5"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="22">
+        <v>11.9</v>
+      </c>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20">
+        <v>11.9</v>
+      </c>
+      <c r="M30" s="19"/>
+      <c r="N30" s="18"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="J24" s="34">
-        <v>5.54</v>
-      </c>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32">
-        <v>5.54</v>
-      </c>
-      <c r="M24" s="29"/>
-      <c r="N24" s="28"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="J25" s="34">
-        <v>34</v>
-      </c>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32">
-        <v>34</v>
-      </c>
-      <c r="M25" s="29"/>
-      <c r="N25" s="28"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="J26" s="34">
-        <v>8.7599999999999997E-2</v>
-      </c>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32">
-        <v>8.7599999999999997E-2</v>
-      </c>
-      <c r="M26" s="29"/>
-      <c r="N26" s="28"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="J27" s="34">
-        <v>12</v>
-      </c>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32">
-        <v>12</v>
-      </c>
-      <c r="M27" s="29"/>
-      <c r="N27" s="28"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="J28" s="34">
-        <v>24.3</v>
-      </c>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32">
-        <v>24.3</v>
-      </c>
-      <c r="M28" s="29"/>
-      <c r="N28" s="28"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="J29" s="34">
-        <v>1.6739999999999999</v>
-      </c>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32">
-        <v>1.6739999999999999</v>
-      </c>
-      <c r="M29" s="29"/>
-      <c r="N29" s="28"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="J30" s="34">
-        <v>11.9</v>
-      </c>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32">
-        <v>11.9</v>
-      </c>
-      <c r="M30" s="29"/>
-      <c r="N30" s="28"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
       <c r="J31" s="1">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="28"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="18"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="28"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="18"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="28"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="18"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="J34" s="36">
+        <v>78</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="23">
         <v>160</v>
       </c>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="28"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="18"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D35" s="7"/>
-      <c r="J35" s="36">
+      <c r="B35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="23">
         <v>324</v>
       </c>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="28"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="18"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="7"/>
-      <c r="J36" s="36">
+      <c r="B36" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="23">
         <v>284</v>
       </c>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="28"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="18"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="7"/>
-      <c r="J37" s="36">
+      <c r="B37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="23">
         <v>210</v>
       </c>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="28"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="18"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="J38" s="36">
+      <c r="B38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="23">
         <v>156</v>
       </c>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="28"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="18"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
       <c r="J39" s="1">
         <v>264.5</v>
       </c>
-      <c r="K39" s="29">
+      <c r="K39" s="19">
         <v>250</v>
       </c>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="28"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="18"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="28"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="18"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="7"/>
-      <c r="J41" s="36">
+        <v>89</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="23">
         <v>16.2</v>
       </c>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="28"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="18"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="7"/>
-      <c r="J42" s="36">
+      <c r="B42" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="23">
         <v>13.4</v>
       </c>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="28"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="18"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D43" s="7"/>
-      <c r="J43" s="36">
+      <c r="B43" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="23">
         <v>6.7</v>
       </c>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="28"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="18"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D44" s="7"/>
-      <c r="J44" s="36">
+      <c r="B44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="23">
         <v>5</v>
       </c>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="28"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="18"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D45" s="7"/>
-      <c r="J45" s="36">
+      <c r="B45" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="23">
         <v>9.1999999999999993</v>
       </c>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="28"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="18"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46" s="7"/>
-      <c r="J46" s="36">
+      <c r="B46" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="23">
         <v>1.849</v>
       </c>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="28"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="18"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
-      <c r="N47" s="28"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="18"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
-      <c r="N48" s="28"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="18"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C49" t="s">
-        <v>118</v>
-      </c>
-      <c r="D49" s="3">
+        <v>104</v>
+      </c>
+      <c r="D49" s="1">
         <v>1.0410000000000001E-2</v>
       </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="30">
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19">
         <f>0.007</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="M49" s="30"/>
-      <c r="N49" s="28"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="18"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="28"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="18"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C51" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D51" s="1"/>
-      <c r="G51" s="33">
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="21">
         <v>5.54</v>
       </c>
-      <c r="J51" s="1"/>
-      <c r="K51" s="29">
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1">
         <v>5.54</v>
       </c>
-      <c r="L51" s="29"/>
-      <c r="M51" s="29"/>
-      <c r="N51" s="28"/>
+      <c r="K51" s="19">
+        <v>5.54</v>
+      </c>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="18"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="29"/>
-      <c r="N52" s="28"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="18"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="J53" s="24">
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1">
         <f>2.328/1000</f>
         <v>2.3279999999999998E-3</v>
       </c>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
-      <c r="N53" s="28"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="18"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>126</v>
-      </c>
-      <c r="J54">
+        <v>112</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1">
         <f>28.1/1000</f>
         <v>2.81E-2</v>
       </c>
-      <c r="K54" s="28"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="28"/>
-      <c r="N54" s="28"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="18"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
-      <c r="N55" s="28"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="18"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="29"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="29"/>
-      <c r="N56" s="28"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="18"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="29"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="29"/>
-      <c r="N57" s="28"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="18"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="29"/>
-      <c r="N58" s="28"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="19"/>
+      <c r="N58" s="18"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="29"/>
-      <c r="N59" s="28"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="18"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="29"/>
-      <c r="N60" s="28"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="19"/>
+      <c r="N60" s="18"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="29"/>
-      <c r="L61" s="29"/>
-      <c r="M61" s="29"/>
-      <c r="N61" s="28"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="18"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="29"/>
-      <c r="L62" s="29"/>
-      <c r="M62" s="29"/>
-      <c r="N62" s="28"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="19"/>
+      <c r="M62" s="19"/>
+      <c r="N62" s="18"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
@@ -4358,11 +4533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4377,960 +4552,1194 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="3">
+        <v>114</v>
+      </c>
+      <c r="D2" s="1">
         <f>(D8*J4+D9*J5+D10*J6+D11*J7)/108.4</f>
         <v>8.6709852398523982E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <f>(E8*J4+E9*J5+E10*J6+E11*J7)/100</f>
         <v>9.2255004000000002E-2</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <f>(F8*J4+F9*J5+F10*J6+F11*J7)/100</f>
         <v>1.3614858000000001E-2</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <f>(G8*J4+G9*J5+G10*J6+G11*J7)/100</f>
         <v>7.4350278000000006E-2</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="1">
         <f>(J4*H8+J5*H9+H10*J6+H11*J7)/SUM(H8:H11)</f>
         <v>8.3014054054054057E-2</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="1">
         <v>3.1427999999999998E-2</v>
       </c>
       <c r="J2" s="1">
         <f>AVERAGE(D2:I2)</f>
         <v>6.3562007742096346E-2</v>
       </c>
-      <c r="K2" s="30">
+      <c r="K2" s="19">
         <v>2E-3</v>
       </c>
-      <c r="L2" s="29">
+      <c r="L2" s="19">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="M2" s="29"/>
+      <c r="M2" s="19"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D3" s="1">
         <v>0.53639999999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.61919999999999997</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>1.1879999999999999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>0.47520000000000001</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>0.71640000000000004</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>3.1427999999999998E-2</v>
       </c>
       <c r="J3" s="1">
         <f>AVERAGE(D3:I3)</f>
         <v>0.59443800000000002</v>
       </c>
-      <c r="K3" s="29">
+      <c r="K3" s="19">
         <v>0.57150000000000001</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="19">
         <v>0.58150000000000002</v>
       </c>
-      <c r="M3" s="29">
+      <c r="M3" s="19">
         <v>0.47</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>130</v>
+        <v>30</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1">
         <v>7.3440000000000005E-2</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>131</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>117</v>
       </c>
       <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>132</v>
+        <v>34</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>118</v>
       </c>
       <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1">
         <f>(0.1332+0.14652)/2</f>
         <v>0.13986000000000001</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="28"/>
+        <v>36</v>
+      </c>
+      <c r="C7" s="18"/>
       <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1">
         <v>7.5599999999999999E-3</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="28"/>
+        <v>37</v>
+      </c>
+      <c r="C8" s="18"/>
       <c r="D8" s="1">
         <v>6.4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>11.7</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="24">
         <v>0.35</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>7.14</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>7</v>
       </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="28"/>
+        <v>38</v>
+      </c>
+      <c r="C9" s="18"/>
       <c r="D9" s="1">
         <v>16.3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>27.7</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>9.98</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>21.73</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
-        <v>51</v>
-      </c>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="28"/>
+        <v>39</v>
+      </c>
+      <c r="C10" s="18"/>
       <c r="D10" s="1">
         <v>60.6</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>56.38</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>3.75</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>45.51</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>7</v>
       </c>
-      <c r="I10" t="s">
-        <v>51</v>
-      </c>
+      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="28"/>
+        <v>40</v>
+      </c>
+      <c r="C11" s="18"/>
       <c r="D11" s="1">
         <v>25.1</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>4.26</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>85.93</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>25.61</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>3.5</v>
       </c>
-      <c r="I11" t="s">
-        <v>51</v>
-      </c>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1">
         <v>3.2530000000000001</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1">
         <v>8.1639999999999997</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1">
         <v>3</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
       <c r="J16" s="1">
         <v>3.8340000000000001</v>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
       <c r="J18" s="1">
         <v>2.37</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="J20" s="33">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="21">
         <v>2.29</v>
       </c>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29">
+      <c r="K20" s="19"/>
+      <c r="L20" s="19">
         <v>2.29</v>
       </c>
-      <c r="M20" s="29"/>
+      <c r="M20" s="19"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="J21" s="33">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="21">
         <v>1.74</v>
       </c>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29">
+      <c r="K21" s="19"/>
+      <c r="L21" s="19">
         <v>1.74</v>
       </c>
-      <c r="M21" s="29"/>
+      <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="J22" s="33">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="21">
         <v>0.61199999999999999</v>
       </c>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29">
+      <c r="K22" s="19"/>
+      <c r="L22" s="19">
         <v>0.61199999999999999</v>
       </c>
-      <c r="M22" s="29"/>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="J23" s="33">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="21">
         <v>0.55300000000000005</v>
       </c>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29">
+      <c r="K23" s="19"/>
+      <c r="L23" s="19">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M23" s="29"/>
+      <c r="M23" s="19"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="J24" s="33">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="21">
         <v>0.223</v>
       </c>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29">
+      <c r="K24" s="19"/>
+      <c r="L24" s="19">
         <v>0.223</v>
       </c>
-      <c r="M24" s="29"/>
+      <c r="M24" s="19"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="J25" s="33">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="21">
         <v>1.75</v>
       </c>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29">
+      <c r="K25" s="19"/>
+      <c r="L25" s="19">
         <v>1.75</v>
       </c>
-      <c r="M25" s="29"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="D26" s="1"/>
-      <c r="J26" s="33">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="21">
         <v>8.3099999999999997E-3</v>
       </c>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29">
+      <c r="K26" s="19"/>
+      <c r="L26" s="19">
         <v>8.3099999999999997E-3</v>
       </c>
-      <c r="M26" s="29"/>
+      <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="J27" s="33">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="21">
         <v>0.95</v>
       </c>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29">
+      <c r="K27" s="19"/>
+      <c r="L27" s="19">
         <v>0.95</v>
       </c>
-      <c r="M27" s="29"/>
+      <c r="M27" s="19"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="J28" s="33">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="21">
         <v>0.56200000000000006</v>
       </c>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29">
+      <c r="K28" s="19"/>
+      <c r="L28" s="19">
         <v>0.56200000000000006</v>
       </c>
-      <c r="M28" s="29"/>
+      <c r="M28" s="19"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="J29" s="33">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="21">
         <v>1.9E-2</v>
       </c>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29">
+      <c r="K29" s="19"/>
+      <c r="L29" s="19">
         <v>1.9E-2</v>
       </c>
-      <c r="M29" s="29"/>
+      <c r="M29" s="19"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="J30" s="33">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="21">
         <v>0.91700000000000004</v>
       </c>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29">
+      <c r="K30" s="19"/>
+      <c r="L30" s="19">
         <v>0.91700000000000004</v>
       </c>
-      <c r="M30" s="29"/>
+      <c r="M30" s="19"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="J32" s="33">
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="21">
         <f>AVERAGE(J20:J30)</f>
         <v>0.87493727272727273</v>
       </c>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29">
+      <c r="K32" s="19"/>
+      <c r="L32" s="19">
         <f>AVERAGE(L20:L30)</f>
         <v>0.87493727272727273</v>
       </c>
-      <c r="M32" s="29"/>
+      <c r="M32" s="19"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="J35" s="1">
         <v>12.4</v>
       </c>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
       <c r="J36" s="1">
         <v>26.7</v>
       </c>
-      <c r="K36" s="29">
+      <c r="K36" s="19">
         <v>9.2200000000000006</v>
       </c>
-      <c r="L36" s="29">
+      <c r="L36" s="19">
         <v>9.7899999999999991</v>
       </c>
-      <c r="M36" s="29"/>
+      <c r="M36" s="19"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
       <c r="J37" s="1">
         <v>22.6</v>
       </c>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
       <c r="J38" s="1">
         <v>16.7</v>
       </c>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
       <c r="J39" s="1">
         <v>12.7</v>
       </c>
-      <c r="K39" s="29"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="29"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D40" s="1"/>
-      <c r="J40">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1">
         <v>25.5</v>
       </c>
-      <c r="K40" s="29"/>
-      <c r="L40" s="28">
+      <c r="K40" s="19"/>
+      <c r="L40" s="19">
         <v>10.97</v>
       </c>
-      <c r="M40" s="28">
+      <c r="M40" s="19">
         <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
       <c r="J42" s="1">
         <v>1.08</v>
       </c>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
       <c r="J43" s="1">
         <v>1.32</v>
       </c>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C44" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
       <c r="J44" s="1">
         <v>0.33400000000000002</v>
       </c>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
       <c r="J45" s="1">
         <v>-0.62</v>
       </c>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="29"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C46" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
       <c r="J46" s="1">
         <v>2.2700000000000001E-2</v>
       </c>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
       <c r="J47" s="1">
         <v>0.1719</v>
       </c>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="29"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>169</v>
-      </c>
-      <c r="D50" s="5">
+        <v>155</v>
+      </c>
+      <c r="D50" s="1">
         <v>6.2500000000000001E-4</v>
       </c>
-      <c r="J50" s="37">
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="21">
         <f>0.0004</f>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K50" s="29"/>
-      <c r="L50" s="31">
+      <c r="K50" s="19"/>
+      <c r="L50" s="19">
         <f>0.0004</f>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="M50" s="31"/>
+      <c r="M50" s="19"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D51" s="4"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="29"/>
-      <c r="L51" s="31"/>
-      <c r="M51" s="31"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B52" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
       <c r="J52" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="29"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="J54" s="24">
+        <v>159</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1">
         <f>0.16386667/1000</f>
         <v>1.6386666999999999E-4</v>
       </c>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D55" s="1"/>
-      <c r="J55">
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1">
         <f>1.89/1000</f>
         <v>1.89E-3</v>
       </c>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="29"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="29"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="29"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="29"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="29"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="19"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="29"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
@@ -5347,7 +5756,7 @@
       <c r="M61" s="1"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D62" s="21"/>
+      <c r="D62" s="12"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -5403,16 +5812,16 @@
       <c r="M69" s="1"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="23"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="14"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D71" s="21"/>
+      <c r="D71" s="12"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>

</xml_diff>

<commit_message>
JW: Transport is updated
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\school\WUR\Master\Programming in python\untitled\ACT\ACT2321\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B657B94E-C55F-44F3-8D3C-59A124C76CC3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
     <sheet name="Energy (MJ)" sheetId="2" r:id="rId2"/>
     <sheet name="CO2eq (kg)" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={ED13EA6E-84B9-4566-9DD1-5F68795B2A3F}</author>
     <author>tc={AA2B32B5-7D1D-400A-A931-EBFBF82EF357}</author>
@@ -69,7 +70,7 @@
     <author>tc={3CBB2313-6869-4ADB-8678-F0A56C53B204}</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="1" shapeId="0">
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="2" shapeId="0">
+    <comment ref="C2" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="3" shapeId="0">
+    <comment ref="D2" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -141,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="4" shapeId="0">
+    <comment ref="E2" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -159,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="5" shapeId="0">
+    <comment ref="F2" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="6" shapeId="0">
+    <comment ref="B3" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="7" shapeId="0">
+    <comment ref="F3" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -213,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="8" shapeId="0">
+    <comment ref="B4" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -231,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="9" shapeId="0">
+    <comment ref="B5" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -249,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="10" shapeId="0">
+    <comment ref="C5" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -267,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="11" shapeId="0">
+    <comment ref="D5" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -285,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="12" shapeId="0">
+    <comment ref="F5" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -303,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="13" shapeId="0">
+    <comment ref="B6" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -321,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="14" shapeId="0">
+    <comment ref="B7" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -339,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="15" shapeId="0">
+    <comment ref="F7" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -357,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="16" shapeId="0">
+    <comment ref="B8" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -375,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="17" shapeId="0">
+    <comment ref="C8" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -393,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="18" shapeId="0">
+    <comment ref="F8" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -411,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="19" shapeId="0">
+    <comment ref="B9" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -429,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="20" shapeId="0">
+    <comment ref="C9" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -447,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="21" shapeId="0">
+    <comment ref="D9" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -465,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="22" shapeId="0">
+    <comment ref="F9" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -483,7 +484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="23" shapeId="0">
+    <comment ref="A10" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -505,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="24" shapeId="0">
+    <comment ref="B10" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -528,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="25" shapeId="0">
+    <comment ref="C10" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -546,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="26" shapeId="0">
+    <comment ref="D10" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -565,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="27" shapeId="0">
+    <comment ref="E10" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -583,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="28" shapeId="0">
+    <comment ref="F10" authorId="28" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -603,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="29" shapeId="0">
+    <comment ref="B11" authorId="29" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -621,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="30" shapeId="0">
+    <comment ref="C11" authorId="30" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -639,7 +640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="31" shapeId="0">
+    <comment ref="D11" authorId="31" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -657,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="32" shapeId="0">
+    <comment ref="F11" authorId="32" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -680,7 +681,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={28C0A1D0-E24D-4A94-B8D7-08380DAD163B}</author>
     <author>tc={F1D6A124-94E9-4537-87FD-64C5756431CC}</author>
@@ -701,7 +702,7 @@
     <author>tc={EB5AF55A-D36E-4291-B324-6215D9703071}</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -719,7 +720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="1" shapeId="0">
+    <comment ref="E3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -737,7 +738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="2" shapeId="0">
+    <comment ref="F3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -755,7 +756,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="3" shapeId="0">
+    <comment ref="G3" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -773,7 +774,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="4" shapeId="0">
+    <comment ref="H3" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -791,7 +792,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0">
+    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -809,7 +810,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="6" shapeId="0">
+    <comment ref="E8" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -827,7 +828,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="7" shapeId="0">
+    <comment ref="F8" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -845,7 +846,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="8" shapeId="0">
+    <comment ref="G8" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -863,7 +864,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="9" shapeId="0">
+    <comment ref="H8" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -881,7 +882,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="10" shapeId="0">
+    <comment ref="J13" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -899,7 +900,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="11" shapeId="0">
+    <comment ref="J18" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -917,7 +918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J39" authorId="12" shapeId="0">
+    <comment ref="J39" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -935,7 +936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="13" shapeId="0">
+    <comment ref="K39" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -953,7 +954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J41" authorId="14" shapeId="0">
+    <comment ref="J41" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -971,7 +972,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="15" shapeId="0">
+    <comment ref="J43" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
       <text>
         <r>
           <rPr>
@@ -989,7 +990,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J45" authorId="16" shapeId="0">
+    <comment ref="J45" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1012,7 +1013,7 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={53C940E0-2140-41F9-A6DF-6EA835ABEC64}</author>
     <author>tc={F8E5DC3C-6251-4EB4-8D84-9AAD62A6919A}</author>
@@ -1044,7 +1045,7 @@
     <author>tc={25BEEA18-2FB0-45C9-B9D8-E5E62F8643F3}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1062,7 +1063,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="1" shapeId="0">
+    <comment ref="K2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1081,7 +1082,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="2" shapeId="0">
+    <comment ref="L2" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1099,7 +1100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="3" shapeId="0">
+    <comment ref="D3" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1117,7 +1118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="4" shapeId="0">
+    <comment ref="M3" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1135,7 +1136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="5" shapeId="0">
+    <comment ref="J4" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1153,7 +1154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="6" shapeId="0">
+    <comment ref="D8" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1171,7 +1172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="7" shapeId="0">
+    <comment ref="E8" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1189,7 +1190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="8" shapeId="0">
+    <comment ref="F8" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1207,7 +1208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="9" shapeId="0">
+    <comment ref="G8" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -1225,7 +1226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="10" shapeId="0">
+    <comment ref="H8" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1243,7 +1244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="11" shapeId="0">
+    <comment ref="J13" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -1261,7 +1262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="12" shapeId="0">
+    <comment ref="J15" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1279,7 +1280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="13" shapeId="0">
+    <comment ref="J18" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -1297,7 +1298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="14" shapeId="0">
+    <comment ref="J20" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -1317,7 +1318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L20" authorId="15" shapeId="0">
+    <comment ref="L20" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
       <text>
         <r>
           <rPr>
@@ -1337,7 +1338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J30" authorId="16" shapeId="0">
+    <comment ref="J30" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1355,7 +1356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L30" authorId="17" shapeId="0">
+    <comment ref="L30" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
       <text>
         <r>
           <rPr>
@@ -1373,7 +1374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K36" authorId="18" shapeId="0">
+    <comment ref="K36" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
       <text>
         <r>
           <rPr>
@@ -1391,7 +1392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L36" authorId="19" shapeId="0">
+    <comment ref="L36" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
       <text>
         <r>
           <rPr>
@@ -1409,7 +1410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J40" authorId="20" shapeId="0">
+    <comment ref="J40" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
       <text>
         <r>
           <rPr>
@@ -1427,7 +1428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L40" authorId="21" shapeId="0">
+    <comment ref="L40" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
       <text>
         <r>
           <rPr>
@@ -1445,7 +1446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M40" authorId="22" shapeId="0">
+    <comment ref="M40" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
       <text>
         <r>
           <rPr>
@@ -1463,7 +1464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J42" authorId="23" shapeId="0">
+    <comment ref="J42" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
       <text>
         <r>
           <rPr>
@@ -1481,7 +1482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J44" authorId="24" shapeId="0">
+    <comment ref="J44" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
       <text>
         <r>
           <rPr>
@@ -1499,7 +1500,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J46" authorId="25" shapeId="0">
+    <comment ref="J46" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -1517,7 +1518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="26" shapeId="0">
+    <comment ref="D50" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -1535,7 +1536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J50" authorId="27" shapeId="0">
+    <comment ref="J50" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -1558,7 +1559,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="163">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -2044,12 +2045,15 @@
   </si>
   <si>
     <t>United States</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -2964,7 +2968,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3210,11 +3214,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3655,7 +3659,9 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1">
         <v>37.700000000000003</v>
@@ -4533,11 +4539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
JW: excel changes of loes implemented in verticalcode
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B657B94E-C55F-44F3-8D3C-59A124C76CC3}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{57ADA31D-221E-46B7-AB07-F826644A3729}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
@@ -2971,17 +2971,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" activeCellId="1" sqref="B2:F11 C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
@@ -4542,7 +4542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
JW: made a start with the seedlings
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{57ADA31D-221E-46B7-AB07-F826644A3729}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{21721E37-C420-4414-B0B7-1A237ED142F4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
@@ -1559,7 +1559,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="165">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -2048,6 +2048,12 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>Se1</t>
+  </si>
+  <si>
+    <t>Se2</t>
   </si>
 </sst>
 </file>
@@ -2971,7 +2977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3217,8 +3223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView topLeftCell="B36" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3655,6 +3661,9 @@
       <c r="B18" t="s">
         <v>51</v>
       </c>
+      <c r="C18" t="s">
+        <v>164</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -4542,8 +4551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4972,6 +4981,9 @@
       <c r="B18" t="s">
         <v>51</v>
       </c>
+      <c r="C18" t="s">
+        <v>163</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>

</xml_diff>

<commit_message>
JW: seedlings are implemented and working
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{21721E37-C420-4414-B0B7-1A237ED142F4}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{8726C29A-CF30-40DC-BA00-6589F3D6DC91}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
@@ -694,7 +694,6 @@
     <author>tc={7A8B2478-7119-468E-A944-CF0C5DF05106}</author>
     <author>tc={C33DE9C9-6AE7-482D-8277-5DB16883D9AF}</author>
     <author>tc={4894AC73-6F3C-482C-BF3B-EF91AD8418D6}</author>
-    <author>tc={BFF5F8B5-9FA9-47FB-B65E-682B51E753EF}</author>
     <author>tc={91C7F82C-9A9F-4C87-A739-6A581FAAD543}</author>
     <author>tc={27297E8D-321A-49D8-9262-B18D44E94748}</author>
     <author>tc={48EF0565-F5AA-4859-B328-8E1C327C14E9}</author>
@@ -900,25 +899,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Ecoinvent V3
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J39" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="J37" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -936,7 +917,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
+    <comment ref="K37" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -954,7 +935,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J41" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
+    <comment ref="J39" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -972,7 +953,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
+    <comment ref="J41" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
       <text>
         <r>
           <rPr>
@@ -990,7 +971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J45" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
+    <comment ref="J43" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1028,7 +1009,6 @@
     <author>tc={7E07B26E-CA23-48A3-A12B-6DA9B1E99E35}</author>
     <author>tc={67393C48-310C-4E8B-87A7-6A02EA78F1F7}</author>
     <author>tc={663D8CF0-4CFD-4F94-B3AD-E16830C73AAE}</author>
-    <author>tc={0BD08DC0-6AE2-48F8-BBCF-BAB58B87B9B4}</author>
     <author>tc={0877BE86-6D42-484E-9886-B6C2FA23BBDF}</author>
     <author>tc={A7925944-D01F-4C9C-B69E-643D7D71DBB7}</author>
     <author>tc={E6BE51FA-33D4-4246-B71B-6E9B6D8B8C8E}</author>
@@ -1280,25 +1260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Ecoinvent v3
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J20" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
+    <comment ref="J18" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -1318,7 +1280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L20" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
+    <comment ref="L18" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
       <text>
         <r>
           <rPr>
@@ -1338,7 +1300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J30" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
+    <comment ref="J28" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1356,7 +1318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L30" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
+    <comment ref="L28" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
       <text>
         <r>
           <rPr>
@@ -1374,7 +1336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K36" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
+    <comment ref="K34" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
       <text>
         <r>
           <rPr>
@@ -1392,7 +1354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L36" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
+    <comment ref="L34" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
       <text>
         <r>
           <rPr>
@@ -1410,7 +1372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J40" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
+    <comment ref="J38" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
       <text>
         <r>
           <rPr>
@@ -1428,7 +1390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L40" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
+    <comment ref="L38" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
       <text>
         <r>
           <rPr>
@@ -1446,7 +1408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M40" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
+    <comment ref="M38" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
       <text>
         <r>
           <rPr>
@@ -1464,7 +1426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J42" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
+    <comment ref="J40" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
       <text>
         <r>
           <rPr>
@@ -1482,7 +1444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J44" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
+    <comment ref="J42" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
       <text>
         <r>
           <rPr>
@@ -1500,7 +1462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J46" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
+    <comment ref="J44" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -1518,7 +1480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D50" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
+    <comment ref="D48" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1498,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J50" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
+    <comment ref="J48" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -1559,7 +1521,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="162">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -1714,9 +1676,6 @@
     <t>Planting material (MJ/kg)</t>
   </si>
   <si>
-    <t>seeds</t>
-  </si>
-  <si>
     <t>Fertilizer (MJ/l)</t>
   </si>
   <si>
@@ -1936,9 +1895,6 @@
     <t>Fo9</t>
   </si>
   <si>
-    <t>Planting material (kgCO2/kg)</t>
-  </si>
-  <si>
     <t>Fertilizer (kgCO2/kg)</t>
   </si>
   <si>
@@ -2047,13 +2003,10 @@
     <t>United States</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>Se1</t>
-  </si>
-  <si>
-    <t>Se2</t>
+    <t>seeds (kgCO2/kg)</t>
+  </si>
+  <si>
+    <t>seeds (MJ/kg)</t>
   </si>
 </sst>
 </file>
@@ -2108,7 +2061,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -2162,40 +2115,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
@@ -2237,9 +2160,123 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -2247,7 +2284,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2255,7 +2292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2269,11 +2306,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2295,13 +2329,34 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2975,10 +3030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2990,9 +3045,10 @@
     <col min="5" max="5" width="21.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -3006,212 +3062,278 @@
       <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="G1" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="24">
         <v>0.58630000000000004</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="24">
         <v>0.8</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="24">
         <v>1.11E-6</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="24">
         <v>620</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="30">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="G2" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H2" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>0.55049999999999999</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="24">
         <v>0.7</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <v>1.11E-6</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="24">
         <v>710</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="30">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="G3" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H3" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>0.2268</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>0.6</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>1.3329999999999999E-5</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="24">
         <v>1080</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="30">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="G4" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H4" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>2.3279999999999999E-4</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>970</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="30">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="G5" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H5" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>4.5799999999999999E-3</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>0.6</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>1.8199999999999999E-6</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>1250</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="30">
         <v>77.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="G6" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H6" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <v>4.0125000000000001E-2</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>0.75</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>3.6399999999999999E-6</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>1930</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="30">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="G7" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H7" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>9.6600000000000005E-2</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <v>0.85</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>1.5999999999999999E-6</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>2000</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="30">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="G8" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H8" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>6.2599999999999999E-3</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>0.75</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <v>3.3000000000000002E-7</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <v>980</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="30">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="G9" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H9" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <v>0.35449999999999998</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>0.67</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>8.5000000000000001E-7</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>790</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="30">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="G10" s="32">
+        <v>2.37</v>
+      </c>
+      <c r="H10" s="28">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="25">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="25">
         <v>0.5</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="25">
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="25">
         <v>16760</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="33">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="29"/>
+      <c r="G11" s="34">
+        <v>2.37</v>
+      </c>
+      <c r="H11" s="35">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3221,10 +3343,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3252,7 +3374,7 @@
         <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -3263,16 +3385,16 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="18"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3311,10 +3433,10 @@
         <f>AVERAGE(D2:I2)</f>
         <v>0.26047889689199161</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3345,16 +3467,16 @@
         <f>AVERAGE(D3:I3)</f>
         <v>6.9581999999999988</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="5"/>
@@ -3366,16 +3488,16 @@
       <c r="J4" s="5">
         <v>1.008</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="18"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="5"/>
@@ -3387,16 +3509,16 @@
       <c r="J5" s="5">
         <v>0.18720000000000001</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="18"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="5"/>
@@ -3409,16 +3531,16 @@
         <f>(0.1332+0.17064)/2</f>
         <v>0.15192</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="18"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="5"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -3428,23 +3550,23 @@
       <c r="J7" s="5">
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="17"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="1">
         <v>6.4</v>
       </c>
       <c r="E8" s="1">
         <v>11.7</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>0.35</v>
       </c>
       <c r="G8" s="1">
@@ -3455,16 +3577,16 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="18"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="17"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="1">
         <v>16.3</v>
       </c>
@@ -3482,16 +3604,16 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="18"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="17"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="1">
         <v>60.6</v>
       </c>
@@ -3509,16 +3631,16 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="18"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="17"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="1">
         <v>25.1</v>
       </c>
@@ -3536,10 +3658,10 @@
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="18"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
@@ -3549,10 +3671,10 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3573,10 +3695,10 @@
       <c r="J13" s="1">
         <v>82.275999999999996</v>
       </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="17"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -3594,10 +3716,10 @@
       <c r="J14" s="1">
         <v>144.43</v>
       </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="17"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -3615,10 +3737,10 @@
       <c r="J15" s="1">
         <v>74</v>
       </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="17"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -3636,10 +3758,10 @@
       <c r="J16" s="1">
         <v>97.024000000000001</v>
       </c>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="17"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
@@ -3649,59 +3771,69 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="17"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D18" s="1"/>
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>162</v>
-      </c>
+      <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1">
-        <v>37.700000000000003</v>
+      <c r="J18" s="21">
+        <v>14.5</v>
       </c>
       <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="18"/>
+      <c r="L18" s="19">
+        <v>14.5</v>
+      </c>
+      <c r="M18" s="18"/>
+      <c r="N18" s="17"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
+      <c r="B19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="J19" s="21">
+        <v>11</v>
+      </c>
       <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="18"/>
+      <c r="L19" s="19">
+        <v>11</v>
+      </c>
+      <c r="M19" s="18"/>
+      <c r="N19" s="17"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="1"/>
@@ -3709,22 +3841,22 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="22">
-        <v>14.5</v>
-      </c>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20">
-        <v>14.5</v>
-      </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="18"/>
+      <c r="J20" s="21">
+        <v>15.6</v>
+      </c>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19">
+        <v>15.6</v>
+      </c>
+      <c r="M20" s="18"/>
+      <c r="N20" s="17"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="1"/>
@@ -3732,22 +3864,22 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="22">
-        <v>11</v>
-      </c>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20">
-        <v>11</v>
-      </c>
-      <c r="M21" s="19"/>
-      <c r="N21" s="18"/>
+      <c r="J21" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19">
+        <v>13.7</v>
+      </c>
+      <c r="M21" s="18"/>
+      <c r="N21" s="17"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="1"/>
@@ -3755,22 +3887,22 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="22">
-        <v>15.6</v>
-      </c>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20">
-        <v>15.6</v>
-      </c>
-      <c r="M22" s="19"/>
-      <c r="N22" s="18"/>
+      <c r="J22" s="21">
+        <v>5.54</v>
+      </c>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19">
+        <v>5.54</v>
+      </c>
+      <c r="M22" s="18"/>
+      <c r="N22" s="17"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
@@ -3778,22 +3910,22 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="22">
-        <v>13.7</v>
-      </c>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20">
-        <v>13.7</v>
-      </c>
-      <c r="M23" s="19"/>
-      <c r="N23" s="18"/>
+      <c r="J23" s="21">
+        <v>34</v>
+      </c>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19">
+        <v>34</v>
+      </c>
+      <c r="M23" s="18"/>
+      <c r="N23" s="17"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="1"/>
@@ -3801,22 +3933,22 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="22">
-        <v>5.54</v>
-      </c>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20">
-        <v>5.54</v>
-      </c>
-      <c r="M24" s="19"/>
-      <c r="N24" s="18"/>
+      <c r="J24" s="21">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="M24" s="18"/>
+      <c r="N24" s="17"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="1"/>
@@ -3824,22 +3956,22 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="22">
-        <v>34</v>
-      </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20">
-        <v>34</v>
-      </c>
-      <c r="M25" s="19"/>
-      <c r="N25" s="18"/>
+      <c r="J25" s="21">
+        <v>12</v>
+      </c>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19">
+        <v>12</v>
+      </c>
+      <c r="M25" s="18"/>
+      <c r="N25" s="17"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="1"/>
@@ -3847,22 +3979,22 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="22">
-        <v>8.7599999999999997E-2</v>
-      </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20">
-        <v>8.7599999999999997E-2</v>
-      </c>
-      <c r="M26" s="19"/>
-      <c r="N26" s="18"/>
+      <c r="J26" s="21">
+        <v>24.3</v>
+      </c>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19">
+        <v>24.3</v>
+      </c>
+      <c r="M26" s="18"/>
+      <c r="N26" s="17"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
@@ -3870,22 +4002,22 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="22">
-        <v>12</v>
-      </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20">
-        <v>12</v>
-      </c>
-      <c r="M27" s="19"/>
-      <c r="N27" s="18"/>
+      <c r="J27" s="21">
+        <v>1.6739999999999999</v>
+      </c>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19">
+        <v>1.6739999999999999</v>
+      </c>
+      <c r="M27" s="18"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="1"/>
@@ -3893,22 +4025,22 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="22">
-        <v>24.3</v>
-      </c>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20">
-        <v>24.3</v>
-      </c>
-      <c r="M28" s="19"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="21">
+        <v>11.9</v>
+      </c>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19">
+        <v>11.9</v>
+      </c>
+      <c r="M28" s="18"/>
+      <c r="N28" s="17"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="1"/>
@@ -3916,98 +4048,94 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="22">
-        <v>1.6739999999999999</v>
-      </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20">
-        <v>1.6739999999999999</v>
-      </c>
-      <c r="M29" s="19"/>
-      <c r="N29" s="18"/>
+      <c r="J29" s="1">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="5"/>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="22">
-        <v>11.9</v>
-      </c>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20">
-        <v>11.9</v>
-      </c>
-      <c r="M30" s="19"/>
-      <c r="N30" s="18"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="17"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1">
-        <v>8.7599999999999997E-2</v>
-      </c>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="18"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="17"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="1"/>
+      <c r="B32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="5"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="J32" s="22">
+        <v>160</v>
+      </c>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
-      <c r="N32" s="18"/>
+      <c r="N32" s="17"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D33" s="1"/>
+      <c r="B33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="5"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="22">
+        <v>324</v>
+      </c>
       <c r="K33" s="19"/>
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
-      <c r="N33" s="18"/>
+      <c r="N33" s="17"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="1"/>
@@ -4015,20 +4143,20 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="23">
-        <v>160</v>
-      </c>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="18"/>
+      <c r="J34" s="22">
+        <v>284</v>
+      </c>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="17"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="1"/>
@@ -4036,20 +4164,20 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="23">
-        <v>324</v>
-      </c>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="18"/>
+      <c r="J35" s="22">
+        <v>210</v>
+      </c>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="17"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="1"/>
@@ -4057,98 +4185,98 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="23">
-        <v>284</v>
-      </c>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="18"/>
+      <c r="J36" s="22">
+        <v>156</v>
+      </c>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="17"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="5"/>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="23">
-        <v>210</v>
-      </c>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="18"/>
+      <c r="J37" s="1">
+        <v>264.5</v>
+      </c>
+      <c r="K37" s="18">
+        <v>250</v>
+      </c>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="17"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="5"/>
+      <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="23">
-        <v>156</v>
-      </c>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="18"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="17"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="1"/>
+      <c r="B39" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="1">
-        <v>264.5</v>
-      </c>
-      <c r="K39" s="19">
-        <v>250</v>
-      </c>
+      <c r="J39" s="22">
+        <v>16.2</v>
+      </c>
+      <c r="K39" s="19"/>
       <c r="L39" s="19"/>
       <c r="M39" s="19"/>
-      <c r="N39" s="18"/>
+      <c r="N39" s="17"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D40" s="1"/>
+      <c r="B40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="J40" s="22">
+        <v>13.4</v>
+      </c>
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
       <c r="M40" s="19"/>
-      <c r="N40" s="18"/>
+      <c r="N40" s="17"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="1"/>
@@ -4156,20 +4284,20 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="23">
-        <v>16.2</v>
-      </c>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="18"/>
+      <c r="J41" s="22">
+        <v>6.7</v>
+      </c>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="17"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="1"/>
@@ -4177,20 +4305,20 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="23">
-        <v>13.4</v>
-      </c>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="18"/>
+      <c r="J42" s="22">
+        <v>5</v>
+      </c>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="17"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="1"/>
@@ -4198,20 +4326,20 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="23">
-        <v>6.7</v>
-      </c>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="18"/>
+      <c r="J43" s="22">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="17"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="1"/>
@@ -4219,71 +4347,68 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="23">
-        <v>5</v>
-      </c>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="18"/>
+      <c r="J44" s="22">
+        <v>1.849</v>
+      </c>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="17"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="5"/>
+      <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="23">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="18"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="17"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D46" s="5"/>
+      <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="23">
-        <v>1.849</v>
-      </c>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="18"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="17"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="C47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1.0410000000000001E-2</v>
+      </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="18"/>
+      <c r="J47" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18">
+        <f>0.007</f>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="M47" s="18"/>
+      <c r="N47" s="17"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
@@ -4293,39 +4418,38 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="19"/>
-      <c r="N48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="17"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1.0410000000000001E-2</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="G49" s="20">
+        <v>5.54</v>
+      </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="K49" s="19"/>
-      <c r="L49" s="19">
-        <f>0.007</f>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="M49" s="19"/>
-      <c r="N49" s="18"/>
+        <v>5.54</v>
+      </c>
+      <c r="K49" s="18">
+        <v>5.54</v>
+      </c>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="17"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
@@ -4335,162 +4459,138 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="17"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C51" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="21">
-        <v>5.54</v>
-      </c>
+      <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1">
-        <v>5.54</v>
-      </c>
-      <c r="K51" s="19">
-        <v>5.54</v>
-      </c>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="18"/>
+        <f>2.328/1000</f>
+        <v>2.3279999999999998E-3</v>
+      </c>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="17"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" t="s">
+        <v>111</v>
+      </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
-      <c r="N52" s="18"/>
+      <c r="J52" s="1">
+        <f>28.1/1000</f>
+        <v>2.81E-2</v>
+      </c>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="17"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1">
-        <f>2.328/1000</f>
-        <v>2.3279999999999998E-3</v>
-      </c>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="18"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="17"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" t="s">
-        <v>112</v>
-      </c>
       <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1">
-        <f>28.1/1000</f>
-        <v>2.81E-2</v>
-      </c>
-      <c r="K54" s="19"/>
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="18"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="17"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="19"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="18"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="17"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="19"/>
-      <c r="N56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="17"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="19"/>
-      <c r="M57" s="19"/>
-      <c r="N57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="17"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+      <c r="N58" s="17"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="19"/>
-      <c r="M59" s="19"/>
-      <c r="N59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="17"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D60" s="1"/>
+      <c r="D60" s="2"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
-      <c r="M60" s="19"/>
-      <c r="N60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="17"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
-      <c r="M61" s="19"/>
-      <c r="N61" s="18"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D62" s="2"/>
+      <c r="D62" s="1"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="19"/>
-      <c r="L62" s="19"/>
-      <c r="M62" s="19"/>
-      <c r="N62" s="18"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
@@ -4526,20 +4626,6 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
-    </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-    </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4549,10 +4635,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4579,7 +4665,7 @@
         <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -4590,25 +4676,25 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="1">
         <f>(D8*J4+D9*J5+D10*J6+D11*J7)/108.4</f>
@@ -4637,20 +4723,20 @@
         <f>AVERAGE(D2:I2)</f>
         <v>6.3562007742096346E-2</v>
       </c>
-      <c r="K2" s="19">
+      <c r="K2" s="18">
         <v>2E-3</v>
       </c>
-      <c r="L2" s="19">
+      <c r="L2" s="18">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="M2" s="19"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="1">
         <v>0.53639999999999999</v>
@@ -4674,13 +4760,13 @@
         <f>AVERAGE(D3:I3)</f>
         <v>0.59443800000000002</v>
       </c>
-      <c r="K3" s="19">
+      <c r="K3" s="18">
         <v>0.57150000000000001</v>
       </c>
-      <c r="L3" s="19">
+      <c r="L3" s="18">
         <v>0.58150000000000002</v>
       </c>
-      <c r="M3" s="19">
+      <c r="M3" s="18">
         <v>0.47</v>
       </c>
     </row>
@@ -4688,8 +4774,8 @@
       <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>116</v>
+      <c r="C4" s="17" t="s">
+        <v>115</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -4700,16 +4786,16 @@
       <c r="J4" s="1">
         <v>7.3440000000000005E-2</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>117</v>
+      <c r="C5" s="17" t="s">
+        <v>116</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -4720,16 +4806,16 @@
       <c r="J5" s="1">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>118</v>
+      <c r="C6" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -4741,15 +4827,15 @@
         <f>(0.1332+0.14652)/2</f>
         <v>0.13986000000000001</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -4759,22 +4845,22 @@
       <c r="J7" s="1">
         <v>7.5599999999999999E-3</v>
       </c>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="1">
         <v>6.4</v>
       </c>
       <c r="E8" s="1">
         <v>11.7</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>0.35</v>
       </c>
       <c r="G8" s="1">
@@ -4785,15 +4871,15 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="1">
         <v>16.3</v>
       </c>
@@ -4811,15 +4897,15 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="1">
         <v>60.6</v>
       </c>
@@ -4837,15 +4923,15 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="1">
         <v>25.1</v>
       </c>
@@ -4863,9 +4949,9 @@
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
@@ -4875,19 +4961,19 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -4898,16 +4984,16 @@
       <c r="J13" s="1">
         <v>3.2530000000000001</v>
       </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -4918,16 +5004,16 @@
       <c r="J14" s="1">
         <v>8.1639999999999997</v>
       </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" t="s">
         <v>122</v>
-      </c>
-      <c r="C15" t="s">
-        <v>123</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -4938,16 +5024,16 @@
       <c r="J15" s="1">
         <v>3</v>
       </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -4958,9 +5044,9 @@
       <c r="J16" s="1">
         <v>3.8340000000000001</v>
       </c>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
@@ -4969,20 +5055,20 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
         <v>125</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>163</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -4990,31 +5076,40 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1">
-        <v>2.37</v>
-      </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
+      <c r="J18" s="20">
+        <v>2.29</v>
+      </c>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18">
+        <v>2.29</v>
+      </c>
+      <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>126</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
+      <c r="J19" s="20">
+        <v>1.74</v>
+      </c>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18">
+        <v>1.74</v>
+      </c>
+      <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>126</v>
-      </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
         <v>127</v>
@@ -5025,18 +5120,18 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="21">
-        <v>2.29</v>
-      </c>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19">
-        <v>2.29</v>
-      </c>
-      <c r="M20" s="19"/>
+      <c r="J20" s="20">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="M20" s="18"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>128</v>
@@ -5047,18 +5142,18 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="21">
-        <v>1.74</v>
-      </c>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19">
-        <v>1.74</v>
-      </c>
-      <c r="M21" s="19"/>
+      <c r="J21" s="20">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
         <v>129</v>
@@ -5069,18 +5164,18 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="21">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="M22" s="19"/>
+      <c r="J22" s="20">
+        <v>0.223</v>
+      </c>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18">
+        <v>0.223</v>
+      </c>
+      <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>130</v>
@@ -5091,18 +5186,18 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="21">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="M23" s="19"/>
+      <c r="J23" s="20">
+        <v>1.75</v>
+      </c>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18">
+        <v>1.75</v>
+      </c>
+      <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
         <v>131</v>
@@ -5113,18 +5208,18 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="21">
-        <v>0.223</v>
-      </c>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19">
-        <v>0.223</v>
-      </c>
-      <c r="M24" s="19"/>
+      <c r="J24" s="20">
+        <v>8.3099999999999997E-3</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18">
+        <v>8.3099999999999997E-3</v>
+      </c>
+      <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
         <v>132</v>
@@ -5135,18 +5230,18 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="21">
-        <v>1.75</v>
-      </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19">
-        <v>1.75</v>
-      </c>
-      <c r="M25" s="19"/>
+      <c r="J25" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18">
+        <v>0.95</v>
+      </c>
+      <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
         <v>133</v>
@@ -5157,18 +5252,18 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="21">
-        <v>8.3099999999999997E-3</v>
-      </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19">
-        <v>8.3099999999999997E-3</v>
-      </c>
-      <c r="M26" s="19"/>
+      <c r="J26" s="20">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
         <v>134</v>
@@ -5179,18 +5274,18 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="21">
-        <v>0.95</v>
-      </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19">
-        <v>0.95</v>
-      </c>
-      <c r="M27" s="19"/>
+      <c r="J27" s="20">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18">
+        <v>1.9E-2</v>
+      </c>
+      <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
         <v>135</v>
@@ -5201,21 +5296,21 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="21">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="M28" s="19"/>
+      <c r="J28" s="20">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -5223,21 +5318,14 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="21">
-        <v>1.9E-2</v>
-      </c>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19">
-        <v>1.9E-2</v>
-      </c>
-      <c r="M29" s="19"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -5245,21 +5333,20 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="21">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="M30" s="19"/>
+      <c r="J30" s="20">
+        <f>AVERAGE(J18:J28)</f>
+        <v>0.87493727272727273</v>
+      </c>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18">
+        <f>AVERAGE(L18:L28)</f>
+        <v>0.87493727272727273</v>
+      </c>
+      <c r="M30" s="18"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>138</v>
-      </c>
-      <c r="C31" t="s">
-        <v>139</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -5267,34 +5354,31 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>77</v>
-      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="21">
-        <f>AVERAGE(J20:J30)</f>
-        <v>0.87493727272727273</v>
-      </c>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19">
-        <f>AVERAGE(L20:L30)</f>
-        <v>0.87493727272727273</v>
-      </c>
-      <c r="M32" s="19"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>139</v>
+      </c>
       <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
         <v>140</v>
       </c>
       <c r="D33" s="1"/>
@@ -5303,29 +5387,40 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
+      <c r="J33" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
+        <v>141</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
+      <c r="J34" s="1">
+        <v>26.7</v>
+      </c>
+      <c r="K34" s="18">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="L34" s="18">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="M34" s="18"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>141</v>
-      </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
         <v>142</v>
@@ -5337,15 +5432,15 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1">
-        <v>12.4</v>
-      </c>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
+        <v>22.6</v>
+      </c>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
         <v>143</v>
@@ -5357,19 +5452,15 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1">
-        <v>26.7</v>
-      </c>
-      <c r="K36" s="19">
-        <v>9.2200000000000006</v>
-      </c>
-      <c r="L36" s="19">
-        <v>9.7899999999999991</v>
-      </c>
-      <c r="M36" s="19"/>
+        <v>16.7</v>
+      </c>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
         <v>144</v>
@@ -5381,18 +5472,15 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1">
-        <v>22.6</v>
-      </c>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
+        <v>12.7</v>
+      </c>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -5401,35 +5489,37 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1">
-        <v>16.7</v>
-      </c>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
+        <v>25.5</v>
+      </c>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18">
+        <v>10.97</v>
+      </c>
+      <c r="M38" s="18">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" t="s">
-        <v>146</v>
-      </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="1">
-        <v>12.7</v>
-      </c>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>145</v>
+      </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>146</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -5438,34 +5528,35 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19">
-        <v>10.97</v>
-      </c>
-      <c r="M40" s="19">
-        <v>18</v>
-      </c>
+        <v>1.08</v>
+      </c>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" t="s">
+        <v>147</v>
+      </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
+      <c r="J41" s="1">
+        <v>1.32</v>
+      </c>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>147</v>
-      </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
         <v>148</v>
@@ -5477,15 +5568,15 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1">
-        <v>1.08</v>
-      </c>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
         <v>149</v>
@@ -5497,15 +5588,15 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1">
-        <v>1.32</v>
-      </c>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
+        <v>-0.62</v>
+      </c>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
         <v>150</v>
@@ -5517,15 +5608,15 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1">
-        <v>0.33400000000000002</v>
-      </c>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C45" t="s">
         <v>151</v>
@@ -5537,18 +5628,15 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1">
-        <v>-0.62</v>
-      </c>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
+        <v>0.1719</v>
+      </c>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" t="s">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -5556,47 +5644,51 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="1">
-        <v>2.2700000000000001E-2</v>
-      </c>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" t="s">
-        <v>153</v>
-      </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="1">
-        <v>0.1719</v>
-      </c>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>152</v>
+      </c>
       <c r="B48" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="1">
+        <v>6.2500000000000001E-4</v>
+      </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="19"/>
+      <c r="J48" s="20">
+        <f>0.0004</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18">
+        <f>0.0004</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
@@ -5606,38 +5698,32 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="19"/>
-      <c r="L49" s="19"/>
-      <c r="M49" s="19"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>154</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C50" t="s">
         <v>155</v>
       </c>
-      <c r="D50" s="1">
-        <v>6.2500000000000001E-4</v>
-      </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="21">
-        <f>0.0004</f>
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19">
-        <f>0.0004</f>
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="M50" s="19"/>
+      <c r="J50" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
@@ -5647,16 +5733,16 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>156</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
         <v>157</v>
@@ -5668,99 +5754,78 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
+        <f>0.16386667/1000</f>
+        <v>1.6386666999999999E-4</v>
+      </c>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>158</v>
+      </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>158</v>
-      </c>
-      <c r="B54" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" t="s">
-        <v>159</v>
-      </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1">
-        <f>0.16386667/1000</f>
-        <v>1.6386666999999999E-4</v>
-      </c>
-      <c r="K54" s="19"/>
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" t="s">
-        <v>160</v>
-      </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1">
+      <c r="J53" s="1">
         <f>1.89/1000</f>
         <v>1.89E-3</v>
       </c>
-      <c r="K55" s="19"/>
-      <c r="L55" s="19"/>
-      <c r="M55" s="19"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="19"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="19"/>
-      <c r="M57" s="19"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="19"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="19"/>
-      <c r="M59" s="19"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D60" s="1"/>
+      <c r="D60" s="11"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -5774,14 +5839,14 @@
       <c r="M61" s="1"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D62" s="12"/>
+      <c r="D62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D63" s="1"/>
+      <c r="D63" s="2"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -5795,7 +5860,7 @@
       <c r="M64" s="1"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D65" s="2"/>
+      <c r="D65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -5816,30 +5881,30 @@
       <c r="M67" s="1"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D68" s="1"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="13"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D69" s="1"/>
+      <c r="D69" s="11"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="14"/>
+      <c r="D70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D71" s="12"/>
+      <c r="D71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -5852,20 +5917,6 @@
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
JW: seedlings warnings + added option "Other crops" into q2. Therefore, removed endive as a crop choice.
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{8726C29A-CF30-40DC-BA00-6589F3D6DC91}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_70300F179F726ECB79E16202CD8D362F8E168157" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B05E11F1-2632-4B9D-9F01-C13BD2AE684F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,8 +41,6 @@
     <author>tc={8FE4F82F-6907-41E0-ACF1-311361FEC4C7}</author>
     <author>tc={F0E4EA42-2698-47D0-A222-D1E83A6DAA7D}</author>
     <author>tc={D21AF469-E910-4274-AF0D-7D27B238D9E7}</author>
-    <author>tc={DEC464CC-8A70-4C86-9116-9C8B145BBB1E}</author>
-    <author>tc={3C953827-5C2D-4742-A6F6-150B1C1BC74D}</author>
     <author>tc={5667D7E8-CE45-48EB-8BEF-B2A681E2E308}</author>
     <author>tc={3D18DAF9-FA04-48E1-A8CB-5C5ED8180794}</author>
     <author>tc={81A05FB6-F8D5-4215-B674-8F1D2351605B}</author>
@@ -68,6 +66,8 @@
     <author>tc={B619E217-C26E-484F-96C6-1045106C5109}</author>
     <author>tc={54D768C3-619F-4830-A4DF-B4A28BE5731C}</author>
     <author>tc={3CBB2313-6869-4ADB-8678-F0A56C53B204}</author>
+    <author>tc={DEC464CC-8A70-4C86-9116-9C8B145BBB1E}</author>
+    <author>tc={3C953827-5C2D-4742-A6F6-150B1C1BC74D}</author>
   </authors>
   <commentList>
     <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -178,43 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    https://www.agriculturejournals.cz/publicFiles/00115.pdf
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    https://medcraveonline.com/APAR/APAR-05-00173.pdf
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B3" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -232,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B4" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -250,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="C4" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -268,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="D4" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="F4" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -304,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="B5" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -322,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="B6" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -340,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="F6" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -358,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="B7" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -376,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="C7" authorId="15" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -394,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="F7" authorId="16" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -412,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="B8" authorId="17" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -430,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="C8" authorId="18" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -448,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="D8" authorId="19" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -466,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="F8" authorId="20" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -484,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="A9" authorId="21" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -506,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+    <comment ref="B9" authorId="22" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -529,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
+    <comment ref="C9" authorId="23" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -547,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
+    <comment ref="D9" authorId="24" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -566,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
+    <comment ref="E9" authorId="25" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -584,7 +548,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="28" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
+    <comment ref="F9" authorId="26" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -604,7 +568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="29" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
+    <comment ref="B10" authorId="27" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -622,7 +586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="30" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
+    <comment ref="C10" authorId="28" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -640,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="31" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
+    <comment ref="D10" authorId="29" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -658,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="32" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
+    <comment ref="F10" authorId="30" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -672,6 +636,42 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://homeguides.sfgate.com/long-mint-need-grow-70659.html
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="31" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.agriculturejournals.cz/publicFiles/00115.pdf
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="32" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://medcraveonline.com/APAR/APAR-05-00173.pdf
 </t>
         </r>
       </text>
@@ -1521,7 +1521,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="164">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -2007,6 +2007,12 @@
   </si>
   <si>
     <t>seeds (MJ/kg)</t>
+  </si>
+  <si>
+    <t>Not used now:</t>
+  </si>
+  <si>
+    <t>Other crops</t>
   </si>
 </sst>
 </file>
@@ -2061,7 +2067,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -2125,36 +2131,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -2246,6 +2222,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -2254,6 +2260,47 @@
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -2268,7 +2315,7 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -2276,12 +2323,14 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -2292,7 +2341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2307,7 +2356,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2326,10 +2374,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2344,9 +2395,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2357,6 +2406,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3030,10 +3089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3062,13 +3121,13 @@
       <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3076,264 +3135,305 @@
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0.58630000000000004</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>0.8</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="23">
         <v>1.11E-6</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="23">
         <v>620</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="28">
         <v>45</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="30">
         <v>2.37</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="26">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="24">
-        <v>0.55049999999999999</v>
-      </c>
-      <c r="C3" s="24">
-        <v>0.7</v>
-      </c>
-      <c r="D3" s="24">
-        <v>1.11E-6</v>
-      </c>
-      <c r="E3" s="24">
-        <v>710</v>
-      </c>
-      <c r="F3" s="30">
-        <v>85</v>
-      </c>
-      <c r="G3" s="32">
+        <v>7</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.2268</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="D3" s="23">
+        <v>1.3329999999999999E-5</v>
+      </c>
+      <c r="E3" s="23">
+        <v>1080</v>
+      </c>
+      <c r="F3" s="28">
+        <v>45</v>
+      </c>
+      <c r="G3" s="30">
         <v>2.37</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="26">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="24">
-        <v>0.2268</v>
-      </c>
-      <c r="C4" s="24">
-        <v>0.6</v>
-      </c>
-      <c r="D4" s="24">
-        <v>1.3329999999999999E-5</v>
-      </c>
-      <c r="E4" s="24">
-        <v>1080</v>
-      </c>
-      <c r="F4" s="30">
-        <v>45</v>
-      </c>
-      <c r="G4" s="32">
+        <v>8</v>
+      </c>
+      <c r="B4" s="23">
+        <v>2.3279999999999999E-4</v>
+      </c>
+      <c r="C4" s="23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D4" s="23">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="E4" s="23">
+        <v>970</v>
+      </c>
+      <c r="F4" s="28">
+        <v>3.5</v>
+      </c>
+      <c r="G4" s="30">
         <v>2.37</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="26">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="24">
-        <v>2.3279999999999999E-4</v>
-      </c>
-      <c r="C5" s="24">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D5" s="24">
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="E5" s="24">
-        <v>970</v>
-      </c>
-      <c r="F5" s="30">
-        <v>3.5</v>
-      </c>
-      <c r="G5" s="32">
+        <v>9</v>
+      </c>
+      <c r="B5" s="23">
+        <v>4.5799999999999999E-3</v>
+      </c>
+      <c r="C5" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1.8199999999999999E-6</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1250</v>
+      </c>
+      <c r="F5" s="28">
+        <v>77.5</v>
+      </c>
+      <c r="G5" s="30">
         <v>2.37</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="26">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="24">
-        <v>4.5799999999999999E-3</v>
-      </c>
-      <c r="C6" s="24">
-        <v>0.6</v>
-      </c>
-      <c r="D6" s="24">
-        <v>1.8199999999999999E-6</v>
-      </c>
-      <c r="E6" s="24">
-        <v>1250</v>
-      </c>
-      <c r="F6" s="30">
-        <v>77.5</v>
-      </c>
-      <c r="G6" s="32">
+        <v>10</v>
+      </c>
+      <c r="B6" s="23">
+        <v>4.0125000000000001E-2</v>
+      </c>
+      <c r="C6" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="23">
+        <v>3.6399999999999999E-6</v>
+      </c>
+      <c r="E6" s="23">
+        <v>1930</v>
+      </c>
+      <c r="F6" s="28">
+        <v>75</v>
+      </c>
+      <c r="G6" s="30">
         <v>2.37</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="26">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="24">
-        <v>4.0125000000000001E-2</v>
-      </c>
-      <c r="C7" s="24">
-        <v>0.75</v>
-      </c>
-      <c r="D7" s="24">
-        <v>3.6399999999999999E-6</v>
-      </c>
-      <c r="E7" s="24">
-        <v>1930</v>
-      </c>
-      <c r="F7" s="30">
-        <v>75</v>
-      </c>
-      <c r="G7" s="32">
+        <v>11</v>
+      </c>
+      <c r="B7" s="23">
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0.85</v>
+      </c>
+      <c r="D7" s="23">
+        <v>1.5999999999999999E-6</v>
+      </c>
+      <c r="E7" s="23">
+        <v>2000</v>
+      </c>
+      <c r="F7" s="28">
+        <v>55</v>
+      </c>
+      <c r="G7" s="30">
         <v>2.37</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="26">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="24">
-        <v>9.6600000000000005E-2</v>
-      </c>
-      <c r="C8" s="24">
-        <v>0.85</v>
-      </c>
-      <c r="D8" s="24">
-        <v>1.5999999999999999E-6</v>
-      </c>
-      <c r="E8" s="24">
-        <v>2000</v>
-      </c>
-      <c r="F8" s="30">
-        <v>55</v>
-      </c>
-      <c r="G8" s="32">
+        <v>12</v>
+      </c>
+      <c r="B8" s="23">
+        <v>6.2599999999999999E-3</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="23">
+        <v>3.3000000000000002E-7</v>
+      </c>
+      <c r="E8" s="23">
+        <v>980</v>
+      </c>
+      <c r="F8" s="28">
+        <v>17.5</v>
+      </c>
+      <c r="G8" s="30">
         <v>2.37</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="26">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="23">
+        <v>0.35449999999999998</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.67</v>
+      </c>
+      <c r="D9" s="23">
+        <v>8.5000000000000001E-7</v>
+      </c>
+      <c r="E9" s="23">
+        <v>790</v>
+      </c>
+      <c r="F9" s="28">
         <v>12</v>
       </c>
-      <c r="B9" s="24">
-        <v>6.2599999999999999E-3</v>
-      </c>
-      <c r="C9" s="24">
-        <v>0.75</v>
-      </c>
-      <c r="D9" s="24">
-        <v>3.3000000000000002E-7</v>
-      </c>
-      <c r="E9" s="24">
-        <v>980</v>
-      </c>
-      <c r="F9" s="30">
-        <v>17.5</v>
-      </c>
-      <c r="G9" s="32">
+      <c r="G9" s="30">
         <v>2.37</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="26">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="24">
-        <v>0.35449999999999998</v>
-      </c>
-      <c r="C10" s="24">
-        <v>0.67</v>
-      </c>
-      <c r="D10" s="24">
-        <v>8.5000000000000001E-7</v>
-      </c>
-      <c r="E10" s="24">
-        <v>790</v>
-      </c>
-      <c r="F10" s="30">
-        <v>12</v>
-      </c>
-      <c r="G10" s="32">
+      <c r="A10" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="32">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="C10" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="32">
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="E10" s="32">
+        <v>16760</v>
+      </c>
+      <c r="F10" s="33">
+        <v>90</v>
+      </c>
+      <c r="G10" s="34">
         <v>2.37</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="35">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="25">
-        <v>7.9100000000000004E-2</v>
-      </c>
-      <c r="C11" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="25">
-        <v>4.9999999999999998E-8</v>
-      </c>
-      <c r="E11" s="25">
-        <v>16760</v>
-      </c>
-      <c r="F11" s="33">
-        <v>90</v>
-      </c>
-      <c r="G11" s="34">
+      <c r="A11" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="37">
+        <f t="shared" ref="B11:H11" si="0">AVERAGE(B2:B10)</f>
+        <v>0.1549442</v>
+      </c>
+      <c r="C11" s="37">
+        <f t="shared" si="0"/>
+        <v>0.6744444444444444</v>
+      </c>
+      <c r="D11" s="37">
+        <f t="shared" si="0"/>
+        <v>8.0811111111111119E-6</v>
+      </c>
+      <c r="E11" s="37">
+        <f t="shared" si="0"/>
+        <v>2931.1111111111113</v>
+      </c>
+      <c r="F11" s="37">
+        <f t="shared" si="0"/>
+        <v>46.722222222222221</v>
+      </c>
+      <c r="G11" s="37">
+        <f t="shared" si="0"/>
+        <v>2.3700000000000006</v>
+      </c>
+      <c r="H11" s="38">
+        <f t="shared" si="0"/>
+        <v>37.699999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="24"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="39"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="23">
+        <v>0.55049999999999999</v>
+      </c>
+      <c r="C20" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="D20" s="23">
+        <v>1.11E-6</v>
+      </c>
+      <c r="E20" s="23">
+        <v>710</v>
+      </c>
+      <c r="F20" s="28">
+        <v>85</v>
+      </c>
+      <c r="G20" s="30">
         <v>2.37</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H20" s="26">
         <v>37.700000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3385,16 +3485,16 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="17"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3433,10 +3533,10 @@
         <f>AVERAGE(D2:I2)</f>
         <v>0.26047889689199161</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3467,16 +3567,16 @@
         <f>AVERAGE(D3:I3)</f>
         <v>6.9581999999999988</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="16"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="5"/>
@@ -3488,16 +3588,16 @@
       <c r="J4" s="5">
         <v>1.008</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="17"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="16"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="5"/>
@@ -3509,16 +3609,16 @@
       <c r="J5" s="5">
         <v>0.18720000000000001</v>
       </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="17"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="5"/>
@@ -3531,16 +3631,16 @@
         <f>(0.1332+0.17064)/2</f>
         <v>0.15192</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="17"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="16"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="5"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -3550,23 +3650,23 @@
       <c r="J7" s="5">
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="16"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="1">
         <v>6.4</v>
       </c>
       <c r="E8" s="1">
         <v>11.7</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>0.35</v>
       </c>
       <c r="G8" s="1">
@@ -3577,16 +3677,16 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="17"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="16"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="1">
         <v>16.3</v>
       </c>
@@ -3604,16 +3704,16 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="17"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="16"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="1">
         <v>60.6</v>
       </c>
@@ -3631,16 +3731,16 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="17"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="16"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="1">
         <v>25.1</v>
       </c>
@@ -3658,10 +3758,10 @@
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="17"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
@@ -3671,10 +3771,10 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="16"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3695,10 +3795,10 @@
       <c r="J13" s="1">
         <v>82.275999999999996</v>
       </c>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="16"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -3716,10 +3816,10 @@
       <c r="J14" s="1">
         <v>144.43</v>
       </c>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="16"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -3737,10 +3837,10 @@
       <c r="J15" s="1">
         <v>74</v>
       </c>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="16"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -3758,10 +3858,10 @@
       <c r="J16" s="1">
         <v>97.024000000000001</v>
       </c>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="16"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
@@ -3771,10 +3871,10 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="16"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -3792,15 +3892,15 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="21">
+      <c r="J18" s="20">
         <v>14.5</v>
       </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19">
+      <c r="K18" s="18"/>
+      <c r="L18" s="18">
         <v>14.5</v>
       </c>
-      <c r="M18" s="18"/>
-      <c r="N18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="16"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
@@ -3815,15 +3915,15 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="21">
+      <c r="J19" s="20">
         <v>11</v>
       </c>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19">
+      <c r="K19" s="18"/>
+      <c r="L19" s="18">
         <v>11</v>
       </c>
-      <c r="M19" s="18"/>
-      <c r="N19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="16"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -3841,15 +3941,15 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="21">
+      <c r="J20" s="20">
         <v>15.6</v>
       </c>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19">
+      <c r="K20" s="18"/>
+      <c r="L20" s="18">
         <v>15.6</v>
       </c>
-      <c r="M20" s="18"/>
-      <c r="N20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="16"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -3864,15 +3964,15 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="21">
+      <c r="J21" s="20">
         <v>13.7</v>
       </c>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19">
+      <c r="K21" s="18"/>
+      <c r="L21" s="18">
         <v>13.7</v>
       </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="16"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
@@ -3887,15 +3987,15 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="21">
+      <c r="J22" s="20">
         <v>5.54</v>
       </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19">
+      <c r="K22" s="18"/>
+      <c r="L22" s="18">
         <v>5.54</v>
       </c>
-      <c r="M22" s="18"/>
-      <c r="N22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="16"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -3910,15 +4010,15 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="21">
+      <c r="J23" s="20">
         <v>34</v>
       </c>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19">
+      <c r="K23" s="18"/>
+      <c r="L23" s="18">
         <v>34</v>
       </c>
-      <c r="M23" s="18"/>
-      <c r="N23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="16"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
@@ -3933,15 +4033,15 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="21">
+      <c r="J24" s="20">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19">
+      <c r="K24" s="18"/>
+      <c r="L24" s="18">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="M24" s="18"/>
-      <c r="N24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="16"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
@@ -3956,15 +4056,15 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="21">
+      <c r="J25" s="20">
         <v>12</v>
       </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19">
+      <c r="K25" s="18"/>
+      <c r="L25" s="18">
         <v>12</v>
       </c>
-      <c r="M25" s="18"/>
-      <c r="N25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="16"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
@@ -3979,15 +4079,15 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="21">
+      <c r="J26" s="20">
         <v>24.3</v>
       </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19">
+      <c r="K26" s="18"/>
+      <c r="L26" s="18">
         <v>24.3</v>
       </c>
-      <c r="M26" s="18"/>
-      <c r="N26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="16"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -4002,15 +4102,15 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="21">
+      <c r="J27" s="20">
         <v>1.6739999999999999</v>
       </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19">
+      <c r="K27" s="18"/>
+      <c r="L27" s="18">
         <v>1.6739999999999999</v>
       </c>
-      <c r="M27" s="18"/>
-      <c r="N27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="16"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
@@ -4025,15 +4125,15 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="21">
+      <c r="J28" s="20">
         <v>11.9</v>
       </c>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19">
+      <c r="K28" s="18"/>
+      <c r="L28" s="18">
         <v>11.9</v>
       </c>
-      <c r="M28" s="18"/>
-      <c r="N28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="16"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
@@ -4051,10 +4151,10 @@
       <c r="J29" s="1">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="16"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -4067,10 +4167,10 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="16"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
@@ -4080,10 +4180,10 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="16"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
@@ -4098,13 +4198,13 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="22">
+      <c r="J32" s="21">
         <v>160</v>
       </c>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="17"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="16"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
@@ -4119,13 +4219,13 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="22">
+      <c r="J33" s="21">
         <v>324</v>
       </c>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="17"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="16"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -4143,13 +4243,13 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="22">
+      <c r="J34" s="21">
         <v>284</v>
       </c>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="17"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="16"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
@@ -4164,13 +4264,13 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="22">
+      <c r="J35" s="21">
         <v>210</v>
       </c>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="17"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="16"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
@@ -4185,13 +4285,13 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="22">
+      <c r="J36" s="21">
         <v>156</v>
       </c>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="17"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="16"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -4206,12 +4306,12 @@
       <c r="J37" s="1">
         <v>264.5</v>
       </c>
-      <c r="K37" s="18">
+      <c r="K37" s="17">
         <v>250</v>
       </c>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="16"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
@@ -4221,10 +4321,10 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="16"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
@@ -4239,13 +4339,13 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="22">
+      <c r="J39" s="21">
         <v>16.2</v>
       </c>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="17"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="16"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
@@ -4260,13 +4360,13 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="22">
+      <c r="J40" s="21">
         <v>13.4</v>
       </c>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="17"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="16"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -4284,13 +4384,13 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="22">
+      <c r="J41" s="21">
         <v>6.7</v>
       </c>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="17"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="16"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
@@ -4305,13 +4405,13 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="22">
+      <c r="J42" s="21">
         <v>5</v>
       </c>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="17"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="16"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
@@ -4326,13 +4426,13 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="22">
+      <c r="J43" s="21">
         <v>9.1999999999999993</v>
       </c>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="17"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="16"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
@@ -4347,13 +4447,13 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="22">
+      <c r="J44" s="21">
         <v>1.849</v>
       </c>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="17"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="16"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -4366,10 +4466,10 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="16"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
@@ -4379,10 +4479,10 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="16"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
@@ -4402,13 +4502,13 @@
       <c r="J47" s="1">
         <v>0.01</v>
       </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18">
+      <c r="K47" s="17"/>
+      <c r="L47" s="17">
         <f>0.007</f>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="M47" s="18"/>
-      <c r="N47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="16"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
@@ -4418,10 +4518,10 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="16"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -4436,7 +4536,7 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="20">
+      <c r="G49" s="19">
         <v>5.54</v>
       </c>
       <c r="H49" s="1"/>
@@ -4444,12 +4544,12 @@
       <c r="J49" s="1">
         <v>5.54</v>
       </c>
-      <c r="K49" s="18">
+      <c r="K49" s="17">
         <v>5.54</v>
       </c>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="16"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
@@ -4459,10 +4559,10 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="16"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -4484,10 +4584,10 @@
         <f>2.328/1000</f>
         <v>2.3279999999999998E-3</v>
       </c>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="18"/>
-      <c r="N51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="16"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
@@ -4506,10 +4606,10 @@
         <f>28.1/1000</f>
         <v>2.81E-2</v>
       </c>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
-      <c r="N52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="16"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -4517,66 +4617,66 @@
       </c>
       <c r="D53" s="1"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="18"/>
-      <c r="N53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="16"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="16"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
       <c r="J55" s="1"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-      <c r="N55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="16"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
-      <c r="N56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="16"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="17"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="16"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="18"/>
-      <c r="L58" s="18"/>
-      <c r="M58" s="18"/>
-      <c r="N58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="16"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="18"/>
-      <c r="L59" s="18"/>
-      <c r="M59" s="18"/>
-      <c r="N59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="16"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D60" s="2"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="18"/>
-      <c r="L60" s="18"/>
-      <c r="M60" s="18"/>
-      <c r="N60" s="17"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="17"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="16"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
@@ -4676,13 +4776,13 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4723,13 +4823,13 @@
         <f>AVERAGE(D2:I2)</f>
         <v>6.3562007742096346E-2</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="17">
         <v>2E-3</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="17">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="M2" s="18"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -4760,13 +4860,13 @@
         <f>AVERAGE(D3:I3)</f>
         <v>0.59443800000000002</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="17">
         <v>0.57150000000000001</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="17">
         <v>0.58150000000000002</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="17">
         <v>0.47</v>
       </c>
     </row>
@@ -4774,7 +4874,7 @@
       <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>115</v>
       </c>
       <c r="D4" s="1"/>
@@ -4786,15 +4886,15 @@
       <c r="J4" s="1">
         <v>7.3440000000000005E-2</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>116</v>
       </c>
       <c r="D5" s="1"/>
@@ -4806,15 +4906,15 @@
       <c r="J5" s="1">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>117</v>
       </c>
       <c r="D6" s="1"/>
@@ -4827,15 +4927,15 @@
         <f>(0.1332+0.14652)/2</f>
         <v>0.13986000000000001</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -4845,22 +4945,22 @@
       <c r="J7" s="1">
         <v>7.5599999999999999E-3</v>
       </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="1">
         <v>6.4</v>
       </c>
       <c r="E8" s="1">
         <v>11.7</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>0.35</v>
       </c>
       <c r="G8" s="1">
@@ -4871,15 +4971,15 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="1">
         <v>16.3</v>
       </c>
@@ -4897,15 +4997,15 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="1">
         <v>60.6</v>
       </c>
@@ -4923,15 +5023,15 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="1">
         <v>25.1</v>
       </c>
@@ -4949,9 +5049,9 @@
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
@@ -4961,9 +5061,9 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -4984,9 +5084,9 @@
       <c r="J13" s="1">
         <v>3.2530000000000001</v>
       </c>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -5004,9 +5104,9 @@
       <c r="J14" s="1">
         <v>8.1639999999999997</v>
       </c>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -5024,9 +5124,9 @@
       <c r="J15" s="1">
         <v>3</v>
       </c>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -5044,9 +5144,9 @@
       <c r="J16" s="1">
         <v>3.8340000000000001</v>
       </c>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
@@ -5055,10 +5155,10 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5076,14 +5176,14 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="20">
+      <c r="J18" s="19">
         <v>2.29</v>
       </c>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18">
+      <c r="K18" s="17"/>
+      <c r="L18" s="17">
         <v>2.29</v>
       </c>
-      <c r="M18" s="18"/>
+      <c r="M18" s="17"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -5098,14 +5198,14 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="20">
+      <c r="J19" s="19">
         <v>1.74</v>
       </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18">
+      <c r="K19" s="17"/>
+      <c r="L19" s="17">
         <v>1.74</v>
       </c>
-      <c r="M19" s="18"/>
+      <c r="M19" s="17"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -5120,14 +5220,14 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="20">
+      <c r="J20" s="19">
         <v>0.61199999999999999</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18">
+      <c r="K20" s="17"/>
+      <c r="L20" s="17">
         <v>0.61199999999999999</v>
       </c>
-      <c r="M20" s="18"/>
+      <c r="M20" s="17"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -5142,14 +5242,14 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="20">
+      <c r="J21" s="19">
         <v>0.55300000000000005</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18">
+      <c r="K21" s="17"/>
+      <c r="L21" s="17">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M21" s="18"/>
+      <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -5164,14 +5264,14 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="20">
+      <c r="J22" s="19">
         <v>0.223</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18">
+      <c r="K22" s="17"/>
+      <c r="L22" s="17">
         <v>0.223</v>
       </c>
-      <c r="M22" s="18"/>
+      <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -5186,14 +5286,14 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="20">
+      <c r="J23" s="19">
         <v>1.75</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18">
+      <c r="K23" s="17"/>
+      <c r="L23" s="17">
         <v>1.75</v>
       </c>
-      <c r="M23" s="18"/>
+      <c r="M23" s="17"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -5208,14 +5308,14 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="20">
+      <c r="J24" s="19">
         <v>8.3099999999999997E-3</v>
       </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18">
+      <c r="K24" s="17"/>
+      <c r="L24" s="17">
         <v>8.3099999999999997E-3</v>
       </c>
-      <c r="M24" s="18"/>
+      <c r="M24" s="17"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -5230,14 +5330,14 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="20">
+      <c r="J25" s="19">
         <v>0.95</v>
       </c>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18">
+      <c r="K25" s="17"/>
+      <c r="L25" s="17">
         <v>0.95</v>
       </c>
-      <c r="M25" s="18"/>
+      <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -5252,14 +5352,14 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="20">
+      <c r="J26" s="19">
         <v>0.56200000000000006</v>
       </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18">
+      <c r="K26" s="17"/>
+      <c r="L26" s="17">
         <v>0.56200000000000006</v>
       </c>
-      <c r="M26" s="18"/>
+      <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -5274,14 +5374,14 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="20">
+      <c r="J27" s="19">
         <v>1.9E-2</v>
       </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18">
+      <c r="K27" s="17"/>
+      <c r="L27" s="17">
         <v>1.9E-2</v>
       </c>
-      <c r="M27" s="18"/>
+      <c r="M27" s="17"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -5296,14 +5396,14 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="20">
+      <c r="J28" s="19">
         <v>0.91700000000000004</v>
       </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18">
+      <c r="K28" s="17"/>
+      <c r="L28" s="17">
         <v>0.91700000000000004</v>
       </c>
-      <c r="M28" s="18"/>
+      <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -5318,10 +5418,10 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -5333,16 +5433,16 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="20">
+      <c r="J30" s="19">
         <f>AVERAGE(J18:J28)</f>
         <v>0.87493727272727273</v>
       </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18">
+      <c r="K30" s="17"/>
+      <c r="L30" s="17">
         <f>AVERAGE(L18:L28)</f>
         <v>0.87493727272727273</v>
       </c>
-      <c r="M30" s="18"/>
+      <c r="M30" s="17"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -5355,9 +5455,9 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
@@ -5367,9 +5467,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -5390,9 +5490,9 @@
       <c r="J33" s="1">
         <v>12.4</v>
       </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
@@ -5410,13 +5510,13 @@
       <c r="J34" s="1">
         <v>26.7</v>
       </c>
-      <c r="K34" s="18">
+      <c r="K34" s="17">
         <v>9.2200000000000006</v>
       </c>
-      <c r="L34" s="18">
+      <c r="L34" s="17">
         <v>9.7899999999999991</v>
       </c>
-      <c r="M34" s="18"/>
+      <c r="M34" s="17"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -5434,9 +5534,9 @@
       <c r="J35" s="1">
         <v>22.6</v>
       </c>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -5454,9 +5554,9 @@
       <c r="J36" s="1">
         <v>16.7</v>
       </c>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -5474,9 +5574,9 @@
       <c r="J37" s="1">
         <v>12.7</v>
       </c>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -5491,11 +5591,11 @@
       <c r="J38" s="1">
         <v>25.5</v>
       </c>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18">
+      <c r="K38" s="17"/>
+      <c r="L38" s="17">
         <v>10.97</v>
       </c>
-      <c r="M38" s="18">
+      <c r="M38" s="17">
         <v>18</v>
       </c>
     </row>
@@ -5507,9 +5607,9 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -5530,9 +5630,9 @@
       <c r="J40" s="1">
         <v>1.08</v>
       </c>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
@@ -5550,9 +5650,9 @@
       <c r="J41" s="1">
         <v>1.32</v>
       </c>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -5570,9 +5670,9 @@
       <c r="J42" s="1">
         <v>0.33400000000000002</v>
       </c>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
@@ -5590,9 +5690,9 @@
       <c r="J43" s="1">
         <v>-0.62</v>
       </c>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -5610,9 +5710,9 @@
       <c r="J44" s="1">
         <v>2.2700000000000001E-2</v>
       </c>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -5630,9 +5730,9 @@
       <c r="J45" s="1">
         <v>0.1719</v>
       </c>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -5645,9 +5745,9 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
@@ -5657,9 +5757,9 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -5679,16 +5779,16 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="20">
+      <c r="J48" s="19">
         <f>0.0004</f>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18">
+      <c r="K48" s="17"/>
+      <c r="L48" s="17">
         <f>0.0004</f>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="M48" s="18"/>
+      <c r="M48" s="17"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
@@ -5698,9 +5798,9 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -5721,9 +5821,9 @@
       <c r="J50" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
@@ -5733,9 +5833,9 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="18"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -5757,9 +5857,9 @@
         <f>0.16386667/1000</f>
         <v>1.6386666999999999E-4</v>
       </c>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
@@ -5778,37 +5878,37 @@
         <f>1.89/1000</f>
         <v>1.89E-3</v>
       </c>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="18"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
       <c r="J55" s="1"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
@@ -5825,7 +5925,7 @@
       <c r="M59" s="1"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D60" s="11"/>
+      <c r="D60" s="10"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -5881,16 +5981,16 @@
       <c r="M67" s="1"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="13"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="12"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D69" s="11"/>
+      <c r="D69" s="10"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>

</xml_diff>

<commit_message>
LvdB: version 25-6, implemented stainless steel
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
@@ -1022,6 +1022,7 @@
     <author>tc={79E25465-3D46-40B7-B8A8-18DD9D6306B0}</author>
     <author>tc={7A90E5E2-2E08-4861-A6C8-2E490EE47A92}</author>
     <author>tc={25BEEA18-2FB0-45C9-B9D8-E5E62F8643F3}</author>
+    <author>Gebruiker</author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0" shapeId="0">
@@ -1512,6 +1513,30 @@
 Comment:
     We need to review this again for each country
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B52" authorId="27" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gebruiker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+combined value of small medium and large truck</t>
         </r>
       </text>
     </comment>
@@ -1520,7 +1545,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="189">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -1672,9 +1697,6 @@
     <t>Fo10</t>
   </si>
   <si>
-    <t>Planting material (MJ/kg)</t>
-  </si>
-  <si>
     <t>Fertilizer (MJ/l)</t>
   </si>
   <si>
@@ -2014,12 +2036,6 @@
     <t>Other crops</t>
   </si>
   <si>
-    <t>Building (CO2eq/kg)</t>
-  </si>
-  <si>
-    <t>Steel</t>
-  </si>
-  <si>
     <t>Aluminium</t>
   </si>
   <si>
@@ -2057,6 +2073,45 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Truck empty return</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>Van empty return</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>Black steel</t>
+  </si>
+  <si>
+    <t>Stainless steel</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>growing system (CO2eq/kg)</t>
+  </si>
+  <si>
+    <t>growing system (MJ/kg)</t>
+  </si>
+  <si>
+    <t>BL4</t>
   </si>
 </sst>
 </file>
@@ -2067,7 +2122,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2103,6 +2158,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3103,8 +3171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3137,10 +3205,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>160</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3388,7 +3456,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" s="35">
         <f t="shared" ref="B11:H11" si="0">AVERAGE(B2:B10)</f>
@@ -3427,7 +3495,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3465,10 +3533,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3496,7 +3564,7 @@
         <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -3505,7 +3573,7 @@
         <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K1" t="s">
         <v>21</v>
@@ -3922,10 +3990,10 @@
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="1"/>
@@ -3946,10 +4014,10 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="1"/>
@@ -3969,14 +4037,11 @@
       <c r="O19" s="16"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
       <c r="B20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="1"/>
@@ -3997,10 +4062,10 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="1"/>
@@ -4021,10 +4086,10 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="1"/>
@@ -4045,10 +4110,10 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
@@ -4069,10 +4134,10 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="1"/>
@@ -4093,10 +4158,10 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="1"/>
@@ -4117,10 +4182,10 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="1"/>
@@ -4141,10 +4206,10 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
@@ -4165,10 +4230,10 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="1"/>
@@ -4189,10 +4254,10 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="1"/>
@@ -4211,7 +4276,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -4242,10 +4307,10 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="1"/>
@@ -4264,10 +4329,10 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="1"/>
@@ -4286,13 +4351,13 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="1"/>
@@ -4311,10 +4376,10 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="1"/>
@@ -4333,10 +4398,10 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="1"/>
@@ -4355,7 +4420,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -4390,10 +4455,10 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="1"/>
@@ -4412,10 +4477,10 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="1"/>
@@ -4434,13 +4499,13 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="1"/>
@@ -4459,10 +4524,10 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="1"/>
@@ -4481,10 +4546,10 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="1"/>
@@ -4503,10 +4568,10 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="1"/>
@@ -4525,7 +4590,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -4556,13 +4621,13 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" t="s">
         <v>101</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>102</v>
-      </c>
-      <c r="C47" t="s">
-        <v>103</v>
       </c>
       <c r="D47" s="1">
         <v>1.0410000000000001E-2</v>
@@ -4574,7 +4639,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1">
-        <v>0.01</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="L47" s="17"/>
       <c r="M47" s="17">
@@ -4600,13 +4665,13 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
         <v>104</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>105</v>
-      </c>
-      <c r="C49" t="s">
-        <v>106</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -4643,13 +4708,13 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" t="s">
         <v>107</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>108</v>
-      </c>
-      <c r="C51" t="s">
-        <v>109</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -4669,10 +4734,10 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s">
         <v>110</v>
-      </c>
-      <c r="C52" t="s">
-        <v>111</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -4691,26 +4756,43 @@
       <c r="O52" s="16"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" t="s">
+        <v>180</v>
+      </c>
       <c r="D53" s="1"/>
-      <c r="K53" s="3"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="38">
+        <v>3.463333</v>
+      </c>
       <c r="L53" s="17"/>
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
       <c r="O53" s="16"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>164</v>
-      </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="C54" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
       <c r="K54" s="38">
-        <v>3.34</v>
+        <v>42.15</v>
       </c>
       <c r="L54" s="17"/>
       <c r="M54" s="17"/>
@@ -4718,31 +4800,25 @@
       <c r="O54" s="16"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>166</v>
-      </c>
-      <c r="C55" s="37" t="s">
-        <v>176</v>
-      </c>
       <c r="D55" s="1"/>
-      <c r="K55" s="38">
-        <v>147</v>
-      </c>
+      <c r="K55" s="3"/>
       <c r="L55" s="17"/>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
       <c r="O55" s="16"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>187</v>
+      </c>
       <c r="B56" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="C56" t="s">
-        <v>177</v>
-      </c>
-      <c r="D56" s="1"/>
-      <c r="K56" s="38">
-        <v>50.1</v>
+        <v>166</v>
+      </c>
+      <c r="K56">
+        <v>37.1</v>
       </c>
       <c r="L56" s="17"/>
       <c r="M56" s="17"/>
@@ -4750,31 +4826,55 @@
       <c r="O56" s="16"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" t="s">
+        <v>173</v>
+      </c>
       <c r="D57" s="1"/>
-      <c r="K57" s="1"/>
+      <c r="K57" s="38">
+        <v>3.34</v>
+      </c>
       <c r="L57" s="17"/>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
       <c r="O57" s="16"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" s="37" t="s">
+        <v>174</v>
+      </c>
       <c r="D58" s="1"/>
-      <c r="K58" s="1"/>
+      <c r="K58" s="38">
+        <v>147</v>
+      </c>
       <c r="L58" s="17"/>
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
       <c r="O58" s="16"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" t="s">
+        <v>184</v>
+      </c>
       <c r="D59" s="1"/>
-      <c r="K59" s="1"/>
+      <c r="K59" s="38">
+        <v>50.1</v>
+      </c>
       <c r="L59" s="17"/>
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
       <c r="O59" s="16"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D60" s="2"/>
+      <c r="D60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="17"/>
       <c r="M60" s="17"/>
@@ -4784,16 +4884,18 @@
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
       <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="16"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D62" s="1"/>
+      <c r="D62" s="2"/>
       <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="16"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
@@ -4829,6 +4931,20 @@
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
+    </row>
+    <row r="68" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+    </row>
+    <row r="69" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4838,10 +4954,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4868,7 +4984,7 @@
         <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -4877,7 +4993,7 @@
         <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K1" t="s">
         <v>21</v>
@@ -4894,13 +5010,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="1">
         <f>(D8*K4+D9*K5+D10*K6+D11*K7)/108.4</f>
@@ -4943,7 +5059,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" s="1">
         <v>0.53639999999999999</v>
@@ -4983,7 +5099,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -5004,7 +5120,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -5025,7 +5141,7 @@
         <v>34</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -5184,13 +5300,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -5211,7 +5327,7 @@
         <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -5229,10 +5345,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" t="s">
         <v>121</v>
-      </c>
-      <c r="C15" t="s">
-        <v>122</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -5253,7 +5369,7 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -5284,13 +5400,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
         <v>124</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>125</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5310,10 +5426,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5333,10 +5449,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -5356,10 +5472,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -5379,10 +5495,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -5402,10 +5518,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -5425,10 +5541,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -5448,10 +5564,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -5471,10 +5587,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -5494,10 +5610,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -5517,10 +5633,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -5540,10 +5656,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" t="s">
         <v>136</v>
-      </c>
-      <c r="C29" t="s">
-        <v>137</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -5552,14 +5668,16 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="19"/>
+      <c r="K29" s="19">
+        <v>8.3099999999999997E-3</v>
+      </c>
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -5569,8 +5687,8 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="19">
-        <f>AVERAGE(K18:K28)</f>
-        <v>0.87493727272727273</v>
+        <f>AVERAGE(K18:K29)</f>
+        <v>0.80271833333333331</v>
       </c>
       <c r="L30" s="17"/>
       <c r="M30" s="17">
@@ -5581,7 +5699,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -5610,13 +5728,13 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
         <v>139</v>
-      </c>
-      <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" t="s">
-        <v>140</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -5634,10 +5752,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -5659,10 +5777,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -5680,10 +5798,10 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -5701,10 +5819,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -5722,7 +5840,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -5757,13 +5875,13 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
         <v>145</v>
-      </c>
-      <c r="B40" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" t="s">
-        <v>146</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -5781,10 +5899,10 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -5802,10 +5920,10 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -5823,10 +5941,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -5844,10 +5962,10 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -5865,10 +5983,10 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -5886,7 +6004,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -5915,13 +6033,13 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="s">
         <v>152</v>
-      </c>
-      <c r="B48" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" t="s">
-        <v>153</v>
       </c>
       <c r="D48" s="1">
         <v>6.2500000000000001E-4</v>
@@ -5958,13 +6076,13 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
         <v>154</v>
-      </c>
-      <c r="B50" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" t="s">
-        <v>155</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -5995,13 +6113,13 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>155</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
         <v>156</v>
-      </c>
-      <c r="B52" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" t="s">
-        <v>157</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -6020,10 +6138,10 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -6041,130 +6159,181 @@
       <c r="N53" s="17"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" t="s">
+        <v>177</v>
+      </c>
       <c r="D54" s="1"/>
-      <c r="K54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="38">
+        <v>0.24399999999999999</v>
+      </c>
       <c r="L54" s="17"/>
       <c r="M54" s="17"/>
       <c r="N54" s="17"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>164</v>
-      </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="C55" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
       <c r="K55" s="38">
-        <v>0.44</v>
+        <v>2.835</v>
       </c>
       <c r="L55" s="17"/>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>166</v>
-      </c>
-      <c r="C56" s="37" t="s">
-        <v>170</v>
-      </c>
       <c r="D56" s="1"/>
-      <c r="K56" s="38">
-        <v>15.3</v>
-      </c>
+      <c r="K56" s="1"/>
       <c r="L56" s="17"/>
       <c r="M56" s="17"/>
       <c r="N56" s="17"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>186</v>
+      </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
-      </c>
-      <c r="D57" s="1"/>
-      <c r="K57" s="38">
-        <v>2.14</v>
+        <v>165</v>
+      </c>
+      <c r="K57">
+        <v>4.54</v>
       </c>
       <c r="L57" s="17"/>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" t="s">
+        <v>167</v>
+      </c>
       <c r="D58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
+      <c r="K58" s="38">
+        <v>0.44</v>
+      </c>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>172</v>
-      </c>
-      <c r="C59" t="s">
-        <v>173</v>
+      <c r="B59" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>168</v>
       </c>
       <c r="D59" s="1"/>
-      <c r="K59" s="1">
-        <v>15</v>
-      </c>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
+      <c r="K59" s="38">
+        <v>15.3</v>
+      </c>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
       <c r="C60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" s="10"/>
-      <c r="K60" s="1">
-        <v>15</v>
+        <v>185</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="K60" s="38">
+        <v>2.14</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>175</v>
-      </c>
       <c r="D61" s="1"/>
-      <c r="K61" s="1">
-        <v>15</v>
-      </c>
+      <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D62" s="1"/>
-      <c r="K62" s="1"/>
+      <c r="A62" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" t="s">
+        <v>183</v>
+      </c>
+      <c r="C62" t="s">
+        <v>170</v>
+      </c>
+      <c r="K62" s="38">
+        <v>15</v>
+      </c>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D63" s="2"/>
-      <c r="K63" s="1"/>
+      <c r="B63" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="K63" s="38">
+        <v>15</v>
+      </c>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D64" s="1"/>
-      <c r="K64" s="1"/>
+      <c r="B64" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="10"/>
+      <c r="K64" s="38">
+        <v>15</v>
+      </c>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>164</v>
+      </c>
+      <c r="C65" t="s">
+        <v>188</v>
+      </c>
       <c r="D65" s="1"/>
-      <c r="K65" s="1"/>
+      <c r="K65" s="38">
+        <v>15</v>
+      </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
@@ -6184,30 +6353,30 @@
       <c r="N67" s="1"/>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="12"/>
+      <c r="D68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D69" s="10"/>
+      <c r="D69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D70" s="1"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="12"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D71" s="1"/>
+      <c r="D71" s="10"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -6220,6 +6389,20 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
     </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
LvdB: version 27-6, Update database
</commit_message>
<xml_diff>
--- a/Database_full.xlsx
+++ b/Database_full.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\school\WUR\Master\ACT\Python_week5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Crop parameters" sheetId="3" r:id="rId1"/>
@@ -808,7 +808,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="6" shapeId="0">
+    <comment ref="E9" authorId="6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -826,7 +826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="7" shapeId="0">
+    <comment ref="F9" authorId="7" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -844,7 +844,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="8" shapeId="0">
+    <comment ref="G9" authorId="8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -862,7 +862,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="9" shapeId="0">
+    <comment ref="H9" authorId="9" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -880,7 +880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K13" authorId="10" shapeId="0">
+    <comment ref="K14" authorId="10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -898,7 +898,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K37" authorId="11" shapeId="0">
+    <comment ref="K38" authorId="11" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -916,7 +916,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L37" authorId="12" shapeId="0">
+    <comment ref="L38" authorId="12" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -934,7 +934,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="13" shapeId="0">
+    <comment ref="K40" authorId="13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -952,7 +952,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K41" authorId="14" shapeId="0">
+    <comment ref="K42" authorId="14" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -970,7 +970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K43" authorId="15" shapeId="0">
+    <comment ref="K44" authorId="15" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1134,7 +1134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="6" shapeId="0">
+    <comment ref="D9" authorId="6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1152,7 +1152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="7" shapeId="0">
+    <comment ref="E9" authorId="7" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1170,7 +1170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="8" shapeId="0">
+    <comment ref="F9" authorId="8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1188,7 +1188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="9" shapeId="0">
+    <comment ref="G9" authorId="9" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1206,7 +1206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="10" shapeId="0">
+    <comment ref="H9" authorId="10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1224,7 +1224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K13" authorId="11" shapeId="0">
+    <comment ref="K14" authorId="11" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1242,7 +1242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K15" authorId="12" shapeId="0">
+    <comment ref="K16" authorId="12" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1260,7 +1260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K18" authorId="13" shapeId="0">
+    <comment ref="K19" authorId="13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1280,7 +1280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M18" authorId="14" shapeId="0">
+    <comment ref="M19" authorId="14" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1300,7 +1300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K28" authorId="15" shapeId="0">
+    <comment ref="K29" authorId="15" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1318,7 +1318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M28" authorId="16" shapeId="0">
+    <comment ref="M29" authorId="16" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1336,7 +1336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L34" authorId="17" shapeId="0">
+    <comment ref="L35" authorId="17" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1354,7 +1354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M34" authorId="18" shapeId="0">
+    <comment ref="M35" authorId="18" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1372,7 +1372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K38" authorId="19" shapeId="0">
+    <comment ref="K39" authorId="19" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1390,7 +1390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M38" authorId="20" shapeId="0">
+    <comment ref="M39" authorId="20" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1408,7 +1408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N38" authorId="21" shapeId="0">
+    <comment ref="N39" authorId="21" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1426,7 +1426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K40" authorId="22" shapeId="0">
+    <comment ref="K41" authorId="22" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1444,7 +1444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K42" authorId="23" shapeId="0">
+    <comment ref="K43" authorId="23" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1462,7 +1462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K44" authorId="24" shapeId="0">
+    <comment ref="K45" authorId="24" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1480,7 +1480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D48" authorId="25" shapeId="0">
+    <comment ref="D49" authorId="25" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1498,7 +1498,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K48" authorId="26" shapeId="0">
+    <comment ref="K49" authorId="26" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1516,7 +1516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="27" shapeId="0">
+    <comment ref="B53" authorId="27" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1545,7 +1545,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="196">
   <si>
     <t>Weight (plant/kg)</t>
   </si>
@@ -2112,15 +2112,37 @@
   </si>
   <si>
     <t>BL4</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>Jute fiber</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>Geothermal energy</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>Geothermal engergy</t>
+  </si>
+  <si>
+    <t>C11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -2425,7 +2447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2497,6 +2519,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3171,8 +3197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3533,10 +3559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O69"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="D40" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3600,23 +3626,23 @@
         <v>27</v>
       </c>
       <c r="D2" s="1">
-        <f>(D8*K4+D9*K5+D10*K6+D11*K7)/108.4</f>
+        <f>(D9*K4+D10*K5+D11*K6+D12*K7)/108.4</f>
         <v>0.18592870848708487</v>
       </c>
       <c r="E2" s="1">
-        <f>(E8*K4+E9*K5+E10*K6+E11*K7)/100</f>
+        <f>(E9*K4+E10*K5+E11*K6+E12*K7)/100</f>
         <v>0.257896656</v>
       </c>
       <c r="F2" s="1">
-        <f>(F8*K4+F9*K5+F10*K6+F11*K7)/100</f>
+        <f>(F9*K4+F10*K5+F11*K6+F12*K7)/100</f>
         <v>7.7403239999999998E-2</v>
       </c>
       <c r="G2" s="1">
-        <f>(G8*K4+G9*K5+G10*K6+G11*K7)/100</f>
+        <f>(G9*K4+G10*K5+G11*K6+G12*K7)/100</f>
         <v>0.19653991200000001</v>
       </c>
       <c r="H2" s="1">
-        <f>(K4*H8+K5*H9+H10*K6+H11*K7)/SUM(H8:H11)</f>
+        <f>(K4*H9+K5*H10+H11*K6+H12*K7)/SUM(H9:H12)</f>
         <v>0.45990486486486493</v>
       </c>
       <c r="I2" s="1">
@@ -3756,27 +3782,22 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="1">
-        <v>6.4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>11.7</v>
-      </c>
-      <c r="F8" s="22">
-        <v>0.35</v>
-      </c>
-      <c r="G8" s="1">
-        <v>7.14</v>
-      </c>
-      <c r="H8" s="1">
-        <v>7</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="5">
+        <f>(1/0.277778)*0.226</f>
+        <v>0.81359934912052068</v>
+      </c>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
@@ -3784,23 +3805,23 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="1">
-        <v>16.3</v>
+        <v>6.4</v>
       </c>
       <c r="E9" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="F9" s="1">
-        <v>9.98</v>
+        <v>11.7</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.35</v>
       </c>
       <c r="G9" s="1">
-        <v>21.73</v>
+        <v>7.14</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3812,23 +3833,23 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="1">
-        <v>60.6</v>
+        <v>16.3</v>
       </c>
       <c r="E10" s="1">
-        <v>56.38</v>
+        <v>27.7</v>
       </c>
       <c r="F10" s="1">
-        <v>3.75</v>
+        <v>9.98</v>
       </c>
       <c r="G10" s="1">
-        <v>45.51</v>
+        <v>21.73</v>
       </c>
       <c r="H10" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3840,23 +3861,23 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="1">
-        <v>25.1</v>
+        <v>60.6</v>
       </c>
       <c r="E11" s="1">
-        <v>4.26</v>
+        <v>56.38</v>
       </c>
       <c r="F11" s="1">
-        <v>85.93</v>
+        <v>3.75</v>
       </c>
       <c r="G11" s="1">
-        <v>25.61</v>
+        <v>45.51</v>
       </c>
       <c r="H11" s="1">
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -3867,29 +3888,34 @@
       <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="B12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.26</v>
+      </c>
+      <c r="F12" s="1">
+        <v>85.93</v>
+      </c>
+      <c r="G12" s="1">
+        <v>25.61</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3.5</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
       <c r="O12" s="16"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -3897,20 +3923,21 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="1">
-        <v>82.275999999999996</v>
-      </c>
+      <c r="K13" s="1"/>
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="16"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3920,7 +3947,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1">
-        <v>144.43</v>
+        <v>82.275999999999996</v>
       </c>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
@@ -3929,10 +3956,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -3942,7 +3969,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1">
-        <v>74</v>
+        <v>144.43</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
@@ -3951,10 +3978,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -3964,7 +3991,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1">
-        <v>97.024000000000001</v>
+        <v>74</v>
       </c>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
@@ -3972,6 +3999,12 @@
       <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3979,45 +4012,37 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1">
+        <v>97.024000000000001</v>
+      </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="16"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="20">
-        <v>14.5</v>
-      </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18">
-        <v>14.5</v>
-      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="16"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="1"/>
@@ -4027,21 +4052,21 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="20">
-        <v>11</v>
+        <v>14.5</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="18">
-        <v>11</v>
+        <v>14.5</v>
       </c>
       <c r="N19" s="17"/>
       <c r="O19" s="16"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="1"/>
@@ -4051,21 +4076,21 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="20">
-        <v>15.6</v>
+        <v>11</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18">
-        <v>15.6</v>
+        <v>11</v>
       </c>
       <c r="N20" s="17"/>
       <c r="O20" s="16"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="1"/>
@@ -4075,21 +4100,21 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="20">
-        <v>13.7</v>
+        <v>15.6</v>
       </c>
       <c r="L21" s="18"/>
       <c r="M21" s="18">
-        <v>13.7</v>
+        <v>15.6</v>
       </c>
       <c r="N21" s="17"/>
       <c r="O21" s="16"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="1"/>
@@ -4099,21 +4124,21 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="20">
-        <v>5.54</v>
+        <v>13.7</v>
       </c>
       <c r="L22" s="18"/>
       <c r="M22" s="18">
-        <v>5.54</v>
+        <v>13.7</v>
       </c>
       <c r="N22" s="17"/>
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
@@ -4123,21 +4148,21 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="20">
-        <v>34</v>
+        <v>5.54</v>
       </c>
       <c r="L23" s="18"/>
       <c r="M23" s="18">
-        <v>34</v>
+        <v>5.54</v>
       </c>
       <c r="N23" s="17"/>
       <c r="O23" s="16"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="1"/>
@@ -4147,21 +4172,21 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="20">
-        <v>8.7599999999999997E-2</v>
+        <v>34</v>
       </c>
       <c r="L24" s="18"/>
       <c r="M24" s="18">
-        <v>8.7599999999999997E-2</v>
+        <v>34</v>
       </c>
       <c r="N24" s="17"/>
       <c r="O24" s="16"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="1"/>
@@ -4171,21 +4196,21 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="20">
-        <v>12</v>
+        <v>8.7599999999999997E-2</v>
       </c>
       <c r="L25" s="18"/>
       <c r="M25" s="18">
-        <v>12</v>
+        <v>8.7599999999999997E-2</v>
       </c>
       <c r="N25" s="17"/>
       <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="1"/>
@@ -4195,21 +4220,21 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="20">
-        <v>24.3</v>
+        <v>12</v>
       </c>
       <c r="L26" s="18"/>
       <c r="M26" s="18">
-        <v>24.3</v>
+        <v>12</v>
       </c>
       <c r="N26" s="17"/>
       <c r="O26" s="16"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
@@ -4219,21 +4244,21 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="20">
-        <v>1.6739999999999999</v>
+        <v>24.3</v>
       </c>
       <c r="L27" s="18"/>
       <c r="M27" s="18">
-        <v>1.6739999999999999</v>
+        <v>24.3</v>
       </c>
       <c r="N27" s="17"/>
       <c r="O27" s="16"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="1"/>
@@ -4243,21 +4268,21 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="20">
-        <v>11.9</v>
+        <v>1.6739999999999999</v>
       </c>
       <c r="L28" s="18"/>
       <c r="M28" s="18">
-        <v>11.9</v>
+        <v>1.6739999999999999</v>
       </c>
       <c r="N28" s="17"/>
       <c r="O28" s="16"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="1"/>
@@ -4266,32 +4291,42 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="1">
-        <v>8.7599999999999997E-2</v>
+      <c r="K29" s="20">
+        <v>11.9</v>
       </c>
       <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
+      <c r="M29" s="18">
+        <v>11.9</v>
+      </c>
       <c r="N29" s="17"/>
       <c r="O29" s="16"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="1"/>
+      <c r="B30" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
+      <c r="K30" s="1">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
       <c r="N30" s="17"/>
       <c r="O30" s="16"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -4306,33 +4341,25 @@
       <c r="O31" s="16"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="21">
-        <v>160</v>
-      </c>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
       <c r="O32" s="16"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="1"/>
@@ -4342,7 +4369,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="21">
-        <v>324</v>
+        <v>160</v>
       </c>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
@@ -4350,14 +4377,11 @@
       <c r="O33" s="16"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>76</v>
-      </c>
       <c r="B34" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="1"/>
@@ -4367,7 +4391,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="21">
-        <v>284</v>
+        <v>324</v>
       </c>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
@@ -4375,11 +4399,14 @@
       <c r="O34" s="16"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
       <c r="B35" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="1"/>
@@ -4389,7 +4416,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="21">
-        <v>210</v>
+        <v>284</v>
       </c>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
@@ -4398,10 +4425,10 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="1"/>
@@ -4411,7 +4438,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="21">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
@@ -4419,8 +4446,1440 @@
       <c r="O36" s="16"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="21">
+        <v>156</v>
+      </c>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="16"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1">
+        <v>264.5</v>
+      </c>
+      <c r="L38" s="17">
+        <v>250</v>
+      </c>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="16"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="16"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="21">
+        <v>16.2</v>
+      </c>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="16"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="21">
+        <v>13.4</v>
+      </c>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="16"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="21">
+        <v>6.7</v>
+      </c>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="16"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="21">
+        <v>5</v>
+      </c>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="16"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="21">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="16"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="21">
+        <v>1.849</v>
+      </c>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="16"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1">
+        <v>2.61</v>
+      </c>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="16"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="16"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1.0410000000000001E-2</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17">
+        <f>0.007</f>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="N48" s="17"/>
+      <c r="O48" s="16"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="16"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="19">
+        <v>5.54</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1">
+        <v>5.54</v>
+      </c>
+      <c r="L50" s="17">
+        <v>5.54</v>
+      </c>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="16"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="16"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="40">
+        <f>2.328/1000</f>
+        <v>2.3279999999999998E-3</v>
+      </c>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="16"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="40">
+        <f>28.1/1000</f>
+        <v>2.81E-2</v>
+      </c>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="16"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="39">
+        <f>3.463333/1000</f>
+        <v>3.4633329999999999E-3</v>
+      </c>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="16"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="39">
+        <f>42.15/1000</f>
+        <v>4.215E-2</v>
+      </c>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="16"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D56" s="1"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="16"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>187</v>
+      </c>
+      <c r="B57" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" t="s">
+        <v>166</v>
+      </c>
+      <c r="K57">
+        <v>37.1</v>
+      </c>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="16"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" t="s">
+        <v>173</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="K58" s="38">
+        <v>3.34</v>
+      </c>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="16"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="K59" s="38">
+        <v>147</v>
+      </c>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="16"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="K60" s="38">
+        <v>50.1</v>
+      </c>
+      <c r="L60" s="17"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="16"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="16"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="16"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D63" s="2"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="16"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+    </row>
+    <row r="65" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+    </row>
+    <row r="66" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+    </row>
+    <row r="67" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+    </row>
+    <row r="68" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+    </row>
+    <row r="69" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+    </row>
+    <row r="70" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="1">
+        <f>(D9*K4+D10*K5+D11*K6+D12*K7)/108.4</f>
+        <v>8.6709852398523982E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <f>(E9*K4+E10*K5+E11*K6+E12*K7)/100</f>
+        <v>9.2255004000000002E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>(F9*K4+F10*K5+F11*K6+F12*K7)/100</f>
+        <v>1.3614858000000001E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <f>(G9*K4+G10*K5+G11*K6+G12*K7)/100</f>
+        <v>7.4350278000000006E-2</v>
+      </c>
+      <c r="H2" s="1">
+        <f>(K4*H9+K5*H10+H11*K6+H12*K7)/SUM(H9:H12)</f>
+        <v>8.3014054054054057E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>3.1427999999999998E-2</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1">
+        <f>AVERAGE(D2:I2)</f>
+        <v>6.3562007742096346E-2</v>
+      </c>
+      <c r="L2" s="17">
+        <v>2E-3</v>
+      </c>
+      <c r="M2" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N2" s="17"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.53639999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.61919999999999997</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.1879999999999999</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.47520000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.71640000000000004</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3.1427999999999998E-2</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1">
+        <f>AVERAGE(D3:I3)</f>
+        <v>0.59443800000000002</v>
+      </c>
+      <c r="L3" s="17">
+        <v>0.57150000000000001</v>
+      </c>
+      <c r="M3" s="17">
+        <v>0.58150000000000002</v>
+      </c>
+      <c r="N3" s="17">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1">
+        <v>7.3440000000000005E-2</v>
+      </c>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <f>(0.1332+0.14652)/2</f>
+        <v>0.13986000000000001</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
+        <v>7.5599999999999999E-3</v>
+      </c>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1">
+        <f>(1/0.277778)*0.0213</f>
+        <v>7.6679938656049065E-2</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.35</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7.14</v>
+      </c>
+      <c r="H9" s="1">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>9.98</v>
+      </c>
+      <c r="G10" s="1">
+        <v>21.73</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="1">
+        <v>60.6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>56.38</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="G11" s="1">
+        <v>45.51</v>
+      </c>
+      <c r="H11" s="1">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.26</v>
+      </c>
+      <c r="F12" s="1">
+        <v>85.93</v>
+      </c>
+      <c r="G12" s="1">
+        <v>25.61</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1">
+        <v>3.2530000000000001</v>
+      </c>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1">
+        <v>8.1639999999999997</v>
+      </c>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1">
+        <v>3</v>
+      </c>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1">
+        <v>3.8340000000000001</v>
+      </c>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="19">
+        <v>2.29</v>
+      </c>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17">
+        <v>2.29</v>
+      </c>
+      <c r="N19" s="17"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="19">
+        <v>1.74</v>
+      </c>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17">
+        <v>1.74</v>
+      </c>
+      <c r="N20" s="17"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="19">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="N21" s="17"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="19">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="N22" s="17"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="19">
+        <v>0.223</v>
+      </c>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17">
+        <v>0.223</v>
+      </c>
+      <c r="N23" s="17"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="19">
+        <v>1.75</v>
+      </c>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17">
+        <v>1.75</v>
+      </c>
+      <c r="N24" s="17"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="19">
+        <v>8.3099999999999997E-3</v>
+      </c>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17">
+        <v>8.3099999999999997E-3</v>
+      </c>
+      <c r="N25" s="17"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="19">
+        <v>0.95</v>
+      </c>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="N26" s="17"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="19">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="N27" s="17"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="19">
+        <v>1.9E-2</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17">
+        <v>1.9E-2</v>
+      </c>
+      <c r="N28" s="17"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="19">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="N29" s="17"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="19">
+        <v>8.3099999999999997E-3</v>
+      </c>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="19">
+        <f>AVERAGE(K19:K30)</f>
+        <v>0.80271833333333331</v>
+      </c>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17">
+        <f>AVERAGE(M19:M29)</f>
+        <v>0.87493727272727273</v>
+      </c>
+      <c r="N31" s="17"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1">
+        <v>26.7</v>
+      </c>
+      <c r="L35" s="17">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="M35" s="17">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="N35" s="17"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1">
+        <v>22.6</v>
+      </c>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="C37" t="s">
+        <v>142</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -4430,16 +5889,19 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1">
-        <v>264.5</v>
-      </c>
-      <c r="L37" s="17">
-        <v>250</v>
-      </c>
+        <v>16.7</v>
+      </c>
+      <c r="L37" s="17"/>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
-      <c r="O37" s="16"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" t="s">
+        <v>143</v>
+      </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -4447,150 +5909,141 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+      <c r="K38" s="1">
+        <v>12.7</v>
+      </c>
       <c r="L38" s="17"/>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
-      <c r="O38" s="16"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="5"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="21">
-        <v>16.2</v>
-      </c>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="16"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="5"/>
+      <c r="K39" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17">
+        <v>10.97</v>
+      </c>
+      <c r="N39" s="17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="21">
-        <v>13.4</v>
-      </c>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="16"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K40" s="1"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="5"/>
+        <v>144</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="21">
-        <v>6.7</v>
-      </c>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="16"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D42" s="5"/>
+      <c r="K41" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="21">
-        <v>5</v>
-      </c>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="16"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="5"/>
+      <c r="K42" s="1">
+        <v>1.32</v>
+      </c>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="21">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="16"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="5"/>
+      <c r="K43" s="1">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="21">
-        <v>1.849</v>
-      </c>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="16"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K44" s="1">
+        <v>-0.62</v>
+      </c>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>75</v>
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>149</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -4599,13 +6052,20 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
+      <c r="K45" s="1">
+        <v>2.2700000000000001E-2</v>
+      </c>
       <c r="L45" s="17"/>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
-      <c r="O45" s="16"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" t="s">
+        <v>150</v>
+      </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -4613,25 +6073,21 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
+      <c r="K46" s="1">
+        <v>0.1719</v>
+      </c>
       <c r="L46" s="17"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
-      <c r="O46" s="16"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>100</v>
-      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>101</v>
+        <v>190</v>
       </c>
       <c r="C47" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1.0410000000000001E-2</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -4639,17 +6095,13 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="L47" s="17"/>
-      <c r="M47" s="17">
-        <f>0.007</f>
-        <v>7.0000000000000001E-3</v>
-      </c>
+      <c r="M47" s="17"/>
       <c r="N47" s="17"/>
-      <c r="O47" s="16"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -4661,38 +6113,38 @@
       <c r="L48" s="17"/>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
-      <c r="O48" s="16"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="D49" s="1">
+        <v>6.2500000000000001E-4</v>
+      </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="19">
-        <v>5.54</v>
-      </c>
+      <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="1">
-        <v>5.54</v>
-      </c>
-      <c r="L49" s="17">
-        <v>5.54</v>
-      </c>
-      <c r="M49" s="17"/>
+      <c r="K49" s="19">
+        <f>0.0004</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17">
+        <f>0.0004</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="N49" s="17"/>
-      <c r="O49" s="16"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -4704,17 +6156,16 @@
       <c r="L50" s="17"/>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
-      <c r="O50" s="16"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -4724,21 +6175,13 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1">
-        <f>2.328/1000</f>
-        <v>2.3279999999999998E-3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L51" s="17"/>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
-      <c r="O51" s="16"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" t="s">
-        <v>110</v>
-      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -4746,21 +6189,20 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="1">
-        <f>28.1/1000</f>
-        <v>2.81E-2</v>
-      </c>
+      <c r="K52" s="1"/>
       <c r="L52" s="17"/>
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
-      <c r="O52" s="16"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>155</v>
+      </c>
       <c r="B53" t="s">
-        <v>176</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -4769,20 +6211,20 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="38">
-        <v>3.463333</v>
+      <c r="K53" s="3">
+        <f>0.16386667/1000</f>
+        <v>1.6386666999999999E-4</v>
       </c>
       <c r="L53" s="17"/>
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
-      <c r="O53" s="16"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>178</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -4791,1400 +6233,20 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="38">
-        <v>42.15</v>
+      <c r="K54" s="3">
+        <f>1.89/1000</f>
+        <v>1.89E-3</v>
       </c>
       <c r="L54" s="17"/>
       <c r="M54" s="17"/>
       <c r="N54" s="17"/>
-      <c r="O54" s="16"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D55" s="1"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="16"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>187</v>
-      </c>
-      <c r="B56" t="s">
-        <v>183</v>
-      </c>
-      <c r="C56" t="s">
-        <v>166</v>
-      </c>
-      <c r="K56">
-        <v>37.1</v>
-      </c>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="16"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" t="s">
-        <v>173</v>
-      </c>
-      <c r="D57" s="1"/>
-      <c r="K57" s="38">
-        <v>3.34</v>
-      </c>
-      <c r="L57" s="17"/>
-      <c r="M57" s="17"/>
-      <c r="N57" s="17"/>
-      <c r="O57" s="16"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>163</v>
-      </c>
-      <c r="C58" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="D58" s="1"/>
-      <c r="K58" s="38">
-        <v>147</v>
-      </c>
-      <c r="L58" s="17"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="16"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>164</v>
-      </c>
-      <c r="C59" t="s">
-        <v>184</v>
-      </c>
-      <c r="D59" s="1"/>
-      <c r="K59" s="38">
-        <v>50.1</v>
-      </c>
-      <c r="L59" s="17"/>
-      <c r="M59" s="17"/>
-      <c r="N59" s="17"/>
-      <c r="O59" s="16"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="17"/>
-      <c r="M60" s="17"/>
-      <c r="N60" s="17"/>
-      <c r="O60" s="16"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
-      <c r="O61" s="16"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D62" s="2"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="17"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="16"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-    </row>
-    <row r="66" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N74"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>158</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="1">
-        <f>(D8*K4+D9*K5+D10*K6+D11*K7)/108.4</f>
-        <v>8.6709852398523982E-2</v>
-      </c>
-      <c r="E2" s="1">
-        <f>(E8*K4+E9*K5+E10*K6+E11*K7)/100</f>
-        <v>9.2255004000000002E-2</v>
-      </c>
-      <c r="F2" s="1">
-        <f>(F8*K4+F9*K5+F10*K6+F11*K7)/100</f>
-        <v>1.3614858000000001E-2</v>
-      </c>
-      <c r="G2" s="1">
-        <f>(G8*K4+G9*K5+G10*K6+G11*K7)/100</f>
-        <v>7.4350278000000006E-2</v>
-      </c>
-      <c r="H2" s="1">
-        <f>(K4*H8+K5*H9+H10*K6+H11*K7)/SUM(H8:H11)</f>
-        <v>8.3014054054054057E-2</v>
-      </c>
-      <c r="I2" s="1">
-        <v>3.1427999999999998E-2</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <f>AVERAGE(D2:I2)</f>
-        <v>6.3562007742096346E-2</v>
-      </c>
-      <c r="L2" s="17">
-        <v>2E-3</v>
-      </c>
-      <c r="M2" s="17">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="N2" s="17"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.53639999999999999</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.61919999999999997</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1.1879999999999999</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.47520000000000001</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.71640000000000004</v>
-      </c>
-      <c r="I3" s="1">
-        <v>3.1427999999999998E-2</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1">
-        <f>AVERAGE(D3:I3)</f>
-        <v>0.59443800000000002</v>
-      </c>
-      <c r="L3" s="17">
-        <v>0.57150000000000001</v>
-      </c>
-      <c r="M3" s="17">
-        <v>0.58150000000000002</v>
-      </c>
-      <c r="N3" s="17">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1">
-        <v>7.3440000000000005E-2</v>
-      </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1">
-        <v>1.6199999999999999E-2</v>
-      </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1">
-        <f>(0.1332+0.14652)/2</f>
-        <v>0.13986000000000001</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1">
-        <v>7.5599999999999999E-3</v>
-      </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="1">
-        <v>6.4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>11.7</v>
-      </c>
-      <c r="F8" s="22">
-        <v>0.35</v>
-      </c>
-      <c r="G8" s="1">
-        <v>7.14</v>
-      </c>
-      <c r="H8" s="1">
-        <v>7</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="1">
-        <v>16.3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>27.7</v>
-      </c>
-      <c r="F9" s="1">
-        <v>9.98</v>
-      </c>
-      <c r="G9" s="1">
-        <v>21.73</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="1">
-        <v>60.6</v>
-      </c>
-      <c r="E10" s="1">
-        <v>56.38</v>
-      </c>
-      <c r="F10" s="1">
-        <v>3.75</v>
-      </c>
-      <c r="G10" s="1">
-        <v>45.51</v>
-      </c>
-      <c r="H10" s="1">
-        <v>7</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="1">
-        <v>25.1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>4.26</v>
-      </c>
-      <c r="F11" s="1">
-        <v>85.93</v>
-      </c>
-      <c r="G11" s="1">
-        <v>25.61</v>
-      </c>
-      <c r="H11" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1">
-        <v>3.2530000000000001</v>
-      </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1">
-        <v>8.1639999999999997</v>
-      </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1">
-        <v>3</v>
-      </c>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1">
-        <v>3.8340000000000001</v>
-      </c>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="19">
-        <v>2.29</v>
-      </c>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17">
-        <v>2.29</v>
-      </c>
-      <c r="N18" s="17"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="19">
-        <v>1.74</v>
-      </c>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17">
-        <v>1.74</v>
-      </c>
-      <c r="N19" s="17"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="19">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="N20" s="17"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="19">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="N21" s="17"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="19">
-        <v>0.223</v>
-      </c>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17">
-        <v>0.223</v>
-      </c>
-      <c r="N22" s="17"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" t="s">
-        <v>129</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="19">
-        <v>1.75</v>
-      </c>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17">
-        <v>1.75</v>
-      </c>
-      <c r="N23" s="17"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>130</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="19">
-        <v>8.3099999999999997E-3</v>
-      </c>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17">
-        <v>8.3099999999999997E-3</v>
-      </c>
-      <c r="N24" s="17"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="19">
-        <v>0.95</v>
-      </c>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17">
-        <v>0.95</v>
-      </c>
-      <c r="N25" s="17"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="19">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="N26" s="17"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" t="s">
-        <v>133</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="19">
-        <v>1.9E-2</v>
-      </c>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17">
-        <v>1.9E-2</v>
-      </c>
-      <c r="N27" s="17"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="19">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="N28" s="17"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="19">
-        <v>8.3099999999999997E-3</v>
-      </c>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="19">
-        <f>AVERAGE(K18:K29)</f>
-        <v>0.80271833333333331</v>
-      </c>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17">
-        <f>AVERAGE(M18:M28)</f>
-        <v>0.87493727272727273</v>
-      </c>
-      <c r="N30" s="17"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>137</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>138</v>
-      </c>
-      <c r="B33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1">
-        <v>12.4</v>
-      </c>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1">
-        <v>26.7</v>
-      </c>
-      <c r="L34" s="17">
-        <v>9.2200000000000006</v>
-      </c>
-      <c r="M34" s="17">
-        <v>9.7899999999999991</v>
-      </c>
-      <c r="N34" s="17"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" t="s">
-        <v>141</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1">
-        <v>22.6</v>
-      </c>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" t="s">
-        <v>142</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1">
-        <v>16.7</v>
-      </c>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" t="s">
-        <v>143</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1">
-        <v>12.7</v>
-      </c>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17">
-        <v>10.97</v>
-      </c>
-      <c r="N38" s="17">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" t="s">
-        <v>145</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1">
-        <v>1.08</v>
-      </c>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" t="s">
-        <v>146</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1">
-        <v>1.32</v>
-      </c>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1">
-        <v>0.33400000000000002</v>
-      </c>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" t="s">
-        <v>148</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1">
-        <v>-0.62</v>
-      </c>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" t="s">
-        <v>149</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1">
-        <v>2.2700000000000001E-2</v>
-      </c>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="17"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" t="s">
-        <v>150</v>
-      </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1">
-        <v>0.1719</v>
-      </c>
-      <c r="L45" s="17"/>
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>75</v>
-      </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="17"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="17"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>151</v>
-      </c>
-      <c r="B48" t="s">
-        <v>101</v>
-      </c>
-      <c r="C48" t="s">
-        <v>152</v>
-      </c>
-      <c r="D48" s="1">
-        <v>6.2500000000000001E-4</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="19">
-        <f>0.0004</f>
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="L48" s="17"/>
-      <c r="M48" s="17">
-        <f>0.0004</f>
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="N48" s="17"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="17"/>
-      <c r="M49" s="17"/>
-      <c r="N49" s="17"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" t="s">
-        <v>154</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="L50" s="17"/>
-      <c r="M50" s="17"/>
-      <c r="N50" s="17"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="17"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="17"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>155</v>
-      </c>
-      <c r="B52" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" t="s">
-        <v>156</v>
-      </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1">
-        <f>0.16386667/1000</f>
-        <v>1.6386666999999999E-4</v>
-      </c>
-      <c r="L52" s="17"/>
-      <c r="M52" s="17"/>
-      <c r="N52" s="17"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" t="s">
-        <v>157</v>
-      </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1">
-        <f>1.89/1000</f>
-        <v>1.89E-3</v>
-      </c>
-      <c r="L53" s="17"/>
-      <c r="M53" s="17"/>
-      <c r="N53" s="17"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>176</v>
-      </c>
-      <c r="C54" t="s">
-        <v>177</v>
-      </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="38">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="L54" s="17"/>
-      <c r="M54" s="17"/>
-      <c r="N54" s="17"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C55" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -6193,47 +6255,55 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
-      <c r="K55" s="38">
-        <v>2.835</v>
+      <c r="K55" s="39">
+        <f>0.244/1000</f>
+        <v>2.4399999999999999E-4</v>
       </c>
       <c r="L55" s="17"/>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>178</v>
+      </c>
+      <c r="C56" t="s">
+        <v>179</v>
+      </c>
       <c r="D56" s="1"/>
-      <c r="K56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="39">
+        <f>2.835/1000</f>
+        <v>2.8349999999999998E-3</v>
+      </c>
       <c r="L56" s="17"/>
       <c r="M56" s="17"/>
       <c r="N56" s="17"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>186</v>
-      </c>
-      <c r="B57" t="s">
-        <v>183</v>
-      </c>
-      <c r="C57" t="s">
-        <v>165</v>
-      </c>
-      <c r="K57">
-        <v>4.54</v>
-      </c>
+      <c r="D57" s="1"/>
+      <c r="K57" s="1"/>
       <c r="L57" s="17"/>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>186</v>
+      </c>
       <c r="B58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
-      </c>
-      <c r="D58" s="1"/>
-      <c r="K58" s="38">
-        <v>0.44</v>
+        <v>165</v>
+      </c>
+      <c r="K58">
+        <v>4.54</v>
       </c>
       <c r="L58" s="17"/>
       <c r="M58" s="17"/>
@@ -6241,14 +6311,14 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>163</v>
-      </c>
-      <c r="C59" s="37" t="s">
-        <v>168</v>
+        <v>182</v>
+      </c>
+      <c r="C59" t="s">
+        <v>167</v>
       </c>
       <c r="D59" s="1"/>
       <c r="K59" s="38">
-        <v>15.3</v>
+        <v>0.44</v>
       </c>
       <c r="L59" s="17"/>
       <c r="M59" s="17"/>
@@ -6256,51 +6326,51 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>164</v>
-      </c>
-      <c r="C60" t="s">
-        <v>185</v>
+        <v>163</v>
+      </c>
+      <c r="C60" s="37" t="s">
+        <v>168</v>
       </c>
       <c r="D60" s="1"/>
       <c r="K60" s="38">
+        <v>15.3</v>
+      </c>
+      <c r="L60" s="17"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>164</v>
+      </c>
+      <c r="C61" t="s">
+        <v>185</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="K61" s="38">
         <v>2.14</v>
       </c>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D61" s="1"/>
-      <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>169</v>
-      </c>
-      <c r="B62" t="s">
-        <v>183</v>
-      </c>
-      <c r="C62" t="s">
-        <v>170</v>
-      </c>
-      <c r="K62" s="38">
-        <v>15</v>
-      </c>
+      <c r="D62" s="1"/>
+      <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>169</v>
+      </c>
       <c r="B63" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
-      </c>
-      <c r="D63" s="1"/>
+        <v>170</v>
+      </c>
       <c r="K63" s="38">
         <v>15</v>
       </c>
@@ -6310,12 +6380,12 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>172</v>
-      </c>
-      <c r="D64" s="10"/>
+        <v>171</v>
+      </c>
+      <c r="D64" s="1"/>
       <c r="K64" s="38">
         <v>15</v>
       </c>
@@ -6325,12 +6395,12 @@
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C65" t="s">
-        <v>188</v>
-      </c>
-      <c r="D65" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="D65" s="10"/>
       <c r="K65" s="38">
         <v>15</v>
       </c>
@@ -6339,8 +6409,16 @@
       <c r="N65" s="1"/>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" t="s">
+        <v>188</v>
+      </c>
       <c r="D66" s="1"/>
-      <c r="K66" s="1"/>
+      <c r="K66" s="38">
+        <v>15</v>
+      </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
@@ -6367,23 +6445,23 @@
       <c r="N69" s="1"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="12"/>
+      <c r="D70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="12"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D72" s="1"/>
+      <c r="D72" s="10"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
@@ -6403,6 +6481,13 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
     </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>